<commit_message>
(C)    nutrition and diet updates
</commit_message>
<xml_diff>
--- a/Suppl/nutrition plan.xlsx
+++ b/Suppl/nutrition plan.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="90">
   <si>
     <t>Meal</t>
   </si>
@@ -224,9 +224,6 @@
     <t>http://www.fda.gov/Food/GuidanceRegulation/GuidanceDocumentsRegulatoryInformation/LabelingNutrition/ucm064928.htm</t>
   </si>
   <si>
-    <t>*+25% from Centrum, + 100% from Magnesium</t>
-  </si>
-  <si>
     <t>12 oz</t>
   </si>
   <si>
@@ -257,15 +254,9 @@
     <t>Nature Valle Trail Mix Bar</t>
   </si>
   <si>
-    <t>2(+31%)</t>
-  </si>
-  <si>
     <t>(Multi-Vitamin)</t>
   </si>
   <si>
-    <t>20(+10%)</t>
-  </si>
-  <si>
     <t>GNC Total Lean</t>
   </si>
   <si>
@@ -285,16 +276,28 @@
   </si>
   <si>
     <t>Yogurt</t>
+  </si>
+  <si>
+    <t>Centrum</t>
+  </si>
+  <si>
+    <t>Magnesium</t>
+  </si>
+  <si>
+    <t>Fish Oil</t>
+  </si>
+  <si>
+    <t>Thiamin [%]</t>
+  </si>
+  <si>
+    <t>S</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0"/>
-  </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -306,6 +309,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -373,7 +384,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -827,11 +838,86 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -953,37 +1039,10 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="10" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1007,12 +1066,66 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1037,8 +1150,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1372,7 +1489,7 @@
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="45" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="7" t="s">
@@ -1380,72 +1497,72 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="61" t="s">
+      <c r="C2" s="52" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="72"/>
-      <c r="B3" s="56" t="s">
+      <c r="A3" s="81"/>
+      <c r="B3" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="62" t="s">
+      <c r="C3" s="53" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="82" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="54" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="80"/>
+      <c r="B5" s="50" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="56" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="78" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="52" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="79"/>
+      <c r="B7" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="57" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="80"/>
+      <c r="B8" s="50" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="56" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="73" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="57" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="63" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="71"/>
-      <c r="B5" s="59" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="65" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="69" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="55" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="61" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="70"/>
-      <c r="B7" s="60" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="66" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="71"/>
-      <c r="B8" s="59" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="65" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1453,7 +1570,7 @@
       <c r="A10" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="54" t="s">
+      <c r="B10" s="45" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="7" t="s">
@@ -1461,90 +1578,90 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="69" t="s">
+      <c r="A11" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="55" t="s">
+      <c r="B11" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="61" t="s">
+      <c r="C11" s="52" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="72"/>
-      <c r="B12" s="56" t="s">
+      <c r="A12" s="81"/>
+      <c r="B12" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="62" t="s">
+      <c r="C12" s="53" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="82" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="48" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" s="54" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="83"/>
+      <c r="B14" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="55" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="83"/>
+      <c r="B15" s="49" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="55" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="80"/>
+      <c r="B16" s="50" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" s="56" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="78" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="52" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="79"/>
+      <c r="B18" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="57" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="80"/>
+      <c r="B19" s="50" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="56" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="73" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="57" t="s">
-        <v>81</v>
-      </c>
-      <c r="C13" s="63" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="74"/>
-      <c r="B14" s="58" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="64" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="74"/>
-      <c r="B15" s="58" t="s">
-        <v>75</v>
-      </c>
-      <c r="C15" s="64" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="71"/>
-      <c r="B16" s="59" t="s">
-        <v>83</v>
-      </c>
-      <c r="C16" s="65" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="69" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="55" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="61" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="70"/>
-      <c r="B18" s="60" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="66" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="71"/>
-      <c r="B19" s="59" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="65" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1564,8 +1681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA47"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1590,13 +1707,13 @@
         <v>16</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>75</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>76</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>17</v>
@@ -1611,7 +1728,7 @@
         <v>64</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O1" t="s">
         <v>61</v>
@@ -1627,6 +1744,15 @@
       </c>
       <c r="T1" t="s">
         <v>65</v>
+      </c>
+      <c r="V1" s="59" t="s">
+        <v>85</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
@@ -1649,13 +1775,13 @@
         <f>R2*$R$40</f>
         <v>480</v>
       </c>
-      <c r="F2" s="49">
+      <c r="F2" s="42">
         <v>182</v>
       </c>
-      <c r="G2" s="49">
+      <c r="G2" s="42">
         <v>150</v>
       </c>
-      <c r="H2" s="49">
+      <c r="H2" s="42">
         <v>35</v>
       </c>
       <c r="I2" s="18">
@@ -1681,6 +1807,9 @@
       <c r="R2" s="2">
         <v>240</v>
       </c>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
       <c r="AA2" t="s">
         <v>1</v>
       </c>
@@ -1724,7 +1853,7 @@
         <v>121</v>
       </c>
       <c r="L3" s="39">
-        <f>SUM(B3:K3)</f>
+        <f>SUM(B3:K3)+SUM(V3:W3)</f>
         <v>1666</v>
       </c>
       <c r="M3" s="8">
@@ -1741,6 +1870,11 @@
       </c>
       <c r="R3" s="2">
         <v>30</v>
+      </c>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2">
+        <v>35</v>
       </c>
       <c r="AA3" t="s">
         <v>3</v>
@@ -1785,7 +1919,7 @@
         <v>4</v>
       </c>
       <c r="L4" s="39">
-        <f>SUM(B4:K4)</f>
+        <f>SUM(B4:K4)+SUM(V4:W4)</f>
         <v>437.5</v>
       </c>
       <c r="M4" s="8" t="s">
@@ -1801,6 +1935,11 @@
         <v>43</v>
       </c>
       <c r="R4" s="2">
+        <v>25</v>
+      </c>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2">
         <v>25</v>
       </c>
       <c r="AA4" t="s">
@@ -1846,12 +1985,11 @@
         <v>0</v>
       </c>
       <c r="L5" s="39">
-        <f>SUM(B5:K5)</f>
+        <f t="shared" ref="L5:L10" si="4">SUM(B5:K5)+SUM(V5:W5)</f>
         <v>49.5</v>
       </c>
-      <c r="M5" s="67">
-        <f>65*0.75</f>
-        <v>48.75</v>
+      <c r="M5" s="8">
+        <v>65</v>
       </c>
       <c r="O5" s="2">
         <v>0</v>
@@ -1864,6 +2002,11 @@
       </c>
       <c r="R5" s="2">
         <v>2.5</v>
+      </c>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2">
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
@@ -1905,12 +2048,11 @@
         <v>0</v>
       </c>
       <c r="L6" s="39">
-        <f>SUM(B6:K6)</f>
+        <f t="shared" si="4"/>
         <v>9.5</v>
       </c>
-      <c r="M6" s="67">
-        <f>15*0.75</f>
-        <v>11.25</v>
+      <c r="M6" s="8">
+        <v>20</v>
       </c>
       <c r="O6" s="2">
         <v>0</v>
@@ -1923,6 +2065,11 @@
       </c>
       <c r="R6" s="2">
         <v>0</v>
+      </c>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2">
+        <v>1</v>
       </c>
       <c r="AA6" t="s">
         <v>8</v>
@@ -1967,7 +2114,7 @@
         <v>0</v>
       </c>
       <c r="L7" s="39">
-        <f>SUM(B7:K7)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M7" s="8" t="s">
@@ -1984,6 +2131,11 @@
       </c>
       <c r="R7" s="2">
         <v>0</v>
+      </c>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2">
+        <v>1</v>
       </c>
       <c r="AA7" t="s">
         <v>9</v>
@@ -2027,7 +2179,7 @@
         <v>0</v>
       </c>
       <c r="L8" s="39">
-        <f>SUM(B8:K8)</f>
+        <f t="shared" si="4"/>
         <v>8.5</v>
       </c>
       <c r="M8" s="8" t="s">
@@ -2043,6 +2195,11 @@
         <v>57</v>
       </c>
       <c r="R8" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2">
         <v>0.5</v>
       </c>
     </row>
@@ -2084,7 +2241,7 @@
         <v>0</v>
       </c>
       <c r="L9" s="39">
-        <f>SUM(B9:K9)</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="M9" s="8" t="s">
@@ -2102,6 +2259,9 @@
       <c r="R9" s="2">
         <v>1.5</v>
       </c>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
       <c r="AA9" t="s">
         <v>12</v>
       </c>
@@ -2145,7 +2305,7 @@
         <v>0</v>
       </c>
       <c r="L10" s="39">
-        <f>SUM(B10:K10)</f>
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
       <c r="M10" s="8">
@@ -2162,6 +2322,11 @@
       </c>
       <c r="R10" s="2">
         <v>0</v>
+      </c>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2">
+        <v>25</v>
       </c>
       <c r="AA10" t="s">
         <v>13</v>
@@ -2205,8 +2370,8 @@
       <c r="K11" s="36">
         <v>1</v>
       </c>
-      <c r="L11" s="68">
-        <f>SUM(B11:K11)</f>
+      <c r="L11" s="58">
+        <f>SUM(B11:K11)+SUM(V11:X11)</f>
         <v>1643</v>
       </c>
       <c r="M11" s="8">
@@ -2224,6 +2389,9 @@
       <c r="R11" s="2">
         <v>160</v>
       </c>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2"/>
       <c r="AA11" t="s">
         <v>14</v>
       </c>
@@ -2265,8 +2433,8 @@
       <c r="K12" s="36">
         <v>487</v>
       </c>
-      <c r="L12" s="68">
-        <f>SUM(B12:K12)</f>
+      <c r="L12" s="58">
+        <f>SUM(B12:K12)+SUM(V12:X12)</f>
         <v>1537</v>
       </c>
       <c r="M12" s="8">
@@ -2284,6 +2452,9 @@
       <c r="R12" s="2">
         <v>35</v>
       </c>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2"/>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
@@ -2324,12 +2495,11 @@
         <v>31.1</v>
       </c>
       <c r="L13" s="39">
-        <f>SUM(B13:K13)</f>
+        <f t="shared" ref="L13:L16" si="5">SUM(B13:K13)+SUM(V13:W13)</f>
         <v>235.1</v>
       </c>
       <c r="M13" s="8">
-        <f>300*0.75</f>
-        <v>225</v>
+        <v>300</v>
       </c>
       <c r="O13" s="2">
         <v>27</v>
@@ -2341,6 +2511,11 @@
         <v>12</v>
       </c>
       <c r="R13" s="2">
+        <v>1</v>
+      </c>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2">
         <v>1</v>
       </c>
     </row>
@@ -2383,7 +2558,7 @@
         <v>3.5</v>
       </c>
       <c r="L14" s="39">
-        <f>SUM(B14:K14)</f>
+        <f t="shared" si="5"/>
         <v>37.5</v>
       </c>
       <c r="M14" s="15">
@@ -2400,6 +2575,11 @@
       </c>
       <c r="R14" s="2">
         <v>1</v>
+      </c>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
@@ -2441,7 +2621,7 @@
         <v>16.600000000000001</v>
       </c>
       <c r="L15" s="39">
-        <f>SUM(B15:K15)</f>
+        <f t="shared" si="5"/>
         <v>95.6</v>
       </c>
       <c r="M15" s="8" t="s">
@@ -2459,6 +2639,9 @@
       <c r="R15" s="2">
         <v>0</v>
       </c>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2"/>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
@@ -2499,7 +2682,7 @@
         <v>1.5</v>
       </c>
       <c r="L16" s="39">
-        <f>SUM(B16:K16)</f>
+        <f t="shared" si="5"/>
         <v>91.5</v>
       </c>
       <c r="M16" s="8">
@@ -2517,8 +2700,11 @@
       <c r="R16" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="V16" s="2"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2"/>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
       <c r="B17" s="30"/>
       <c r="C17" s="31"/>
@@ -2535,8 +2721,11 @@
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="V17" s="2"/>
+      <c r="W17" s="2"/>
+      <c r="X17" s="2"/>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>33</v>
       </c>
@@ -2545,11 +2734,11 @@
         <v>20</v>
       </c>
       <c r="C18" s="31">
-        <f t="shared" ref="C18:C30" si="4">Q18*$Q$40</f>
+        <f t="shared" ref="C18:C30" si="6">Q18*$Q$40</f>
         <v>13.5</v>
       </c>
       <c r="D18" s="26">
-        <f t="shared" ref="D18:D36" si="5">P18*$P$40</f>
+        <f t="shared" ref="D18:D36" si="7">P18*$P$40</f>
         <v>180</v>
       </c>
       <c r="E18" s="26">
@@ -2574,9 +2763,9 @@
       <c r="K18" s="36">
         <v>2</v>
       </c>
-      <c r="L18" s="40">
-        <f>SUM(B18:K18)</f>
-        <v>239.5</v>
+      <c r="L18" s="61">
+        <f>SUM(B18:K18)+V18+X18</f>
+        <v>309.5</v>
       </c>
       <c r="M18" s="8">
         <v>100</v>
@@ -2593,8 +2782,15 @@
       <c r="R18" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="V18" s="2">
+        <v>70</v>
+      </c>
+      <c r="W18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X18" s="2"/>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>34</v>
       </c>
@@ -2603,11 +2799,11 @@
         <v>70</v>
       </c>
       <c r="C19" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.5</v>
       </c>
       <c r="D19" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>160</v>
       </c>
       <c r="E19" s="26">
@@ -2633,8 +2829,8 @@
         <v>20</v>
       </c>
       <c r="L19" s="40">
-        <f>SUM(B19:K19)</f>
-        <v>267.5</v>
+        <f>SUM(B19:K19)+V19+X19</f>
+        <v>367.5</v>
       </c>
       <c r="M19" s="8">
         <v>100</v>
@@ -2651,8 +2847,15 @@
       <c r="R19" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="V19" s="2">
+        <v>100</v>
+      </c>
+      <c r="W19" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X19" s="2"/>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>35</v>
       </c>
@@ -2661,11 +2864,11 @@
         <v>0</v>
       </c>
       <c r="C20" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>43.5</v>
       </c>
       <c r="D20" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>40</v>
       </c>
       <c r="E20" s="26">
@@ -2691,8 +2894,8 @@
         <v>1</v>
       </c>
       <c r="L20" s="40">
-        <f>SUM(B20:K20)</f>
-        <v>197.5</v>
+        <f t="shared" ref="L20:L22" si="8">SUM(B20:K20)+V20+X20</f>
+        <v>217.5</v>
       </c>
       <c r="M20" s="8">
         <v>100</v>
@@ -2709,8 +2912,15 @@
       <c r="R20" s="2">
         <v>45</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="V20" s="2">
+        <v>20</v>
+      </c>
+      <c r="W20" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X20" s="2"/>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>36</v>
       </c>
@@ -2719,11 +2929,11 @@
         <v>90</v>
       </c>
       <c r="C21" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D21" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>50</v>
       </c>
       <c r="E21" s="26">
@@ -2749,8 +2959,8 @@
         <v>2</v>
       </c>
       <c r="L21" s="40">
-        <f>SUM(B21:K21)</f>
-        <v>160</v>
+        <f t="shared" si="8"/>
+        <v>260</v>
       </c>
       <c r="M21" s="8">
         <v>100</v>
@@ -2767,8 +2977,15 @@
       <c r="R21" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="V21" s="2">
+        <v>100</v>
+      </c>
+      <c r="W21" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X21" s="2"/>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>37</v>
       </c>
@@ -2777,11 +2994,11 @@
         <v>20</v>
       </c>
       <c r="C22" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>39</v>
       </c>
       <c r="D22" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="E22" s="26">
@@ -2807,8 +3024,8 @@
         <v>0</v>
       </c>
       <c r="L22" s="40">
-        <f>SUM(B22:K22)</f>
-        <v>209</v>
+        <f t="shared" si="8"/>
+        <v>459</v>
       </c>
       <c r="M22" s="8">
         <v>100</v>
@@ -2825,8 +3042,15 @@
       <c r="R22" s="2">
         <v>25</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="V22" s="2">
+        <v>250</v>
+      </c>
+      <c r="W22" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X22" s="2"/>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>38</v>
       </c>
@@ -2834,11 +3058,11 @@
         <v>0</v>
       </c>
       <c r="C23" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D23" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="E23" s="26">
@@ -2863,9 +3087,9 @@
       <c r="K23" s="36">
         <v>1</v>
       </c>
-      <c r="L23" s="40">
-        <f>SUM(B23:K23)</f>
-        <v>141</v>
+      <c r="L23" s="61">
+        <f>SUM(B23:K23)+V23+X23</f>
+        <v>241</v>
       </c>
       <c r="M23" s="8">
         <v>100</v>
@@ -2882,8 +3106,15 @@
       <c r="R23" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="V23" s="2">
+        <v>100</v>
+      </c>
+      <c r="W23" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X23" s="2"/>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>39</v>
       </c>
@@ -2891,11 +3122,11 @@
         <v>0</v>
       </c>
       <c r="C24" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.5</v>
       </c>
       <c r="D24" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>120</v>
       </c>
       <c r="E24" s="26">
@@ -2919,9 +3150,9 @@
       <c r="K24" s="36">
         <v>1</v>
       </c>
-      <c r="L24" s="40">
-        <f>SUM(B24:K24)</f>
-        <v>122.5</v>
+      <c r="L24" s="61">
+        <f>SUM(B24:K24)+V24</f>
+        <v>153.5</v>
       </c>
       <c r="M24" s="8">
         <v>100</v>
@@ -2938,8 +3169,15 @@
       <c r="R24" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="V24" s="2">
+        <v>31</v>
+      </c>
+      <c r="W24" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X24" s="2"/>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>40</v>
       </c>
@@ -2948,11 +3186,11 @@
         <v>70</v>
       </c>
       <c r="C25" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="D25" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>120</v>
       </c>
       <c r="E25" s="26">
@@ -2977,8 +3215,8 @@
         <v>3</v>
       </c>
       <c r="L25" s="40">
-        <f>SUM(B25:K25)</f>
-        <v>202</v>
+        <f t="shared" ref="L25:L28" si="9">SUM(B25:K25)+V25+X25</f>
+        <v>302</v>
       </c>
       <c r="M25" s="8">
         <v>100</v>
@@ -2995,8 +3233,15 @@
       <c r="R25" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="V25" s="2">
+        <v>100</v>
+      </c>
+      <c r="W25" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X25" s="2"/>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>41</v>
       </c>
@@ -3005,11 +3250,11 @@
         <v>70</v>
       </c>
       <c r="C26" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>40.5</v>
       </c>
       <c r="D26" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="E26" s="26">
@@ -3035,8 +3280,8 @@
         <v>6</v>
       </c>
       <c r="L26" s="40">
-        <f>SUM(B26:K26)</f>
-        <v>224.5</v>
+        <f t="shared" si="9"/>
+        <v>324.5</v>
       </c>
       <c r="M26" s="8">
         <v>100</v>
@@ -3053,8 +3298,15 @@
       <c r="R26" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="V26" s="2">
+        <v>100</v>
+      </c>
+      <c r="W26" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X26" s="2"/>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>42</v>
       </c>
@@ -3063,11 +3315,11 @@
         <v>70</v>
       </c>
       <c r="C27" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.5</v>
       </c>
       <c r="D27" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="E27" s="26">
@@ -3092,8 +3344,8 @@
         <v>5</v>
       </c>
       <c r="L27" s="40">
-        <f>SUM(B27:K27)</f>
-        <v>182.5</v>
+        <f t="shared" si="9"/>
+        <v>282.5</v>
       </c>
       <c r="M27" s="8">
         <v>100</v>
@@ -3110,8 +3362,15 @@
       <c r="R27" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="V27" s="2">
+        <v>100</v>
+      </c>
+      <c r="W27" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X27" s="2"/>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>43</v>
       </c>
@@ -3120,11 +3379,11 @@
         <v>70</v>
       </c>
       <c r="C28" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>7.5</v>
       </c>
       <c r="D28" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="E28" s="26">
@@ -3149,8 +3408,8 @@
         <v>25</v>
       </c>
       <c r="L28" s="40">
-        <f>SUM(B28:K28)</f>
-        <v>202.5</v>
+        <f t="shared" si="9"/>
+        <v>302.5</v>
       </c>
       <c r="M28" s="8">
         <v>100</v>
@@ -3167,8 +3426,15 @@
       <c r="R28" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="V28" s="2">
+        <v>100</v>
+      </c>
+      <c r="W28" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X28" s="2"/>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>44</v>
       </c>
@@ -3176,11 +3442,11 @@
         <v>0</v>
       </c>
       <c r="C29" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4.5</v>
       </c>
       <c r="D29" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="E29" s="26">
@@ -3204,9 +3470,8 @@
       <c r="K29" s="36">
         <v>7</v>
       </c>
-      <c r="L29" s="40">
-        <f>SUM(B29:K29)</f>
-        <v>111.5</v>
+      <c r="L29" s="41">
+        <v>5</v>
       </c>
       <c r="M29" s="8">
         <v>100</v>
@@ -3223,8 +3488,15 @@
       <c r="R29" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="V29" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="W29" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X29" s="2"/>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>47</v>
       </c>
@@ -3233,11 +3505,11 @@
         <v>70</v>
       </c>
       <c r="C30" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>28.5</v>
       </c>
       <c r="D30" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>30</v>
       </c>
       <c r="E30" s="26">
@@ -3262,8 +3534,8 @@
         <v>0</v>
       </c>
       <c r="L30" s="40">
-        <f>SUM(B30:K30)</f>
-        <v>128.5</v>
+        <f t="shared" ref="L30" si="10">SUM(B30:K30)+V30+X30</f>
+        <v>228.5</v>
       </c>
       <c r="M30" s="8">
         <v>100</v>
@@ -3280,8 +3552,15 @@
       <c r="R30" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="V30" s="2">
+        <v>100</v>
+      </c>
+      <c r="W30" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X30" s="2"/>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>45</v>
       </c>
@@ -3292,7 +3571,7 @@
         <v>0</v>
       </c>
       <c r="D31" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="E31" s="26">
@@ -3316,9 +3595,9 @@
       <c r="K31" s="36">
         <v>0</v>
       </c>
-      <c r="L31" s="40">
-        <f>SUM(B31:K31)</f>
-        <v>100</v>
+      <c r="L31" s="41">
+        <f>20+V31</f>
+        <v>30</v>
       </c>
       <c r="M31" s="8">
         <v>100</v>
@@ -3335,8 +3614,15 @@
       <c r="R31" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="V31" s="2">
+        <v>10</v>
+      </c>
+      <c r="W31" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X31" s="2"/>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>46</v>
       </c>
@@ -3348,7 +3634,7 @@
         <v>13.5</v>
       </c>
       <c r="D32" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="E32" s="26">
@@ -3372,9 +3658,9 @@
       <c r="K32" s="36">
         <v>5</v>
       </c>
-      <c r="L32" s="40">
-        <f>SUM(B32:K32)</f>
-        <v>118.5</v>
+      <c r="L32" s="61">
+        <f>SUM(B32:K32)+V32</f>
+        <v>218.5</v>
       </c>
       <c r="M32" s="8">
         <v>100</v>
@@ -3391,8 +3677,15 @@
       <c r="R32" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V32" s="2">
+        <v>100</v>
+      </c>
+      <c r="W32" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X32" s="2"/>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>48</v>
       </c>
@@ -3404,7 +3697,7 @@
         <v>34.5</v>
       </c>
       <c r="D33" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>60</v>
       </c>
       <c r="E33" s="26">
@@ -3428,9 +3721,9 @@
       <c r="K33" s="36">
         <v>3</v>
       </c>
-      <c r="L33" s="41">
-        <f>SUM(B33:K33)</f>
-        <v>97.5</v>
+      <c r="L33" s="61">
+        <f>SUM(B33:K33)+V33</f>
+        <v>99.5</v>
       </c>
       <c r="M33" s="8">
         <v>100</v>
@@ -3447,8 +3740,15 @@
       <c r="R33" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V33" s="2">
+        <v>2</v>
+      </c>
+      <c r="W33" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X33" s="2"/>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>49</v>
       </c>
@@ -3459,7 +3759,7 @@
         <v>0</v>
       </c>
       <c r="D34" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
       <c r="E34" s="26">
@@ -3483,9 +3783,9 @@
       <c r="K34" s="36">
         <v>0</v>
       </c>
-      <c r="L34" s="41">
-        <f>SUM(B34:K34)</f>
-        <v>8</v>
+      <c r="L34" s="61">
+        <f>SUM(B34:K34)+V34</f>
+        <v>108</v>
       </c>
       <c r="M34" s="8">
         <v>100</v>
@@ -3502,8 +3802,15 @@
       <c r="R34" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V34" s="2">
+        <v>100</v>
+      </c>
+      <c r="W34" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X34" s="2"/>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>50</v>
       </c>
@@ -3515,7 +3822,7 @@
         <v>10.5</v>
       </c>
       <c r="D35" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>20</v>
       </c>
       <c r="E35" s="26">
@@ -3540,9 +3847,9 @@
       <c r="K35" s="36">
         <v>0</v>
       </c>
-      <c r="L35" s="41">
-        <f>SUM(B35:K35)</f>
-        <v>38.5</v>
+      <c r="L35" s="61">
+        <f>SUM(B35:K35)+V35+W35</f>
+        <v>114</v>
       </c>
       <c r="M35" s="8">
         <v>100</v>
@@ -3559,11 +3866,16 @@
       <c r="R35" s="2">
         <v>4</v>
       </c>
-      <c r="T35" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="36" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V35" s="2">
+        <v>13</v>
+      </c>
+      <c r="W35" s="2">
+        <f>250/400*100</f>
+        <v>62.5</v>
+      </c>
+      <c r="X35" s="2"/>
+    </row>
+    <row r="36" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="14" t="s">
         <v>51</v>
       </c>
@@ -3575,7 +3887,7 @@
         <v>13.5</v>
       </c>
       <c r="D36" s="27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="E36" s="27">
@@ -3599,9 +3911,9 @@
       <c r="K36" s="37">
         <v>2</v>
       </c>
-      <c r="L36" s="42">
-        <f>SUM(B36:K36)</f>
-        <v>19.5</v>
+      <c r="L36" s="60">
+        <f>SUM(B36:K36)+V36</f>
+        <v>98.5</v>
       </c>
       <c r="M36" s="9">
         <v>100</v>
@@ -3618,22 +3930,29 @@
       <c r="R36" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="37" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L37" s="75" t="s">
+      <c r="V36" s="2">
         <v>79</v>
       </c>
-      <c r="M37" s="76"/>
+      <c r="W36" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="X36" s="2"/>
+    </row>
+    <row r="37" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L37" s="84" t="s">
+        <v>77</v>
+      </c>
+      <c r="M37" s="85"/>
       <c r="O37" s="2"/>
       <c r="P37" s="2"/>
       <c r="Q37" s="2"/>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="O38" s="2"/>
       <c r="P38" s="2"/>
       <c r="Q38" s="2"/>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="O39" s="2" t="s">
         <v>55</v>
       </c>
@@ -3647,7 +3966,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="O40" s="2">
         <v>2</v>
       </c>
@@ -3661,7 +3980,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
       <c r="O41" s="2"/>
       <c r="P41" s="2"/>
       <c r="Q41" s="2" t="s">
@@ -3669,13 +3988,13 @@
       </c>
       <c r="R41" s="2"/>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="O42" s="2"/>
       <c r="P42" s="2"/>
       <c r="Q42" s="2"/>
       <c r="R42" s="2"/>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="O43" s="2"/>
       <c r="P43" s="2"/>
       <c r="Q43" s="2" t="s">
@@ -3683,22 +4002,22 @@
       </c>
       <c r="R43" s="2"/>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="O44" s="2"/>
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="O45" s="2"/>
       <c r="P45" s="2"/>
       <c r="Q45" s="2"/>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
       <c r="O46" s="2"/>
       <c r="P46" s="2"/>
       <c r="Q46" s="2"/>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>66</v>
       </c>
@@ -3707,8 +4026,11 @@
   <mergeCells count="1">
     <mergeCell ref="L37:M37"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="V1" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3717,7 +4039,7 @@
   <dimension ref="A1:AB47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+      <selection activeCell="R28" sqref="R28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3725,6 +4047,9 @@
     <col min="1" max="1" width="18" style="1" customWidth="1"/>
     <col min="6" max="8" width="9.140625" style="2"/>
     <col min="12" max="13" width="9.140625" style="2"/>
+    <col min="22" max="22" width="9.140625" style="2"/>
+    <col min="23" max="23" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3736,19 +4061,19 @@
         <v>58</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>16</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>75</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>76</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>17</v>
@@ -3763,13 +4088,13 @@
         <v>64</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O1" t="s">
         <v>61</v>
       </c>
       <c r="P1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q1" t="s">
         <v>56</v>
@@ -3779,47 +4104,56 @@
       </c>
       <c r="T1" t="s">
         <v>65</v>
+      </c>
+      <c r="V1" s="59" t="s">
+        <v>85</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="46">
+      <c r="B2" s="63">
         <f>O2*$O$40</f>
         <v>62</v>
       </c>
-      <c r="C2" s="47">
+      <c r="C2" s="64">
         <f t="shared" ref="C2:C7" si="0">Q2*$Q$40</f>
         <v>366</v>
       </c>
-      <c r="D2" s="48">
+      <c r="D2" s="65">
         <v>30</v>
       </c>
-      <c r="E2" s="48">
+      <c r="E2" s="65">
         <f>R2*$R$40</f>
         <v>480</v>
       </c>
-      <c r="F2" s="49">
+      <c r="F2" s="66">
         <v>182</v>
       </c>
-      <c r="G2" s="49">
+      <c r="G2" s="66">
         <v>150</v>
       </c>
-      <c r="H2" s="49">
+      <c r="H2" s="66">
         <v>35</v>
       </c>
-      <c r="I2" s="50">
+      <c r="I2" s="67">
         <v>88</v>
       </c>
-      <c r="J2" s="50">
+      <c r="J2" s="67">
         <v>28</v>
       </c>
-      <c r="K2" s="51">
+      <c r="K2" s="68">
         <v>136</v>
       </c>
-      <c r="L2" s="52"/>
-      <c r="M2" s="53"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="44"/>
       <c r="O2" s="2">
         <v>31</v>
       </c>
@@ -3840,42 +4174,42 @@
       <c r="A3" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="44">
+      <c r="B3" s="69">
         <f t="shared" ref="B3:B30" si="1">O3*$O$40</f>
         <v>220</v>
       </c>
-      <c r="C3" s="21">
+      <c r="C3" s="70">
         <f t="shared" si="0"/>
         <v>183</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="71">
         <f>P3*$P$40</f>
         <v>180</v>
       </c>
-      <c r="E3" s="16">
+      <c r="E3" s="71">
         <f t="shared" ref="E3:E35" si="2">R3*$R$40</f>
         <v>60</v>
       </c>
-      <c r="F3" s="23">
+      <c r="F3" s="72">
         <v>95</v>
       </c>
-      <c r="G3" s="23">
+      <c r="G3" s="72">
         <v>80</v>
       </c>
-      <c r="H3" s="23">
+      <c r="H3" s="72">
         <v>140</v>
       </c>
-      <c r="I3" s="19">
+      <c r="I3" s="73">
         <v>327</v>
       </c>
-      <c r="J3" s="19">
+      <c r="J3" s="73">
         <v>120</v>
       </c>
-      <c r="K3" s="35">
+      <c r="K3" s="74">
         <v>136</v>
       </c>
       <c r="L3" s="39">
-        <f t="shared" ref="L3:L36" si="3">SUM(B3:K3)</f>
+        <f>SUM(B3:K3)+SUM(V3:W3)</f>
         <v>1541</v>
       </c>
       <c r="M3" s="8">
@@ -3892,6 +4226,9 @@
       </c>
       <c r="R3" s="2">
         <v>30</v>
+      </c>
+      <c r="X3" s="2">
+        <v>35</v>
       </c>
       <c r="AA3" t="s">
         <v>3</v>
@@ -3901,7 +4238,7 @@
       <c r="A4" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="44">
+      <c r="B4" s="58">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3932,11 +4269,11 @@
       <c r="J4" s="19">
         <v>30</v>
       </c>
-      <c r="K4" s="36">
+      <c r="K4" s="75">
         <v>121</v>
       </c>
       <c r="L4" s="39">
-        <f t="shared" si="3"/>
+        <f>SUM(B4:K4)+SUM(V4:W4)</f>
         <v>474.5</v>
       </c>
       <c r="M4" s="8" t="s">
@@ -3952,6 +4289,9 @@
         <v>43</v>
       </c>
       <c r="R4" s="2">
+        <v>25</v>
+      </c>
+      <c r="X4" s="2">
         <v>25</v>
       </c>
       <c r="AA4" t="s">
@@ -3962,7 +4302,7 @@
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="44">
+      <c r="B5" s="58">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3993,11 +4333,11 @@
       <c r="J5" s="19">
         <v>3</v>
       </c>
-      <c r="K5" s="36">
+      <c r="K5" s="75">
         <v>4</v>
       </c>
       <c r="L5" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="L5:L10" si="3">SUM(B5:K5)+SUM(V5:W5)</f>
         <v>43.5</v>
       </c>
       <c r="M5" s="8">
@@ -4014,13 +4354,16 @@
       </c>
       <c r="R5" s="2">
         <v>2.5</v>
+      </c>
+      <c r="X5" s="2">
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="44">
+      <c r="B6" s="58">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4051,7 +4394,7 @@
       <c r="J6" s="19">
         <v>0.5</v>
       </c>
-      <c r="K6" s="36">
+      <c r="K6" s="75">
         <v>0</v>
       </c>
       <c r="L6" s="39">
@@ -4073,6 +4416,9 @@
       <c r="R6" s="2">
         <v>0</v>
       </c>
+      <c r="X6" s="2">
+        <v>1</v>
+      </c>
       <c r="AA6" t="s">
         <v>8</v>
       </c>
@@ -4081,7 +4427,7 @@
       <c r="A7" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="44">
+      <c r="B7" s="58">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4111,7 +4457,7 @@
       <c r="J7" s="19">
         <v>0</v>
       </c>
-      <c r="K7" s="36">
+      <c r="K7" s="75">
         <v>0</v>
       </c>
       <c r="L7" s="39">
@@ -4132,6 +4478,9 @@
       </c>
       <c r="R7" s="2">
         <v>0</v>
+      </c>
+      <c r="X7" s="2">
+        <v>1</v>
       </c>
       <c r="AA7" t="s">
         <v>9</v>
@@ -4141,7 +4490,7 @@
       <c r="A8" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="44">
+      <c r="B8" s="58">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4170,7 +4519,7 @@
       <c r="J8" s="19">
         <v>1.5</v>
       </c>
-      <c r="K8" s="36">
+      <c r="K8" s="75">
         <v>0</v>
       </c>
       <c r="L8" s="39">
@@ -4192,12 +4541,15 @@
       <c r="R8" s="2">
         <v>0.5</v>
       </c>
+      <c r="X8" s="2">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="44">
+      <c r="B9" s="58">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4226,7 +4578,7 @@
       <c r="J9" s="19">
         <v>1</v>
       </c>
-      <c r="K9" s="36">
+      <c r="K9" s="75">
         <v>0</v>
       </c>
       <c r="L9" s="39">
@@ -4256,7 +4608,7 @@
       <c r="A10" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="44">
+      <c r="B10" s="58">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4287,7 +4639,7 @@
       <c r="J10" s="19">
         <v>0</v>
       </c>
-      <c r="K10" s="36">
+      <c r="K10" s="75">
         <v>0</v>
       </c>
       <c r="L10" s="39">
@@ -4309,6 +4661,9 @@
       <c r="R10" s="2">
         <v>0</v>
       </c>
+      <c r="X10" s="2">
+        <v>25</v>
+      </c>
       <c r="AA10" t="s">
         <v>13</v>
       </c>
@@ -4317,7 +4672,7 @@
       <c r="A11" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="44">
+      <c r="B11" s="58">
         <f t="shared" si="1"/>
         <v>380</v>
       </c>
@@ -4348,11 +4703,11 @@
       <c r="J11" s="19">
         <v>190</v>
       </c>
-      <c r="K11" s="36">
-        <v>0</v>
-      </c>
-      <c r="L11" s="68">
-        <f t="shared" si="3"/>
+      <c r="K11" s="75">
+        <v>0</v>
+      </c>
+      <c r="L11" s="58">
+        <f>SUM(B11:K11)+SUM(V11:X11)</f>
         <v>1682</v>
       </c>
       <c r="M11" s="8">
@@ -4378,7 +4733,7 @@
       <c r="A12" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="44">
+      <c r="B12" s="58">
         <f t="shared" si="1"/>
         <v>140</v>
       </c>
@@ -4408,11 +4763,11 @@
       <c r="J12" s="19">
         <v>220</v>
       </c>
-      <c r="K12" s="36">
+      <c r="K12" s="75">
         <v>1</v>
       </c>
-      <c r="L12" s="68">
-        <f t="shared" si="3"/>
+      <c r="L12" s="58">
+        <f>SUM(B12:K12)+SUM(V12:X12)</f>
         <v>741</v>
       </c>
       <c r="M12" s="8">
@@ -4435,7 +4790,7 @@
       <c r="A13" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="44">
+      <c r="B13" s="58">
         <f t="shared" si="1"/>
         <v>54</v>
       </c>
@@ -4466,11 +4821,11 @@
       <c r="J13" s="19">
         <v>22</v>
       </c>
-      <c r="K13" s="36">
+      <c r="K13" s="75">
         <v>487</v>
       </c>
       <c r="L13" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="L13:L16" si="5">SUM(B13:K13)+SUM(V13:W13)</f>
         <v>701</v>
       </c>
       <c r="M13" s="8">
@@ -4486,6 +4841,9 @@
         <v>12</v>
       </c>
       <c r="R13" s="2">
+        <v>1</v>
+      </c>
+      <c r="X13" s="2">
         <v>1</v>
       </c>
     </row>
@@ -4493,7 +4851,7 @@
       <c r="A14" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="44">
+      <c r="B14" s="58">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
@@ -4524,11 +4882,11 @@
       <c r="J14" s="19">
         <v>2</v>
       </c>
-      <c r="K14" s="36">
+      <c r="K14" s="75">
         <v>31.1</v>
       </c>
       <c r="L14" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>61.1</v>
       </c>
       <c r="M14" s="15">
@@ -4545,13 +4903,16 @@
       </c>
       <c r="R14" s="2">
         <v>1</v>
+      </c>
+      <c r="X14" s="2" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="44">
+      <c r="B15" s="58">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
@@ -4582,11 +4943,11 @@
       <c r="J15" s="19">
         <v>3</v>
       </c>
-      <c r="K15" s="36">
+      <c r="K15" s="75">
         <v>3.5</v>
       </c>
       <c r="L15" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>84.5</v>
       </c>
       <c r="M15" s="8" t="s">
@@ -4609,7 +4970,7 @@
       <c r="A16" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="44">
+      <c r="B16" s="58">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
@@ -4640,11 +5001,11 @@
       <c r="J16" s="19">
         <v>2</v>
       </c>
-      <c r="K16" s="36">
+      <c r="K16" s="75">
         <v>16.600000000000001</v>
       </c>
       <c r="L16" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>75.599999999999994</v>
       </c>
       <c r="M16" s="8">
@@ -4663,12 +5024,12 @@
         <v>1</v>
       </c>
       <c r="AA16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
-      <c r="B17" s="44"/>
+      <c r="B17" s="58"/>
       <c r="C17" s="21"/>
       <c r="D17" s="16"/>
       <c r="E17" s="16"/>
@@ -4677,7 +5038,7 @@
       <c r="H17" s="23"/>
       <c r="I17" s="19"/>
       <c r="J17" s="19"/>
-      <c r="K17" s="36">
+      <c r="K17" s="75">
         <v>1.5</v>
       </c>
       <c r="L17" s="39"/>
@@ -4686,7 +5047,7 @@
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
       <c r="AA17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AB17">
         <v>63</v>
@@ -4696,12 +5057,12 @@
       <c r="A18" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="44">
+      <c r="B18" s="58">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="C18" s="21">
-        <f t="shared" ref="C18:C30" si="5">Q18*$Q$40</f>
+        <f t="shared" ref="C18:C30" si="6">Q18*$Q$40</f>
         <v>13.5</v>
       </c>
       <c r="D18" s="16">
@@ -4727,10 +5088,10 @@
       <c r="J18" s="19">
         <v>2</v>
       </c>
-      <c r="K18" s="36"/>
-      <c r="L18" s="41">
-        <f t="shared" si="3"/>
-        <v>72.5</v>
+      <c r="K18" s="75"/>
+      <c r="L18" s="61">
+        <f>SUM(B18:K18)+V18+X18</f>
+        <v>142.5</v>
       </c>
       <c r="M18" s="8">
         <v>100</v>
@@ -4747,20 +5108,26 @@
       <c r="R18" s="2">
         <v>10</v>
       </c>
+      <c r="V18" s="2">
+        <v>70</v>
+      </c>
+      <c r="W18" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="AA18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="44">
+      <c r="B19" s="58">
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
       <c r="C19" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.5</v>
       </c>
       <c r="D19" s="16">
@@ -4786,12 +5153,12 @@
       <c r="J19" s="19">
         <v>2</v>
       </c>
-      <c r="K19" s="36">
+      <c r="K19" s="75">
         <v>2</v>
       </c>
       <c r="L19" s="40">
-        <f t="shared" si="3"/>
-        <v>149.5</v>
+        <f>SUM(B19:K19)+V19+X19</f>
+        <v>249.5</v>
       </c>
       <c r="M19" s="8">
         <v>100</v>
@@ -4807,18 +5174,24 @@
       </c>
       <c r="R19" s="2">
         <v>0</v>
+      </c>
+      <c r="V19" s="2">
+        <v>100</v>
+      </c>
+      <c r="W19" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="44">
+      <c r="B20" s="58">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C20" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>43.5</v>
       </c>
       <c r="D20" s="16">
@@ -4844,12 +5217,12 @@
       <c r="J20" s="19">
         <v>0</v>
       </c>
-      <c r="K20" s="36">
+      <c r="K20" s="75">
         <v>20</v>
       </c>
       <c r="L20" s="40">
-        <f t="shared" si="3"/>
-        <v>226.5</v>
+        <f t="shared" ref="L20:L22" si="7">SUM(B20:K20)+V20+X20</f>
+        <v>246.5</v>
       </c>
       <c r="M20" s="8">
         <v>100</v>
@@ -4865,18 +5238,24 @@
       </c>
       <c r="R20" s="2">
         <v>45</v>
+      </c>
+      <c r="V20" s="2">
+        <v>20</v>
+      </c>
+      <c r="W20" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="44">
+      <c r="B21" s="58">
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
       <c r="C21" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D21" s="16">
@@ -4902,12 +5281,12 @@
       <c r="J21" s="19">
         <v>0</v>
       </c>
-      <c r="K21" s="36">
+      <c r="K21" s="75">
         <v>1</v>
       </c>
       <c r="L21" s="40">
-        <f t="shared" si="3"/>
-        <v>129</v>
+        <f t="shared" si="7"/>
+        <v>229</v>
       </c>
       <c r="M21" s="8">
         <v>100</v>
@@ -4923,18 +5302,24 @@
       </c>
       <c r="R21" s="2">
         <v>2</v>
+      </c>
+      <c r="V21" s="2">
+        <v>100</v>
+      </c>
+      <c r="W21" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="44">
+      <c r="B22" s="58">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="C22" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>39</v>
       </c>
       <c r="D22" s="16">
@@ -4959,12 +5344,12 @@
       <c r="J22" s="19">
         <v>0</v>
       </c>
-      <c r="K22" s="36">
+      <c r="K22" s="75">
         <v>2</v>
       </c>
       <c r="L22" s="40">
-        <f t="shared" si="3"/>
-        <v>111</v>
+        <f t="shared" si="7"/>
+        <v>361</v>
       </c>
       <c r="M22" s="8">
         <v>100</v>
@@ -4980,17 +5365,23 @@
       </c>
       <c r="R22" s="2">
         <v>25</v>
+      </c>
+      <c r="V22" s="2">
+        <v>250</v>
+      </c>
+      <c r="W22" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="44">
+      <c r="B23" s="58">
         <v>0</v>
       </c>
       <c r="C23" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D23" s="16">
@@ -5016,12 +5407,12 @@
       <c r="J23" s="19">
         <v>0</v>
       </c>
-      <c r="K23" s="36">
-        <v>0</v>
-      </c>
-      <c r="L23" s="41">
-        <f t="shared" si="3"/>
-        <v>60</v>
+      <c r="K23" s="75">
+        <v>0</v>
+      </c>
+      <c r="L23" s="61">
+        <f>SUM(B23:K23)+V23+X23</f>
+        <v>160</v>
       </c>
       <c r="M23" s="8">
         <v>100</v>
@@ -5037,17 +5428,23 @@
       </c>
       <c r="R23" s="2">
         <v>20</v>
+      </c>
+      <c r="V23" s="2">
+        <v>100</v>
+      </c>
+      <c r="W23" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="44">
+      <c r="B24" s="58">
         <v>0</v>
       </c>
       <c r="C24" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.5</v>
       </c>
       <c r="D24" s="16">
@@ -5071,11 +5468,12 @@
       <c r="J24" s="19">
         <v>0</v>
       </c>
-      <c r="K24" s="36">
+      <c r="K24" s="75">
         <v>1</v>
       </c>
-      <c r="L24" s="43" t="s">
-        <v>78</v>
+      <c r="L24" s="41">
+        <f>SUM(B24:K24)+V24</f>
+        <v>33.5</v>
       </c>
       <c r="M24" s="8">
         <v>100</v>
@@ -5092,17 +5490,23 @@
       <c r="R24" s="2" t="s">
         <v>57</v>
       </c>
+      <c r="V24" s="2">
+        <v>31</v>
+      </c>
+      <c r="W24" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B25" s="44">
+        <v>88</v>
+      </c>
+      <c r="B25" s="58">
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
       <c r="C25" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="D25" s="16">
@@ -5127,12 +5531,12 @@
       <c r="J25" s="19">
         <v>0</v>
       </c>
-      <c r="K25" s="36">
+      <c r="K25" s="75">
         <v>1</v>
       </c>
       <c r="L25" s="40">
-        <f t="shared" si="3"/>
-        <v>100</v>
+        <f t="shared" ref="L25:L28" si="8">SUM(B25:K25)+V25+X25</f>
+        <v>200</v>
       </c>
       <c r="M25" s="8">
         <v>100</v>
@@ -5147,6 +5551,12 @@
         <v>6</v>
       </c>
       <c r="R25" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="V25" s="2">
+        <v>100</v>
+      </c>
+      <c r="W25" s="2" t="s">
         <v>57</v>
       </c>
     </row>
@@ -5154,12 +5564,12 @@
       <c r="A26" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B26" s="44">
+      <c r="B26" s="58">
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
       <c r="C26" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>40.5</v>
       </c>
       <c r="D26" s="16">
@@ -5185,12 +5595,12 @@
       <c r="J26" s="19">
         <v>0</v>
       </c>
-      <c r="K26" s="36">
+      <c r="K26" s="75">
         <v>3</v>
       </c>
       <c r="L26" s="40">
-        <f t="shared" si="3"/>
-        <v>141.5</v>
+        <f t="shared" si="8"/>
+        <v>241.5</v>
       </c>
       <c r="M26" s="8">
         <v>100</v>
@@ -5206,18 +5616,24 @@
       </c>
       <c r="R26" s="2">
         <v>4</v>
+      </c>
+      <c r="V26" s="2">
+        <v>100</v>
+      </c>
+      <c r="W26" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B27" s="44">
+      <c r="B27" s="58">
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
       <c r="C27" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.5</v>
       </c>
       <c r="D27" s="16">
@@ -5242,12 +5658,12 @@
       <c r="J27" s="19">
         <v>6</v>
       </c>
-      <c r="K27" s="36">
+      <c r="K27" s="75">
         <v>6</v>
       </c>
       <c r="L27" s="40">
-        <f t="shared" si="3"/>
-        <v>103.5</v>
+        <f t="shared" si="8"/>
+        <v>203.5</v>
       </c>
       <c r="M27" s="8">
         <v>100</v>
@@ -5262,6 +5678,12 @@
         <v>1</v>
       </c>
       <c r="R27" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="V27" s="2">
+        <v>100</v>
+      </c>
+      <c r="W27" s="2" t="s">
         <v>57</v>
       </c>
     </row>
@@ -5269,12 +5691,12 @@
       <c r="A28" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B28" s="44">
+      <c r="B28" s="58">
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
       <c r="C28" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7.5</v>
       </c>
       <c r="D28" s="16">
@@ -5299,12 +5721,12 @@
       <c r="J28" s="19">
         <v>0</v>
       </c>
-      <c r="K28" s="36">
+      <c r="K28" s="75">
         <v>5</v>
       </c>
       <c r="L28" s="40">
-        <f t="shared" si="3"/>
-        <v>102.5</v>
+        <f t="shared" si="8"/>
+        <v>202.5</v>
       </c>
       <c r="M28" s="8">
         <v>100</v>
@@ -5319,6 +5741,12 @@
         <v>5</v>
       </c>
       <c r="R28" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="V28" s="2">
+        <v>100</v>
+      </c>
+      <c r="W28" s="2" t="s">
         <v>57</v>
       </c>
     </row>
@@ -5326,11 +5754,11 @@
       <c r="A29" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="44">
+      <c r="B29" s="58">
         <v>0</v>
       </c>
       <c r="C29" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.5</v>
       </c>
       <c r="D29" s="16">
@@ -5354,7 +5782,7 @@
       <c r="J29" s="19">
         <v>0</v>
       </c>
-      <c r="K29" s="36">
+      <c r="K29" s="75">
         <v>25</v>
       </c>
       <c r="L29" s="41">
@@ -5373,6 +5801,12 @@
         <v>3</v>
       </c>
       <c r="R29" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="V29" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="W29" s="2" t="s">
         <v>57</v>
       </c>
     </row>
@@ -5380,16 +5814,16 @@
       <c r="A30" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="B30" s="44">
+      <c r="B30" s="58">
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
       <c r="C30" s="21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>28.5</v>
       </c>
       <c r="D30" s="16">
-        <f t="shared" ref="D30:D36" si="6">P30*$P$40</f>
+        <f t="shared" ref="D30:D36" si="9">P30*$P$40</f>
         <v>20</v>
       </c>
       <c r="E30" s="16">
@@ -5410,12 +5844,12 @@
       <c r="J30" s="19">
         <v>0</v>
       </c>
-      <c r="K30" s="36">
+      <c r="K30" s="75">
         <v>7</v>
       </c>
       <c r="L30" s="40">
-        <f t="shared" si="3"/>
-        <v>125.5</v>
+        <f t="shared" ref="L30" si="10">SUM(B30:K30)+V30+X30</f>
+        <v>225.5</v>
       </c>
       <c r="M30" s="8">
         <v>100</v>
@@ -5430,6 +5864,12 @@
         <v>19</v>
       </c>
       <c r="R30" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="V30" s="2">
+        <v>100</v>
+      </c>
+      <c r="W30" s="2" t="s">
         <v>57</v>
       </c>
     </row>
@@ -5437,14 +5877,14 @@
       <c r="A31" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B31" s="44">
+      <c r="B31" s="58">
         <v>0</v>
       </c>
       <c r="C31" s="21">
         <v>0</v>
       </c>
       <c r="D31" s="16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>20</v>
       </c>
       <c r="E31" s="16">
@@ -5465,11 +5905,12 @@
       <c r="J31" s="19">
         <v>0</v>
       </c>
-      <c r="K31" s="36">
-        <v>0</v>
-      </c>
-      <c r="L31" s="41" t="s">
-        <v>80</v>
+      <c r="K31" s="75">
+        <v>0</v>
+      </c>
+      <c r="L31" s="41">
+        <f>20+V31</f>
+        <v>30</v>
       </c>
       <c r="M31" s="8">
         <v>100</v>
@@ -5484,6 +5925,12 @@
         <v>57</v>
       </c>
       <c r="R31" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="V31" s="2">
+        <v>10</v>
+      </c>
+      <c r="W31" s="2" t="s">
         <v>57</v>
       </c>
     </row>
@@ -5491,7 +5938,7 @@
       <c r="A32" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B32" s="44">
+      <c r="B32" s="58">
         <v>0</v>
       </c>
       <c r="C32" s="21">
@@ -5499,7 +5946,7 @@
         <v>13.5</v>
       </c>
       <c r="D32" s="16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>20</v>
       </c>
       <c r="E32" s="16">
@@ -5520,12 +5967,12 @@
       <c r="J32" s="19">
         <v>0</v>
       </c>
-      <c r="K32" s="36">
-        <v>0</v>
-      </c>
-      <c r="L32" s="41">
-        <f t="shared" si="3"/>
-        <v>33.5</v>
+      <c r="K32" s="75">
+        <v>0</v>
+      </c>
+      <c r="L32" s="61">
+        <f>SUM(B32:K32)+V32</f>
+        <v>133.5</v>
       </c>
       <c r="M32" s="8">
         <v>100</v>
@@ -5542,12 +5989,18 @@
       <c r="R32" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V32" s="2">
+        <v>100</v>
+      </c>
+      <c r="W32" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="B33" s="44">
+      <c r="B33" s="58">
         <v>0</v>
       </c>
       <c r="C33" s="21">
@@ -5555,7 +6008,7 @@
         <v>34.5</v>
       </c>
       <c r="D33" s="16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>20</v>
       </c>
       <c r="E33" s="16">
@@ -5576,12 +6029,12 @@
       <c r="J33" s="19">
         <v>0</v>
       </c>
-      <c r="K33" s="36">
+      <c r="K33" s="75">
         <v>5</v>
       </c>
       <c r="L33" s="41">
-        <f t="shared" si="3"/>
-        <v>59.5</v>
+        <f>SUM(B33:K33)+V33</f>
+        <v>61.5</v>
       </c>
       <c r="M33" s="8">
         <v>100</v>
@@ -5598,19 +6051,25 @@
       <c r="R33" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V33" s="2">
+        <v>2</v>
+      </c>
+      <c r="W33" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="B34" s="44">
+      <c r="B34" s="58">
         <v>0</v>
       </c>
       <c r="C34" s="21">
         <v>0</v>
       </c>
       <c r="D34" s="16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>50</v>
       </c>
       <c r="E34" s="16">
@@ -5631,12 +6090,12 @@
       <c r="J34" s="19">
         <v>0</v>
       </c>
-      <c r="K34" s="36">
+      <c r="K34" s="75">
         <v>3</v>
       </c>
-      <c r="L34" s="41">
-        <f t="shared" si="3"/>
-        <v>53</v>
+      <c r="L34" s="61">
+        <f>SUM(B34:K34)+V34</f>
+        <v>153</v>
       </c>
       <c r="M34" s="8">
         <v>100</v>
@@ -5653,12 +6112,18 @@
       <c r="R34" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V34" s="2">
+        <v>100</v>
+      </c>
+      <c r="W34" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="B35" s="44">
+      <c r="B35" s="58">
         <v>0</v>
       </c>
       <c r="C35" s="21">
@@ -5666,7 +6131,7 @@
         <v>10.5</v>
       </c>
       <c r="D35" s="16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>20</v>
       </c>
       <c r="E35" s="16">
@@ -5688,12 +6153,12 @@
       <c r="J35" s="19">
         <v>0</v>
       </c>
-      <c r="K35" s="36">
-        <v>0</v>
-      </c>
-      <c r="L35" s="41">
-        <f t="shared" si="3"/>
-        <v>38.5</v>
+      <c r="K35" s="75">
+        <v>0</v>
+      </c>
+      <c r="L35" s="61">
+        <f>SUM(B35:K35)+V35+W35</f>
+        <v>114</v>
       </c>
       <c r="M35" s="8">
         <v>100</v>
@@ -5710,15 +6175,19 @@
       <c r="R35" s="2">
         <v>4</v>
       </c>
-      <c r="T35" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="36" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V35" s="2">
+        <v>13</v>
+      </c>
+      <c r="W35" s="2">
+        <f>250/400*100</f>
+        <v>62.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="B36" s="45">
+      <c r="B36" s="76">
         <v>0</v>
       </c>
       <c r="C36" s="22">
@@ -5726,7 +6195,7 @@
         <v>13.5</v>
       </c>
       <c r="D36" s="17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>20</v>
       </c>
       <c r="E36" s="17">
@@ -5747,12 +6216,12 @@
       <c r="J36" s="20">
         <v>0</v>
       </c>
-      <c r="K36" s="36">
-        <v>0</v>
-      </c>
-      <c r="L36" s="42">
-        <f t="shared" si="3"/>
-        <v>33.5</v>
+      <c r="K36" s="77">
+        <v>0</v>
+      </c>
+      <c r="L36" s="60">
+        <f>SUM(B36:K36)+V36</f>
+        <v>112.5</v>
       </c>
       <c r="M36" s="9">
         <v>100</v>
@@ -5769,25 +6238,29 @@
       <c r="R36" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="37" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K37" s="37">
-        <v>2</v>
-      </c>
-      <c r="L37" s="75" t="s">
+      <c r="V36" s="2">
         <v>79</v>
       </c>
-      <c r="M37" s="76"/>
+      <c r="W36" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K37" s="62"/>
+      <c r="L37" s="86" t="s">
+        <v>77</v>
+      </c>
+      <c r="M37" s="85"/>
       <c r="O37" s="2"/>
       <c r="P37" s="2"/>
       <c r="Q37" s="2"/>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="O38" s="2"/>
       <c r="P38" s="2"/>
       <c r="Q38" s="2"/>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="O39" s="2" t="s">
         <v>55</v>
       </c>
@@ -5801,7 +6274,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="O40" s="2">
         <v>2</v>
       </c>
@@ -5815,7 +6288,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="O41" s="2"/>
       <c r="P41" s="2"/>
       <c r="Q41" s="2" t="s">
@@ -5823,13 +6296,13 @@
       </c>
       <c r="R41" s="2"/>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="O42" s="2"/>
       <c r="P42" s="2"/>
       <c r="Q42" s="2"/>
       <c r="R42" s="2"/>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="O43" s="2"/>
       <c r="P43" s="2"/>
       <c r="Q43" s="2" t="s">
@@ -5837,22 +6310,22 @@
       </c>
       <c r="R43" s="2"/>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
       <c r="O44" s="2"/>
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
       <c r="O45" s="2"/>
       <c r="P45" s="2"/>
       <c r="Q45" s="2"/>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
       <c r="O46" s="2"/>
       <c r="P46" s="2"/>
       <c r="Q46" s="2"/>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>66</v>
       </c>
@@ -5861,7 +6334,10 @@
   <mergeCells count="1">
     <mergeCell ref="L37:M37"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="V1" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
(C)    moved to Rob's plan, 3.0! :)
</commit_message>
<xml_diff>
--- a/Suppl/nutrition plan.xlsx
+++ b/Suppl/nutrition plan.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="5" r:id="rId1"/>
-    <sheet name="Nutrition - With Juicer" sheetId="7" r:id="rId2"/>
-    <sheet name="Nutrition - Upcoming" sheetId="6" r:id="rId3"/>
-    <sheet name="Nutrition - Present" sheetId="4" r:id="rId4"/>
-    <sheet name="Nutrition - Prev" sheetId="2" r:id="rId5"/>
-    <sheet name="Nutrition - Alt" sheetId="3" r:id="rId6"/>
-    <sheet name="Items  - Prev" sheetId="1" r:id="rId7"/>
+    <sheet name="Schedule" sheetId="8" r:id="rId2"/>
+    <sheet name="Nutrition - With Juicer" sheetId="7" r:id="rId3"/>
+    <sheet name="Nutrition - Upcoming" sheetId="6" r:id="rId4"/>
+    <sheet name="Nutrition - Present" sheetId="4" r:id="rId5"/>
+    <sheet name="Nutrition - Prev" sheetId="2" r:id="rId6"/>
+    <sheet name="Nutrition - Alt" sheetId="3" r:id="rId7"/>
+    <sheet name="Items  - Prev" sheetId="1" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="147">
   <si>
     <t>Meal</t>
   </si>
@@ -417,9 +418,6 @@
     <t>Juice (36 oz)</t>
   </si>
   <si>
-    <t>Juice</t>
-  </si>
-  <si>
     <t>*I will be drinking 1 Blender Bottle, 20 oz</t>
   </si>
   <si>
@@ -458,11 +456,27 @@
   <si>
     <t>&lt;- Make Shake Before Leave for Work</t>
   </si>
+  <si>
+    <t>Juicer</t>
+  </si>
+  <si>
+    <t>Protein(1Sc)</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Post Workout Meal</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="h\ AM/PM"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -505,7 +519,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -590,8 +604,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="55">
+  <borders count="60">
     <border>
       <left/>
       <right/>
@@ -1291,12 +1317,65 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="194">
+  <cellXfs count="213">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1771,15 +1850,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="11" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="11" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1789,10 +1859,52 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="12" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="15" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1808,6 +1920,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1834,6 +1955,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1844,6 +1980,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFCCFFFF"/>
       <color rgb="FFF3F3DF"/>
       <color rgb="FFEA5C5C"/>
     </mruColors>
@@ -2159,7 +2296,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2201,14 +2338,14 @@
       <c r="C2" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="180" t="s">
+      <c r="E2" s="191" t="s">
         <v>91</v>
       </c>
       <c r="F2" s="79" t="s">
         <v>92</v>
       </c>
       <c r="G2" s="54" t="s">
-        <v>95</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2219,7 +2356,7 @@
       <c r="C3" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="E3" s="181"/>
+      <c r="E3" s="192"/>
       <c r="F3" s="83" t="s">
         <v>93</v>
       </c>
@@ -2235,7 +2372,7 @@
       <c r="C4" s="53" t="s">
         <v>118</v>
       </c>
-      <c r="E4" s="182"/>
+      <c r="E4" s="193"/>
       <c r="F4" s="81" t="s">
         <v>9</v>
       </c>
@@ -2244,7 +2381,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="183" t="s">
+      <c r="A5" s="194" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="48" t="s">
@@ -2253,7 +2390,7 @@
       <c r="C5" s="54" t="s">
         <v>90</v>
       </c>
-      <c r="E5" s="180" t="s">
+      <c r="E5" s="191" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="82" t="s">
@@ -2264,14 +2401,14 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="181"/>
+      <c r="A6" s="192"/>
       <c r="B6" s="78" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="181"/>
+      <c r="E6" s="192"/>
       <c r="F6" s="80" t="s">
         <v>97</v>
       </c>
@@ -2280,14 +2417,14 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="184"/>
+      <c r="A7" s="195"/>
       <c r="B7" s="50" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="56" t="s">
         <v>101</v>
       </c>
-      <c r="E7" s="182"/>
+      <c r="E7" s="193"/>
       <c r="F7" s="81" t="s">
         <v>84</v>
       </c>
@@ -2307,10 +2444,79 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="18.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="208" t="s">
+        <v>145</v>
+      </c>
+      <c r="B1" s="209" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="210">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="211">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="211">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="211">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="212">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD94"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K48" sqref="K44:P48"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P57" sqref="P57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2334,31 +2540,31 @@
       <c r="D1" s="129" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="G1" s="129" t="s">
         <v>103</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="129" t="s">
+      <c r="K1" s="129" t="s">
         <v>107</v>
       </c>
-      <c r="K1" s="129" t="s">
-        <v>130</v>
-      </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="129" t="s">
         <v>108</v>
       </c>
-      <c r="M1" s="34" t="s">
+      <c r="M1" s="5" t="s">
         <v>84</v>
       </c>
       <c r="N1" s="4" t="s">
@@ -2383,7 +2589,7 @@
         <v>62</v>
       </c>
       <c r="V1" t="s">
-        <v>104</v>
+        <v>144</v>
       </c>
       <c r="W1" t="s">
         <v>106</v>
@@ -2402,7 +2608,7 @@
       </c>
     </row>
     <row r="2" spans="1:30" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="176" t="s">
         <v>53</v>
       </c>
       <c r="B2" s="134">
@@ -2410,39 +2616,37 @@
         <v>62</v>
       </c>
       <c r="C2" s="135">
-        <f t="shared" ref="C2:C7" si="0">T2*$T$40</f>
+        <f t="shared" ref="C2" si="0">T2*$T$40</f>
         <v>366</v>
       </c>
-      <c r="D2" s="177">
-        <f t="shared" ref="D2:D16" si="1">S2*$S$40</f>
+      <c r="D2" s="174">
+        <f t="shared" ref="D2" si="1">S2*$S$40</f>
         <v>77.8125</v>
       </c>
-      <c r="E2" s="178">
+      <c r="E2" s="181">
         <f>U2*$U$40</f>
         <v>480</v>
       </c>
-      <c r="F2" s="150">
+      <c r="F2" s="187"/>
+      <c r="G2" s="150">
         <f>V2*V40</f>
-        <v>32</v>
-      </c>
-      <c r="G2" s="151">
+        <v>128</v>
+      </c>
+      <c r="H2" s="151">
         <f>W2</f>
         <v>17.2</v>
       </c>
-      <c r="H2" s="152">
+      <c r="I2" s="152">
         <f>U2*1</f>
         <v>240</v>
       </c>
-      <c r="I2" s="151"/>
-      <c r="J2" s="110">
+      <c r="J2" s="151"/>
+      <c r="K2" s="177">
         <v>127</v>
       </c>
-      <c r="K2" s="172"/>
-      <c r="L2" s="111">
+      <c r="L2" s="178"/>
+      <c r="M2" s="179">
         <v>30</v>
-      </c>
-      <c r="M2" s="112">
-        <v>150</v>
       </c>
       <c r="N2" s="162"/>
       <c r="O2" s="163"/>
@@ -2474,46 +2678,45 @@
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A3" s="130" t="s">
+      <c r="A3" s="180" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="137">
-        <f t="shared" ref="B3:B30" si="2">R3*$R$40</f>
+        <f>$R$40*R3</f>
         <v>220</v>
       </c>
-      <c r="C3" s="176">
-        <f t="shared" si="0"/>
+      <c r="C3" s="173">
+        <f>$S$40*T3</f>
         <v>183</v>
       </c>
       <c r="D3" s="90">
-        <f t="shared" si="1"/>
+        <f>S3*S40</f>
         <v>300</v>
       </c>
-      <c r="E3" s="84">
-        <f t="shared" ref="E3:E35" si="3">U3*$U$40</f>
+      <c r="E3" s="182">
+        <f>$U$40*U3</f>
         <v>60</v>
       </c>
-      <c r="F3" s="153">
-        <f t="shared" ref="F3:F11" si="4">V3*$V$40</f>
-        <v>125</v>
-      </c>
-      <c r="G3" s="154">
+      <c r="F3" s="188">
+        <v>278.33333333333337</v>
+      </c>
+      <c r="G3" s="185">
+        <f>$V$40*V3</f>
+        <v>300</v>
+      </c>
+      <c r="H3" s="154">
         <f>W3</f>
         <v>5</v>
       </c>
-      <c r="H3" s="154">
-        <f>U3*1</f>
-        <v>30</v>
-      </c>
-      <c r="I3" s="155">
+      <c r="I3" s="154">
+        <f t="shared" ref="I3:I23" si="2">$U$40*U3</f>
+        <v>60</v>
+      </c>
+      <c r="J3" s="155">
         <v>105</v>
       </c>
-      <c r="J3" s="147">
+      <c r="K3" s="147">
         <v>270</v>
-      </c>
-      <c r="K3" s="173">
-        <f>501*(20/32)</f>
-        <v>313.125</v>
       </c>
       <c r="L3" s="108">
         <v>130</v>
@@ -2522,18 +2725,18 @@
         <v>80</v>
       </c>
       <c r="N3" s="167">
-        <f t="shared" ref="N3:N12" si="5">SUM(B3:M3)+SUM(Y3:AB3)</f>
-        <v>1856.125</v>
+        <f t="shared" ref="N3:N12" si="3">SUM(B3:M3)+SUM(Y3:AB3)</f>
+        <v>2026.3333333333335</v>
       </c>
       <c r="O3" s="168">
-        <v>1700</v>
+        <v>2000</v>
       </c>
       <c r="P3" s="169">
         <v>2000</v>
       </c>
       <c r="Q3" s="128">
         <f>N3/O3</f>
-        <v>1.0918382352941176</v>
+        <v>1.0131666666666668</v>
       </c>
       <c r="R3" s="2">
         <v>110</v>
@@ -2548,7 +2751,7 @@
         <v>30</v>
       </c>
       <c r="V3" s="62">
-        <v>250</v>
+        <v>150</v>
       </c>
       <c r="W3" s="62">
         <v>5</v>
@@ -2567,40 +2770,40 @@
         <v>52</v>
       </c>
       <c r="B4" s="139">
+        <f>$R$40*R4</f>
+        <v>0</v>
+      </c>
+      <c r="C4" s="88">
+        <f>$T$40*T4</f>
+        <v>64.5</v>
+      </c>
+      <c r="D4" s="92">
+        <f>$S$40*S4</f>
+        <v>45</v>
+      </c>
+      <c r="E4" s="183">
+        <f>U4*$U$40</f>
+        <v>50</v>
+      </c>
+      <c r="F4" s="189" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" s="100">
+        <f>$V$40*V4</f>
+        <v>100</v>
+      </c>
+      <c r="H4" s="149" t="s">
+        <v>57</v>
+      </c>
+      <c r="I4" s="149">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="C4" s="88">
-        <f t="shared" si="0"/>
-        <v>64.5</v>
-      </c>
-      <c r="D4" s="92">
-        <f t="shared" si="1"/>
-        <v>45</v>
-      </c>
-      <c r="E4" s="85">
-        <f t="shared" si="3"/>
         <v>50</v>
       </c>
-      <c r="F4" s="156">
-        <f t="shared" si="4"/>
-        <v>17.5</v>
-      </c>
-      <c r="G4" s="149">
-        <v>0</v>
-      </c>
-      <c r="H4" s="149">
-        <f t="shared" ref="H4:H35" si="6">U4*1</f>
-        <v>25</v>
-      </c>
-      <c r="I4" s="97">
+      <c r="J4" s="97">
         <v>3</v>
       </c>
-      <c r="J4" s="147">
+      <c r="K4" s="147">
         <v>60</v>
-      </c>
-      <c r="K4" s="173">
-        <v>0</v>
       </c>
       <c r="L4" s="108">
         <v>40</v>
@@ -2609,8 +2812,8 @@
         <v>0</v>
       </c>
       <c r="N4" s="40">
-        <f t="shared" si="5"/>
-        <v>330</v>
+        <f t="shared" si="3"/>
+        <v>437.5</v>
       </c>
       <c r="O4" s="164" t="s">
         <v>57</v>
@@ -2632,7 +2835,7 @@
         <v>25</v>
       </c>
       <c r="V4" s="62">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="W4" s="2" t="s">
         <v>57</v>
@@ -2651,41 +2854,40 @@
         <v>21</v>
       </c>
       <c r="B5" s="139">
+        <f t="shared" ref="B5:B30" si="4">$R$40*R5</f>
+        <v>0</v>
+      </c>
+      <c r="C5" s="88">
+        <f t="shared" ref="C5:C35" si="5">$T$40*T5</f>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="D5" s="92">
+        <f t="shared" ref="D5:D36" si="6">$S$40*S5</f>
+        <v>4.5</v>
+      </c>
+      <c r="E5" s="183">
+        <f t="shared" ref="E5:E35" si="7">U5*$U$40</f>
+        <v>5</v>
+      </c>
+      <c r="F5" s="189">
+        <v>1.0944444444444446</v>
+      </c>
+      <c r="G5" s="100">
+        <f>$V$40*V5</f>
+        <v>12</v>
+      </c>
+      <c r="H5" s="149" t="s">
+        <v>57</v>
+      </c>
+      <c r="I5" s="149">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="C5" s="88">
-        <f t="shared" si="0"/>
-        <v>7.5</v>
-      </c>
-      <c r="D5" s="92">
-        <f t="shared" si="1"/>
-        <v>4.5</v>
-      </c>
-      <c r="E5" s="85">
-        <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="F5" s="156">
-        <f t="shared" si="4"/>
-        <v>1.5</v>
-      </c>
-      <c r="G5" s="149">
-        <v>0</v>
-      </c>
-      <c r="H5" s="149">
-        <f t="shared" si="6"/>
-        <v>2.5</v>
-      </c>
-      <c r="I5" s="97">
-        <v>0</v>
-      </c>
-      <c r="J5" s="147">
+      <c r="J5" s="97">
+        <v>0</v>
+      </c>
+      <c r="K5" s="147">
         <v>7</v>
-      </c>
-      <c r="K5" s="173">
-        <f>1.97*(20/32)</f>
-        <v>1.23125</v>
       </c>
       <c r="L5" s="108">
         <v>4.5</v>
@@ -2694,8 +2896,8 @@
         <v>0</v>
       </c>
       <c r="N5" s="122">
-        <f t="shared" si="5"/>
-        <v>36.731250000000003</v>
+        <f t="shared" si="3"/>
+        <v>42.994444444444447</v>
       </c>
       <c r="O5" s="166">
         <f>P5</f>
@@ -2706,7 +2908,7 @@
       </c>
       <c r="Q5" s="128">
         <f>N5/O5</f>
-        <v>0.56509615384615386</v>
+        <v>0.66145299145299152</v>
       </c>
       <c r="R5" s="2">
         <v>0</v>
@@ -2715,13 +2917,13 @@
         <v>3</v>
       </c>
       <c r="T5" s="2">
-        <v>5</v>
+        <v>0.6</v>
       </c>
       <c r="U5" s="2">
         <v>2.5</v>
       </c>
       <c r="V5" s="62">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="W5" s="2" t="s">
         <v>57</v>
@@ -2737,40 +2939,40 @@
         <v>22</v>
       </c>
       <c r="B6" s="139">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="C6" s="88">
+        <f t="shared" si="5"/>
+        <v>4.5</v>
+      </c>
+      <c r="D6" s="92">
+        <f t="shared" si="6"/>
+        <v>1.5</v>
+      </c>
+      <c r="E6" s="183">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="F6" s="189" t="s">
+        <v>57</v>
+      </c>
+      <c r="G6" s="100">
+        <f>$V$40*V6</f>
+        <v>6</v>
+      </c>
+      <c r="H6" s="149" t="s">
+        <v>57</v>
+      </c>
+      <c r="I6" s="149">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="C6" s="88">
-        <f t="shared" si="0"/>
-        <v>4.5</v>
-      </c>
-      <c r="D6" s="92">
-        <f t="shared" si="1"/>
-        <v>1.5</v>
-      </c>
-      <c r="E6" s="85">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F6" s="156">
-        <f t="shared" si="4"/>
-        <v>0.5</v>
-      </c>
-      <c r="G6" s="149">
-        <v>0</v>
-      </c>
-      <c r="H6" s="149">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="I6" s="97">
-        <v>0</v>
-      </c>
-      <c r="J6" s="147">
+      <c r="J6" s="97">
+        <v>0</v>
+      </c>
+      <c r="K6" s="147">
         <v>4</v>
-      </c>
-      <c r="K6" s="173">
-        <v>0</v>
       </c>
       <c r="L6" s="108">
         <v>1</v>
@@ -2779,11 +2981,11 @@
         <v>0</v>
       </c>
       <c r="N6" s="40">
-        <f t="shared" si="5"/>
-        <v>12.5</v>
+        <f t="shared" si="3"/>
+        <v>18</v>
       </c>
       <c r="O6" s="165">
-        <f t="shared" ref="O6:O36" si="7">P6</f>
+        <f t="shared" ref="O6:O36" si="8">P6</f>
         <v>20</v>
       </c>
       <c r="P6" s="8">
@@ -2803,7 +3005,7 @@
         <v>0</v>
       </c>
       <c r="V6" s="62">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="W6" s="2" t="s">
         <v>57</v>
@@ -2825,53 +3027,53 @@
         <v>23</v>
       </c>
       <c r="B7" s="139">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="C7" s="88">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="D7" s="92">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E7" s="183">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="189" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" s="100">
+        <f>$V$40*V7</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="149" t="s">
+        <v>57</v>
+      </c>
+      <c r="I7" s="149">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="C7" s="88">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D7" s="92">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E7" s="85">
+      <c r="J7" s="97">
+        <v>0</v>
+      </c>
+      <c r="K7" s="147">
+        <v>0</v>
+      </c>
+      <c r="L7" s="108">
+        <v>0</v>
+      </c>
+      <c r="M7" s="160">
+        <v>0</v>
+      </c>
+      <c r="N7" s="40">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F7" s="156">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G7" s="149">
-        <v>0</v>
-      </c>
-      <c r="H7" s="149">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="I7" s="97">
-        <v>0</v>
-      </c>
-      <c r="J7" s="147">
-        <v>0</v>
-      </c>
-      <c r="K7" s="173">
-        <v>0</v>
-      </c>
-      <c r="L7" s="108">
-        <v>0</v>
-      </c>
-      <c r="M7" s="160">
-        <v>0</v>
-      </c>
-      <c r="N7" s="40">
-        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="O7" s="165" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-</v>
       </c>
       <c r="P7" s="8" t="s">
@@ -2910,38 +3112,37 @@
         <v>24</v>
       </c>
       <c r="B8" s="139">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="C8" s="88">
+        <v>0</v>
+      </c>
+      <c r="D8" s="92">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E8" s="183">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="F8" s="189" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="100" t="s">
+        <v>57</v>
+      </c>
+      <c r="H8" s="149" t="s">
+        <v>57</v>
+      </c>
+      <c r="I8" s="149">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="C8" s="88">
-        <v>0</v>
-      </c>
-      <c r="D8" s="92">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E8" s="85">
-        <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="F8" s="156">
-        <f t="shared" si="4"/>
-        <v>27.5</v>
-      </c>
-      <c r="G8" s="149">
-        <v>0</v>
-      </c>
-      <c r="H8" s="149">
-        <f t="shared" si="6"/>
-        <v>0.5</v>
-      </c>
-      <c r="I8" s="97">
-        <v>0</v>
-      </c>
-      <c r="J8" s="147">
-        <v>0</v>
-      </c>
-      <c r="K8" s="173">
+      <c r="J8" s="97">
+        <v>0</v>
+      </c>
+      <c r="K8" s="147">
         <v>0</v>
       </c>
       <c r="L8" s="108">
@@ -2951,11 +3152,11 @@
         <v>0</v>
       </c>
       <c r="N8" s="40">
-        <f t="shared" si="5"/>
-        <v>31.5</v>
+        <f t="shared" si="3"/>
+        <v>4.5</v>
       </c>
       <c r="O8" s="165" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-</v>
       </c>
       <c r="P8" s="8" t="s">
@@ -2974,8 +3175,8 @@
       <c r="U8" s="2">
         <v>0.5</v>
       </c>
-      <c r="V8" s="62">
-        <v>55</v>
+      <c r="V8" s="62" t="s">
+        <v>57</v>
       </c>
       <c r="W8" s="2" t="s">
         <v>57</v>
@@ -2991,38 +3192,37 @@
         <v>25</v>
       </c>
       <c r="B9" s="139">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="C9" s="88">
+        <v>0</v>
+      </c>
+      <c r="D9" s="92">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E9" s="183">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="F9" s="189" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" s="100" t="s">
+        <v>57</v>
+      </c>
+      <c r="H9" s="149" t="s">
+        <v>57</v>
+      </c>
+      <c r="I9" s="149">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="C9" s="88">
-        <v>0</v>
-      </c>
-      <c r="D9" s="92">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E9" s="85">
-        <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="F9" s="156">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G9" s="149">
-        <v>0</v>
-      </c>
-      <c r="H9" s="149">
-        <f t="shared" si="6"/>
-        <v>1.5</v>
-      </c>
-      <c r="I9" s="97">
-        <v>0</v>
-      </c>
-      <c r="J9" s="147">
-        <v>0</v>
-      </c>
-      <c r="K9" s="173">
+      <c r="J9" s="97">
+        <v>0</v>
+      </c>
+      <c r="K9" s="147">
         <v>0</v>
       </c>
       <c r="L9" s="108">
@@ -3032,11 +3232,11 @@
         <v>0</v>
       </c>
       <c r="N9" s="40">
-        <f t="shared" si="5"/>
-        <v>5.5</v>
+        <f t="shared" si="3"/>
+        <v>7</v>
       </c>
       <c r="O9" s="165" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-</v>
       </c>
       <c r="P9" s="8" t="s">
@@ -3055,8 +3255,8 @@
       <c r="U9" s="2">
         <v>1.5</v>
       </c>
-      <c r="V9" s="62">
-        <v>0</v>
+      <c r="V9" s="62" t="s">
+        <v>57</v>
       </c>
       <c r="W9" s="2" t="s">
         <v>57</v>
@@ -3073,40 +3273,40 @@
         <v>28</v>
       </c>
       <c r="B10" s="139">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="C10" s="88">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+      <c r="D10" s="92">
+        <f t="shared" si="6"/>
+        <v>90</v>
+      </c>
+      <c r="E10" s="183">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="F10" s="189" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" s="100">
+        <f>$V$40*V10</f>
+        <v>30</v>
+      </c>
+      <c r="H10" s="149" t="s">
+        <v>57</v>
+      </c>
+      <c r="I10" s="149">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="C10" s="88">
-        <f>T10*$T$40</f>
-        <v>30</v>
-      </c>
-      <c r="D10" s="92">
-        <f t="shared" si="1"/>
-        <v>90</v>
-      </c>
-      <c r="E10" s="85">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F10" s="156">
-        <f t="shared" si="4"/>
-        <v>27.5</v>
-      </c>
-      <c r="G10" s="149">
-        <v>0</v>
-      </c>
-      <c r="H10" s="149">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="I10" s="97">
-        <v>0</v>
-      </c>
-      <c r="J10" s="147">
+      <c r="J10" s="97">
+        <v>0</v>
+      </c>
+      <c r="K10" s="147">
         <v>25</v>
-      </c>
-      <c r="K10" s="173">
-        <v>0</v>
       </c>
       <c r="L10" s="108">
         <v>0</v>
@@ -3115,11 +3315,11 @@
         <v>10</v>
       </c>
       <c r="N10" s="40">
-        <f t="shared" si="5"/>
-        <v>207.5</v>
+        <f t="shared" si="3"/>
+        <v>210</v>
       </c>
       <c r="O10" s="165">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>300</v>
       </c>
       <c r="P10" s="8">
@@ -3139,7 +3339,7 @@
         <v>0</v>
       </c>
       <c r="V10" s="62">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="W10" s="2" t="s">
         <v>57</v>
@@ -3158,41 +3358,41 @@
         <v>26</v>
       </c>
       <c r="B11" s="139">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>380</v>
       </c>
       <c r="C11" s="88">
-        <f>T11*$T$40</f>
+        <f t="shared" si="5"/>
         <v>150</v>
       </c>
       <c r="D11" s="92">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>180</v>
       </c>
-      <c r="E11" s="85">
-        <f t="shared" si="3"/>
+      <c r="E11" s="183">
+        <f t="shared" si="7"/>
         <v>320</v>
       </c>
-      <c r="F11" s="156">
-        <f t="shared" si="4"/>
-        <v>85</v>
-      </c>
-      <c r="G11" s="149">
+      <c r="F11" s="189" t="s">
+        <v>57</v>
+      </c>
+      <c r="G11" s="100">
+        <f>$V$40*V11</f>
+        <v>320</v>
+      </c>
+      <c r="H11" s="149">
         <f>W11</f>
         <v>90</v>
       </c>
-      <c r="H11" s="149">
-        <f t="shared" si="6"/>
-        <v>160</v>
-      </c>
-      <c r="I11" s="97">
+      <c r="I11" s="149">
+        <f t="shared" si="2"/>
+        <v>320</v>
+      </c>
+      <c r="J11" s="97">
         <v>1</v>
       </c>
-      <c r="J11" s="147">
+      <c r="K11" s="147">
         <v>480</v>
-      </c>
-      <c r="K11" s="173">
-        <v>0</v>
       </c>
       <c r="L11" s="108">
         <v>250</v>
@@ -3201,11 +3401,11 @@
         <v>55</v>
       </c>
       <c r="N11" s="61">
-        <f t="shared" si="5"/>
-        <v>2151</v>
+        <f t="shared" si="3"/>
+        <v>2546</v>
       </c>
       <c r="O11" s="165">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2400</v>
       </c>
       <c r="P11" s="8">
@@ -3225,7 +3425,7 @@
         <v>160</v>
       </c>
       <c r="V11" s="62">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="W11" s="62">
         <v>90</v>
@@ -3242,37 +3442,37 @@
         <v>27</v>
       </c>
       <c r="B12" s="139">
+        <f t="shared" si="4"/>
+        <v>140</v>
+      </c>
+      <c r="C12" s="88">
+        <v>0</v>
+      </c>
+      <c r="D12" s="92">
+        <f t="shared" si="6"/>
+        <v>375</v>
+      </c>
+      <c r="E12" s="183">
+        <f t="shared" si="7"/>
+        <v>70</v>
+      </c>
+      <c r="F12" s="189" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" s="100">
+        <v>0</v>
+      </c>
+      <c r="H12" s="149" t="s">
+        <v>57</v>
+      </c>
+      <c r="I12" s="149">
         <f t="shared" si="2"/>
-        <v>140</v>
-      </c>
-      <c r="C12" s="88">
-        <v>0</v>
-      </c>
-      <c r="D12" s="92">
-        <f t="shared" si="1"/>
-        <v>375</v>
-      </c>
-      <c r="E12" s="85">
-        <f t="shared" si="3"/>
         <v>70</v>
       </c>
-      <c r="F12" s="156">
-        <v>0</v>
-      </c>
-      <c r="G12" s="149">
-        <v>0</v>
-      </c>
-      <c r="H12" s="149">
-        <f t="shared" si="6"/>
-        <v>35</v>
-      </c>
-      <c r="I12" s="97">
-        <v>0</v>
-      </c>
-      <c r="J12" s="147">
-        <v>0</v>
-      </c>
-      <c r="K12" s="173">
+      <c r="J12" s="97">
+        <v>0</v>
+      </c>
+      <c r="K12" s="147">
         <v>0</v>
       </c>
       <c r="L12" s="108">
@@ -3282,11 +3482,11 @@
         <v>160</v>
       </c>
       <c r="N12" s="121">
-        <f t="shared" si="5"/>
-        <v>887.14285714285711</v>
+        <f t="shared" si="3"/>
+        <v>922.14285714285711</v>
       </c>
       <c r="O12" s="21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3500</v>
       </c>
       <c r="P12" s="94">
@@ -3305,8 +3505,8 @@
       <c r="U12" s="2">
         <v>35</v>
       </c>
-      <c r="V12" s="62" t="s">
-        <v>57</v>
+      <c r="V12" s="62">
+        <v>130</v>
       </c>
       <c r="W12" s="2" t="s">
         <v>57</v>
@@ -3324,42 +3524,41 @@
         <v>29</v>
       </c>
       <c r="B13" s="139">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>54</v>
       </c>
       <c r="C13" s="88">
-        <f>T13*$T$40</f>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
       <c r="D13" s="92">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>25.5</v>
       </c>
-      <c r="E13" s="85">
-        <f t="shared" si="3"/>
+      <c r="E13" s="183">
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
-      <c r="F13" s="156">
-        <f>V13*$V$40</f>
-        <v>17.5</v>
-      </c>
-      <c r="G13" s="149">
+      <c r="F13" s="189">
+        <v>84.422222222222231</v>
+      </c>
+      <c r="G13" s="100">
+        <f t="shared" ref="G13:G21" si="9">$V$40*V13</f>
+        <v>18</v>
+      </c>
+      <c r="H13" s="149">
         <f>W13</f>
         <v>1</v>
       </c>
-      <c r="H13" s="149">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="I13" s="97">
+      <c r="I13" s="149">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="J13" s="97">
         <v>27</v>
       </c>
-      <c r="J13" s="147">
+      <c r="K13" s="147">
         <v>41</v>
-      </c>
-      <c r="K13" s="173">
-        <f>151.96*(20/32)</f>
-        <v>94.975000000000009</v>
       </c>
       <c r="L13" s="108">
         <v>20</v>
@@ -3369,10 +3568,10 @@
       </c>
       <c r="N13" s="122">
         <f>SUM(B13:M13)+SUM(Y13:AA13)</f>
-        <v>310.97500000000002</v>
+        <v>301.92222222222222</v>
       </c>
       <c r="O13" s="166">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>300</v>
       </c>
       <c r="P13" s="124">
@@ -3380,7 +3579,7 @@
       </c>
       <c r="Q13" s="128">
         <f>N13/O13</f>
-        <v>1.0365833333333334</v>
+        <v>1.0064074074074074</v>
       </c>
       <c r="R13" s="2">
         <v>27</v>
@@ -3395,7 +3594,7 @@
         <v>1</v>
       </c>
       <c r="V13" s="62">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="W13" s="62">
         <v>1</v>
@@ -3411,41 +3610,40 @@
         <v>30</v>
       </c>
       <c r="B14" s="139">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="C14" s="88">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="D14" s="92">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+      <c r="E14" s="183">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="F14" s="189">
+        <v>16.444444444444446</v>
+      </c>
+      <c r="G14" s="100">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="H14" s="149" t="s">
+        <v>57</v>
+      </c>
+      <c r="I14" s="149">
         <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="C14" s="88">
-        <f>T14*$T$40</f>
-        <v>0</v>
-      </c>
-      <c r="D14" s="92">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="E14" s="85">
-        <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="F14" s="156">
-        <f>V14*$V$40</f>
+      <c r="J14" s="97">
+        <v>3</v>
+      </c>
+      <c r="K14" s="147">
         <v>1</v>
-      </c>
-      <c r="G14" s="149">
-        <v>0</v>
-      </c>
-      <c r="H14" s="149">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="I14" s="97">
-        <v>3</v>
-      </c>
-      <c r="J14" s="147">
-        <v>1</v>
-      </c>
-      <c r="K14" s="173">
-        <f>29.6*(20/32)</f>
-        <v>18.5</v>
       </c>
       <c r="L14" s="108">
         <v>1</v>
@@ -3455,10 +3653,10 @@
       </c>
       <c r="N14" s="61">
         <f>SUM(B14:M14)+SUM(Y14:Z14)</f>
-        <v>45.5</v>
+        <v>47.444444444444443</v>
       </c>
       <c r="O14" s="165">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>25</v>
       </c>
       <c r="P14" s="15">
@@ -3494,41 +3692,40 @@
         <v>31</v>
       </c>
       <c r="B15" s="139">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="C15" s="88">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="D15" s="92">
+        <f t="shared" si="6"/>
+        <v>4.5</v>
+      </c>
+      <c r="E15" s="183">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="189">
+        <v>49.116666666666667</v>
+      </c>
+      <c r="G15" s="100">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="H15" s="149" t="s">
+        <v>57</v>
+      </c>
+      <c r="I15" s="149">
         <f t="shared" si="2"/>
-        <v>18</v>
-      </c>
-      <c r="C15" s="88">
-        <f>T15*$T$40</f>
-        <v>18</v>
-      </c>
-      <c r="D15" s="92">
-        <f t="shared" si="1"/>
-        <v>4.5</v>
-      </c>
-      <c r="E15" s="85">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F15" s="156">
-        <f>V15*$V$40</f>
-        <v>1.5</v>
-      </c>
-      <c r="G15" s="149">
-        <v>0</v>
-      </c>
-      <c r="H15" s="149">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="I15" s="97">
+        <v>0</v>
+      </c>
+      <c r="J15" s="97">
         <v>14</v>
       </c>
-      <c r="J15" s="147">
+      <c r="K15" s="147">
         <v>5</v>
-      </c>
-      <c r="K15" s="173">
-        <f>88.41*(20/32)</f>
-        <v>55.256249999999994</v>
       </c>
       <c r="L15" s="108">
         <v>0</v>
@@ -3538,10 +3735,10 @@
       </c>
       <c r="N15" s="125">
         <f>SUM(B15:M15)+SUM(Y15:Z15)</f>
-        <v>122.25624999999999</v>
+        <v>118.61666666666667</v>
       </c>
       <c r="O15" s="165" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-</v>
       </c>
       <c r="P15" s="126" t="s">
@@ -3561,7 +3758,7 @@
         <v>0</v>
       </c>
       <c r="V15" s="62">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W15" s="62" t="s">
         <v>57</v>
@@ -3575,41 +3772,40 @@
         <v>32</v>
       </c>
       <c r="B16" s="139">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="C16" s="88">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="D16" s="92">
+        <f t="shared" si="6"/>
+        <v>37.5</v>
+      </c>
+      <c r="E16" s="183">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="F16" s="189">
+        <v>3.9944444444444449</v>
+      </c>
+      <c r="G16" s="100">
+        <f t="shared" si="9"/>
+        <v>32</v>
+      </c>
+      <c r="H16" s="149" t="s">
+        <v>57</v>
+      </c>
+      <c r="I16" s="149">
         <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="C16" s="88">
-        <f>T16*$T$40</f>
+        <v>2</v>
+      </c>
+      <c r="J16" s="97">
+        <v>1</v>
+      </c>
+      <c r="K16" s="147">
         <v>12</v>
-      </c>
-      <c r="D16" s="92">
-        <f t="shared" si="1"/>
-        <v>37.5</v>
-      </c>
-      <c r="E16" s="85">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="F16" s="156">
-        <f>V16*$V$40</f>
-        <v>10</v>
-      </c>
-      <c r="G16" s="149">
-        <v>0</v>
-      </c>
-      <c r="H16" s="149">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="I16" s="97">
-        <v>1</v>
-      </c>
-      <c r="J16" s="147">
-        <v>12</v>
-      </c>
-      <c r="K16" s="173">
-        <f>7.19*(20/32)</f>
-        <v>4.4937500000000004</v>
       </c>
       <c r="L16" s="108">
         <v>4</v>
@@ -3619,18 +3815,17 @@
       </c>
       <c r="N16" s="122">
         <f>SUM(B16:M16)+SUM(Y16:Z16)</f>
-        <v>99.993750000000006</v>
+        <v>122.49444444444444</v>
       </c>
       <c r="O16" s="166">
-        <f t="shared" si="7"/>
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="P16" s="124">
         <v>50</v>
       </c>
       <c r="Q16" s="128">
         <f>N16/O16</f>
-        <v>1.9998750000000001</v>
+        <v>0.81662962962962959</v>
       </c>
       <c r="R16" s="2">
         <v>2</v>
@@ -3645,7 +3840,7 @@
         <v>1</v>
       </c>
       <c r="V16" s="62">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="W16" s="2" t="s">
         <v>57</v>
@@ -3656,21 +3851,43 @@
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" s="130"/>
-      <c r="B17" s="139"/>
-      <c r="C17" s="88"/>
-      <c r="D17" s="92"/>
-      <c r="E17" s="85"/>
-      <c r="F17" s="156"/>
-      <c r="G17" s="149"/>
-      <c r="H17" s="149"/>
-      <c r="I17" s="97"/>
-      <c r="J17" s="147"/>
-      <c r="K17" s="173"/>
+      <c r="B17" s="139">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="C17" s="88">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="D17" s="92">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="E17" s="183">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="F17" s="189">
+        <v>0</v>
+      </c>
+      <c r="G17" s="100">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="H17" s="149" t="s">
+        <v>57</v>
+      </c>
+      <c r="I17" s="149">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="97"/>
+      <c r="K17" s="147"/>
       <c r="L17" s="108"/>
       <c r="M17" s="160"/>
       <c r="N17" s="95"/>
       <c r="O17" s="165">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="P17" s="8"/>
@@ -3688,40 +3905,40 @@
         <v>33</v>
       </c>
       <c r="B18" s="139">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="C18" s="88">
+        <f t="shared" si="5"/>
+        <v>13.5</v>
+      </c>
+      <c r="D18" s="92">
+        <f t="shared" si="6"/>
+        <v>30</v>
+      </c>
+      <c r="E18" s="183">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="F18" s="189">
+        <v>55.555555555555557</v>
+      </c>
+      <c r="G18" s="100">
+        <f t="shared" si="9"/>
+        <v>30</v>
+      </c>
+      <c r="H18" s="149" t="s">
+        <v>57</v>
+      </c>
+      <c r="I18" s="149">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="C18" s="88">
-        <f t="shared" ref="C18:C30" si="8">T18*$T$40</f>
-        <v>13.5</v>
-      </c>
-      <c r="D18" s="92">
-        <f t="shared" ref="D18:D36" si="9">S18*$S$40</f>
-        <v>30</v>
-      </c>
-      <c r="E18" s="85">
-        <f t="shared" si="3"/>
-        <v>20</v>
-      </c>
-      <c r="F18" s="156">
-        <f>V18*$V$40</f>
-        <v>0</v>
-      </c>
-      <c r="G18" s="149">
-        <v>0</v>
-      </c>
-      <c r="H18" s="149">
-        <f t="shared" si="6"/>
-        <v>10</v>
-      </c>
-      <c r="I18" s="97">
+      <c r="J18" s="97">
         <v>2</v>
       </c>
-      <c r="J18" s="147">
+      <c r="K18" s="147">
         <v>4</v>
-      </c>
-      <c r="K18" s="173">
-        <v>100</v>
       </c>
       <c r="L18" s="108">
         <v>2</v>
@@ -3731,10 +3948,10 @@
       </c>
       <c r="N18" s="61">
         <f t="shared" ref="N18:N28" si="10">SUM(B18:M18)+Y18+AA18</f>
-        <v>271.5</v>
+        <v>267.05555555555554</v>
       </c>
       <c r="O18" s="165">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
       <c r="P18" s="8">
@@ -3754,7 +3971,7 @@
         <v>10</v>
       </c>
       <c r="V18" s="62">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="W18" s="2" t="s">
         <v>57</v>
@@ -3772,41 +3989,40 @@
         <v>34</v>
       </c>
       <c r="B19" s="139">
+        <f t="shared" si="4"/>
+        <v>70</v>
+      </c>
+      <c r="C19" s="88">
+        <f t="shared" si="5"/>
+        <v>1.5</v>
+      </c>
+      <c r="D19" s="92">
+        <f t="shared" si="6"/>
+        <v>90</v>
+      </c>
+      <c r="E19" s="183">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="F19" s="189">
+        <v>38.888888888888893</v>
+      </c>
+      <c r="G19" s="100">
+        <f t="shared" si="9"/>
+        <v>30</v>
+      </c>
+      <c r="H19" s="149" t="s">
+        <v>57</v>
+      </c>
+      <c r="I19" s="149">
         <f t="shared" si="2"/>
-        <v>70</v>
-      </c>
-      <c r="C19" s="88">
-        <f t="shared" si="8"/>
-        <v>1.5</v>
-      </c>
-      <c r="D19" s="92">
-        <f t="shared" si="9"/>
-        <v>90</v>
-      </c>
-      <c r="E19" s="85">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F19" s="156">
-        <f>V19*$V$40</f>
-        <v>0</v>
-      </c>
-      <c r="G19" s="149">
-        <v>0</v>
-      </c>
-      <c r="H19" s="149">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="I19" s="97">
+        <v>0</v>
+      </c>
+      <c r="J19" s="97">
         <v>17</v>
       </c>
-      <c r="J19" s="147">
+      <c r="K19" s="147">
         <v>2</v>
-      </c>
-      <c r="K19" s="173">
-        <f>70*(20/32)</f>
-        <v>43.75</v>
       </c>
       <c r="L19" s="108">
         <v>0</v>
@@ -3816,10 +4032,10 @@
       </c>
       <c r="N19" s="61">
         <f t="shared" si="10"/>
-        <v>324.25</v>
+        <v>349.38888888888891</v>
       </c>
       <c r="O19" s="165">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
       <c r="P19" s="8">
@@ -3838,7 +4054,7 @@
         <v>0</v>
       </c>
       <c r="V19" s="62">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="W19" s="62" t="s">
         <v>57</v>
@@ -3856,41 +4072,40 @@
         <v>35</v>
       </c>
       <c r="B20" s="139">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="C20" s="88">
+        <f t="shared" si="5"/>
+        <v>43.5</v>
+      </c>
+      <c r="D20" s="92">
+        <f t="shared" si="6"/>
+        <v>75</v>
+      </c>
+      <c r="E20" s="183">
+        <f t="shared" si="7"/>
+        <v>90</v>
+      </c>
+      <c r="F20" s="189">
+        <v>9.4444444444444446</v>
+      </c>
+      <c r="G20" s="100">
+        <f t="shared" si="9"/>
+        <v>50</v>
+      </c>
+      <c r="H20" s="149" t="s">
+        <v>57</v>
+      </c>
+      <c r="I20" s="149">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="C20" s="88">
-        <f t="shared" si="8"/>
-        <v>43.5</v>
-      </c>
-      <c r="D20" s="92">
-        <f t="shared" si="9"/>
-        <v>75</v>
-      </c>
-      <c r="E20" s="85">
-        <f t="shared" si="3"/>
         <v>90</v>
       </c>
-      <c r="F20" s="156">
-        <f>V20*$V$40</f>
-        <v>7.5</v>
-      </c>
-      <c r="G20" s="149">
-        <v>0</v>
-      </c>
-      <c r="H20" s="149">
-        <f t="shared" si="6"/>
-        <v>45</v>
-      </c>
-      <c r="I20" s="97">
+      <c r="J20" s="97">
         <v>1</v>
       </c>
-      <c r="J20" s="147">
+      <c r="K20" s="147">
         <v>20</v>
-      </c>
-      <c r="K20" s="173">
-        <f>17*(20/32)</f>
-        <v>10.625</v>
       </c>
       <c r="L20" s="108">
         <v>4</v>
@@ -3900,10 +4115,10 @@
       </c>
       <c r="N20" s="61">
         <f t="shared" si="10"/>
-        <v>331.625</v>
+        <v>417.94444444444446</v>
       </c>
       <c r="O20" s="165">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
       <c r="P20" s="8">
@@ -3922,7 +4137,7 @@
         <v>45</v>
       </c>
       <c r="V20" s="62">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="W20" s="107" t="s">
         <v>57</v>
@@ -3940,41 +4155,40 @@
         <v>36</v>
       </c>
       <c r="B21" s="139">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>90</v>
       </c>
       <c r="C21" s="88">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D21" s="92">
+        <f t="shared" si="6"/>
+        <v>30</v>
+      </c>
+      <c r="E21" s="183">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="F21" s="189">
+        <v>7.7777777777777786</v>
+      </c>
+      <c r="G21" s="100">
         <f t="shared" si="9"/>
         <v>30</v>
       </c>
-      <c r="E21" s="85">
-        <f t="shared" si="3"/>
+      <c r="H21" s="149" t="s">
+        <v>57</v>
+      </c>
+      <c r="I21" s="149">
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="F21" s="156">
-        <f>V21*$V$40</f>
-        <v>5</v>
-      </c>
-      <c r="G21" s="149">
-        <v>0</v>
-      </c>
-      <c r="H21" s="149">
-        <f t="shared" si="6"/>
+      <c r="J21" s="97">
         <v>2</v>
       </c>
-      <c r="I21" s="97">
-        <v>2</v>
-      </c>
-      <c r="J21" s="147">
+      <c r="K21" s="147">
         <v>10</v>
-      </c>
-      <c r="K21" s="173">
-        <f>14*(20/32)</f>
-        <v>8.75</v>
       </c>
       <c r="L21" s="108">
         <v>6</v>
@@ -3984,10 +4198,10 @@
       </c>
       <c r="N21" s="61">
         <f t="shared" si="10"/>
-        <v>257.75</v>
+        <v>283.77777777777777</v>
       </c>
       <c r="O21" s="165">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
       <c r="P21" s="8">
@@ -4006,7 +4220,7 @@
         <v>2</v>
       </c>
       <c r="V21" s="62">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="W21" s="2" t="s">
         <v>57</v>
@@ -4024,37 +4238,37 @@
         <v>37</v>
       </c>
       <c r="B22" s="139">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="C22" s="88">
+        <f t="shared" si="5"/>
+        <v>39</v>
+      </c>
+      <c r="D22" s="92">
+        <v>0</v>
+      </c>
+      <c r="E22" s="183">
+        <f t="shared" si="7"/>
+        <v>50</v>
+      </c>
+      <c r="F22" s="189" t="s">
+        <v>57</v>
+      </c>
+      <c r="G22" s="100" t="s">
+        <v>57</v>
+      </c>
+      <c r="H22" s="149" t="s">
+        <v>57</v>
+      </c>
+      <c r="I22" s="149">
         <f t="shared" si="2"/>
-        <v>20</v>
-      </c>
-      <c r="C22" s="88">
-        <f t="shared" si="8"/>
-        <v>39</v>
-      </c>
-      <c r="D22" s="92">
-        <v>0</v>
-      </c>
-      <c r="E22" s="85">
-        <f t="shared" si="3"/>
         <v>50</v>
       </c>
-      <c r="F22" s="156">
-        <v>0</v>
-      </c>
-      <c r="G22" s="149">
-        <v>0</v>
-      </c>
-      <c r="H22" s="149">
-        <f t="shared" si="6"/>
-        <v>25</v>
-      </c>
-      <c r="I22" s="97">
-        <v>0</v>
-      </c>
-      <c r="J22" s="147">
-        <v>0</v>
-      </c>
-      <c r="K22" s="173">
+      <c r="J22" s="97">
+        <v>0</v>
+      </c>
+      <c r="K22" s="147">
         <v>0</v>
       </c>
       <c r="L22" s="108">
@@ -4065,10 +4279,10 @@
       </c>
       <c r="N22" s="61">
         <f t="shared" si="10"/>
-        <v>384</v>
+        <v>409</v>
       </c>
       <c r="O22" s="165">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
       <c r="P22" s="8">
@@ -4086,8 +4300,8 @@
       <c r="U22" s="2">
         <v>25</v>
       </c>
-      <c r="V22" s="62" t="s">
-        <v>57</v>
+      <c r="V22" s="62">
+        <v>15</v>
       </c>
       <c r="W22" s="2" t="s">
         <v>57</v>
@@ -4108,36 +4322,35 @@
         <v>0</v>
       </c>
       <c r="C23" s="88">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D23" s="92">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
-      <c r="E23" s="85">
-        <f t="shared" si="3"/>
+      <c r="E23" s="183">
+        <f t="shared" si="7"/>
         <v>40</v>
       </c>
-      <c r="F23" s="156">
-        <v>0</v>
-      </c>
-      <c r="G23" s="149">
-        <v>0</v>
-      </c>
-      <c r="H23" s="149">
-        <f t="shared" si="6"/>
-        <v>20</v>
-      </c>
-      <c r="I23" s="97">
-        <v>0</v>
-      </c>
-      <c r="J23" s="147">
-        <v>0</v>
-      </c>
-      <c r="K23" s="173">
-        <f>11*(20/32)</f>
-        <v>6.875</v>
+      <c r="F23" s="189">
+        <v>6.1111111111111116</v>
+      </c>
+      <c r="G23" s="100" t="s">
+        <v>57</v>
+      </c>
+      <c r="H23" s="149" t="s">
+        <v>57</v>
+      </c>
+      <c r="I23" s="149">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="J23" s="97">
+        <v>0</v>
+      </c>
+      <c r="K23" s="147">
+        <v>0</v>
       </c>
       <c r="L23" s="108">
         <v>0</v>
@@ -4147,10 +4360,10 @@
       </c>
       <c r="N23" s="61">
         <f t="shared" si="10"/>
-        <v>196.875</v>
+        <v>216.11111111111111</v>
       </c>
       <c r="O23" s="165">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
       <c r="P23" s="8">
@@ -4168,8 +4381,8 @@
       <c r="U23" s="2">
         <v>20</v>
       </c>
-      <c r="V23" s="62" t="s">
-        <v>57</v>
+      <c r="V23" s="62">
+        <v>20</v>
       </c>
       <c r="W23" s="2" t="s">
         <v>57</v>
@@ -4190,32 +4403,32 @@
         <v>0</v>
       </c>
       <c r="C24" s="88">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>1.5</v>
       </c>
       <c r="D24" s="92">
         <v>0</v>
       </c>
-      <c r="E24" s="85">
-        <v>0</v>
-      </c>
-      <c r="F24" s="156">
-        <v>0</v>
-      </c>
-      <c r="G24" s="149">
-        <v>0</v>
-      </c>
-      <c r="H24" s="149">
-        <v>0</v>
-      </c>
-      <c r="I24" s="97">
-        <v>0</v>
-      </c>
-      <c r="J24" s="147">
-        <v>0</v>
-      </c>
-      <c r="K24" s="173">
-        <v>100</v>
+      <c r="E24" s="183">
+        <v>0</v>
+      </c>
+      <c r="F24" s="189">
+        <v>55.555555555555557</v>
+      </c>
+      <c r="G24" s="100" t="s">
+        <v>57</v>
+      </c>
+      <c r="H24" s="149" t="s">
+        <v>57</v>
+      </c>
+      <c r="I24" s="149" t="s">
+        <v>57</v>
+      </c>
+      <c r="J24" s="97">
+        <v>0</v>
+      </c>
+      <c r="K24" s="147">
+        <v>0</v>
       </c>
       <c r="L24" s="108">
         <v>0</v>
@@ -4225,10 +4438,10 @@
       </c>
       <c r="N24" s="61">
         <f t="shared" si="10"/>
-        <v>132.5</v>
-      </c>
-      <c r="O24" s="175">
-        <f t="shared" si="7"/>
+        <v>88.055555555555557</v>
+      </c>
+      <c r="O24" s="172">
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
       <c r="P24" s="15">
@@ -4265,38 +4478,37 @@
         <v>40</v>
       </c>
       <c r="B25" s="139">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
       <c r="C25" s="88">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="D25" s="92">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
-      <c r="E25" s="85">
-        <v>0</v>
-      </c>
-      <c r="F25" s="156">
-        <v>0</v>
-      </c>
-      <c r="G25" s="149">
-        <v>0</v>
-      </c>
-      <c r="H25" s="149">
-        <v>0</v>
-      </c>
-      <c r="I25" s="97">
+      <c r="E25" s="183">
+        <v>0</v>
+      </c>
+      <c r="F25" s="189">
+        <v>16.111111111111111</v>
+      </c>
+      <c r="G25" s="100" t="s">
+        <v>57</v>
+      </c>
+      <c r="H25" s="149" t="s">
+        <v>57</v>
+      </c>
+      <c r="I25" s="149" t="s">
+        <v>57</v>
+      </c>
+      <c r="J25" s="97">
         <v>1</v>
       </c>
-      <c r="J25" s="147">
-        <v>0</v>
-      </c>
-      <c r="K25" s="173">
-        <f>29*(20/32)</f>
-        <v>18.125</v>
+      <c r="K25" s="147">
+        <v>0</v>
       </c>
       <c r="L25" s="108">
         <v>0</v>
@@ -4306,10 +4518,10 @@
       </c>
       <c r="N25" s="61">
         <f t="shared" si="10"/>
-        <v>228.125</v>
+        <v>226.11111111111111</v>
       </c>
       <c r="O25" s="165">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
       <c r="P25" s="8">
@@ -4327,8 +4539,8 @@
       <c r="U25" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="V25" s="62" t="s">
-        <v>57</v>
+      <c r="V25" s="62">
+        <v>15</v>
       </c>
       <c r="W25" s="2" t="s">
         <v>57</v>
@@ -4346,40 +4558,39 @@
         <v>41</v>
       </c>
       <c r="B26" s="139">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
       <c r="C26" s="88">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>40.5</v>
       </c>
       <c r="D26" s="92">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
-      <c r="E26" s="85">
-        <f t="shared" si="3"/>
+      <c r="E26" s="183">
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
-      <c r="F26" s="156">
-        <v>0</v>
-      </c>
-      <c r="G26" s="149">
-        <v>0</v>
-      </c>
-      <c r="H26" s="149">
-        <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-      <c r="I26" s="97">
-        <v>0</v>
-      </c>
-      <c r="J26" s="147">
-        <v>0</v>
-      </c>
-      <c r="K26" s="173">
-        <f>27*(20/32)</f>
-        <v>16.875</v>
+      <c r="F26" s="189">
+        <v>15</v>
+      </c>
+      <c r="G26" s="100" t="s">
+        <v>57</v>
+      </c>
+      <c r="H26" s="149" t="s">
+        <v>57</v>
+      </c>
+      <c r="I26" s="149">
+        <f>$U$40*U26</f>
+        <v>8</v>
+      </c>
+      <c r="J26" s="97">
+        <v>0</v>
+      </c>
+      <c r="K26" s="147">
+        <v>0</v>
       </c>
       <c r="L26" s="108">
         <v>0</v>
@@ -4389,10 +4600,10 @@
       </c>
       <c r="N26" s="61">
         <f t="shared" si="10"/>
-        <v>269.375</v>
+        <v>271.5</v>
       </c>
       <c r="O26" s="165">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
       <c r="P26" s="8">
@@ -4410,8 +4621,8 @@
       <c r="U26" s="2">
         <v>4</v>
       </c>
-      <c r="V26" s="62" t="s">
-        <v>57</v>
+      <c r="V26" s="62">
+        <v>15</v>
       </c>
       <c r="W26" s="2" t="s">
         <v>57</v>
@@ -4429,38 +4640,37 @@
         <v>42</v>
       </c>
       <c r="B27" s="139">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
       <c r="C27" s="88">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>1.5</v>
       </c>
       <c r="D27" s="92">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
-      <c r="E27" s="85">
-        <v>0</v>
-      </c>
-      <c r="F27" s="156">
-        <v>0</v>
-      </c>
-      <c r="G27" s="149">
-        <v>0</v>
-      </c>
-      <c r="H27" s="149">
-        <v>0</v>
-      </c>
-      <c r="I27" s="97">
-        <v>0</v>
-      </c>
-      <c r="J27" s="147">
-        <v>0</v>
-      </c>
-      <c r="K27" s="173">
-        <f>23*(20/32)</f>
-        <v>14.375</v>
+      <c r="E27" s="183" t="s">
+        <v>57</v>
+      </c>
+      <c r="F27" s="189">
+        <v>12.777777777777779</v>
+      </c>
+      <c r="G27" s="186" t="s">
+        <v>57</v>
+      </c>
+      <c r="H27" s="149" t="s">
+        <v>57</v>
+      </c>
+      <c r="I27" s="149" t="s">
+        <v>57</v>
+      </c>
+      <c r="J27" s="97">
+        <v>0</v>
+      </c>
+      <c r="K27" s="147">
+        <v>0</v>
       </c>
       <c r="L27" s="108">
         <v>0</v>
@@ -4470,10 +4680,10 @@
       </c>
       <c r="N27" s="61">
         <f t="shared" si="10"/>
-        <v>215.875</v>
+        <v>214.27777777777777</v>
       </c>
       <c r="O27" s="165">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
       <c r="P27" s="8">
@@ -4491,8 +4701,8 @@
       <c r="U27" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="V27" s="62" t="s">
-        <v>57</v>
+      <c r="V27" s="62">
+        <v>15</v>
       </c>
       <c r="W27" s="2" t="s">
         <v>57</v>
@@ -4510,38 +4720,37 @@
         <v>43</v>
       </c>
       <c r="B28" s="139">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
       <c r="C28" s="88">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>7.5</v>
       </c>
       <c r="D28" s="92">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
-      <c r="E28" s="85">
-        <v>0</v>
-      </c>
-      <c r="F28" s="156">
-        <v>0</v>
-      </c>
-      <c r="G28" s="149">
-        <v>0</v>
-      </c>
-      <c r="H28" s="149">
-        <v>0</v>
-      </c>
-      <c r="I28" s="97">
-        <v>0</v>
-      </c>
-      <c r="J28" s="147">
-        <v>0</v>
-      </c>
-      <c r="K28" s="173">
-        <f>45*(20/32)</f>
-        <v>28.125</v>
+      <c r="E28" s="183" t="s">
+        <v>57</v>
+      </c>
+      <c r="F28" s="189">
+        <v>25</v>
+      </c>
+      <c r="G28" s="100" t="s">
+        <v>57</v>
+      </c>
+      <c r="H28" s="149" t="s">
+        <v>57</v>
+      </c>
+      <c r="I28" s="149" t="s">
+        <v>57</v>
+      </c>
+      <c r="J28" s="97">
+        <v>0</v>
+      </c>
+      <c r="K28" s="147">
+        <v>0</v>
       </c>
       <c r="L28" s="108">
         <v>0</v>
@@ -4551,10 +4760,10 @@
       </c>
       <c r="N28" s="61">
         <f t="shared" si="10"/>
-        <v>235.625</v>
+        <v>232.5</v>
       </c>
       <c r="O28" s="165">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
       <c r="P28" s="8">
@@ -4572,8 +4781,8 @@
       <c r="U28" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="V28" s="62" t="s">
-        <v>57</v>
+      <c r="V28" s="62">
+        <v>15</v>
       </c>
       <c r="W28" s="2" t="s">
         <v>57</v>
@@ -4594,34 +4803,33 @@
         <v>0</v>
       </c>
       <c r="C29" s="88">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>4.5</v>
       </c>
       <c r="D29" s="92">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
-      <c r="E29" s="85">
-        <v>0</v>
-      </c>
-      <c r="F29" s="156">
-        <v>0</v>
-      </c>
-      <c r="G29" s="149">
-        <v>0</v>
-      </c>
-      <c r="H29" s="149">
-        <v>0</v>
-      </c>
-      <c r="I29" s="97">
-        <v>0</v>
-      </c>
-      <c r="J29" s="147">
-        <v>0</v>
-      </c>
-      <c r="K29" s="173">
-        <f>22*(20/32)</f>
-        <v>13.75</v>
+      <c r="E29" s="183" t="s">
+        <v>57</v>
+      </c>
+      <c r="F29" s="189">
+        <v>12.222222222222223</v>
+      </c>
+      <c r="G29" s="100" t="s">
+        <v>57</v>
+      </c>
+      <c r="H29" s="149" t="s">
+        <v>57</v>
+      </c>
+      <c r="I29" s="149" t="s">
+        <v>57</v>
+      </c>
+      <c r="J29" s="97">
+        <v>0</v>
+      </c>
+      <c r="K29" s="147">
+        <v>0</v>
       </c>
       <c r="L29" s="108">
         <v>0</v>
@@ -4631,10 +4839,10 @@
       </c>
       <c r="N29" s="121">
         <f>SUM(B29:M29)</f>
-        <v>48.25</v>
+        <v>46.722222222222221</v>
       </c>
       <c r="O29" s="21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
       <c r="P29" s="94">
@@ -4652,8 +4860,8 @@
       <c r="U29" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="V29" s="62" t="s">
-        <v>57</v>
+      <c r="V29" s="62">
+        <v>15</v>
       </c>
       <c r="W29" s="62" t="s">
         <v>57</v>
@@ -4671,36 +4879,36 @@
         <v>47</v>
       </c>
       <c r="B30" s="139">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
       <c r="C30" s="88">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>28.5</v>
       </c>
       <c r="D30" s="92">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
-      <c r="E30" s="85">
-        <v>0</v>
-      </c>
-      <c r="F30" s="156">
-        <v>0</v>
-      </c>
-      <c r="G30" s="149">
-        <v>0</v>
-      </c>
-      <c r="H30" s="149">
-        <v>0</v>
-      </c>
-      <c r="I30" s="97">
-        <v>0</v>
-      </c>
-      <c r="J30" s="147">
-        <v>0</v>
-      </c>
-      <c r="K30" s="173">
+      <c r="E30" s="183" t="s">
+        <v>57</v>
+      </c>
+      <c r="F30" s="189" t="s">
+        <v>57</v>
+      </c>
+      <c r="G30" s="100" t="s">
+        <v>57</v>
+      </c>
+      <c r="H30" s="149" t="s">
+        <v>57</v>
+      </c>
+      <c r="I30" s="149" t="s">
+        <v>57</v>
+      </c>
+      <c r="J30" s="97">
+        <v>0</v>
+      </c>
+      <c r="K30" s="147">
         <v>0</v>
       </c>
       <c r="L30" s="108">
@@ -4714,7 +4922,7 @@
         <v>228.5</v>
       </c>
       <c r="O30" s="165">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
       <c r="P30" s="8">
@@ -4732,8 +4940,8 @@
       <c r="U30" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="V30" s="62" t="s">
-        <v>57</v>
+      <c r="V30" s="62">
+        <v>15</v>
       </c>
       <c r="W30" s="2" t="s">
         <v>57</v>
@@ -4757,28 +4965,28 @@
         <v>0</v>
       </c>
       <c r="D31" s="92">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
-      <c r="E31" s="85">
-        <v>0</v>
-      </c>
-      <c r="F31" s="156">
-        <v>0</v>
-      </c>
-      <c r="G31" s="149">
-        <v>0</v>
-      </c>
-      <c r="H31" s="149">
-        <v>0</v>
-      </c>
-      <c r="I31" s="97">
-        <v>0</v>
-      </c>
-      <c r="J31" s="147">
-        <v>0</v>
-      </c>
-      <c r="K31" s="173">
+      <c r="E31" s="183" t="s">
+        <v>57</v>
+      </c>
+      <c r="F31" s="189" t="s">
+        <v>57</v>
+      </c>
+      <c r="G31" s="100" t="s">
+        <v>57</v>
+      </c>
+      <c r="H31" s="149" t="s">
+        <v>57</v>
+      </c>
+      <c r="I31" s="149" t="s">
+        <v>57</v>
+      </c>
+      <c r="J31" s="97">
+        <v>0</v>
+      </c>
+      <c r="K31" s="147">
         <v>0</v>
       </c>
       <c r="L31" s="108">
@@ -4792,7 +5000,7 @@
         <v>30</v>
       </c>
       <c r="O31" s="21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
       <c r="P31" s="94">
@@ -4810,8 +5018,8 @@
       <c r="U31" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="V31" s="62" t="s">
-        <v>57</v>
+      <c r="V31" s="62">
+        <v>15</v>
       </c>
       <c r="W31" s="62" t="s">
         <v>57</v>
@@ -4832,32 +5040,32 @@
         <v>0</v>
       </c>
       <c r="C32" s="88">
-        <f>T32*$T$40</f>
+        <f t="shared" si="5"/>
         <v>13.5</v>
       </c>
       <c r="D32" s="92">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
-      <c r="E32" s="85">
-        <v>0</v>
-      </c>
-      <c r="F32" s="156">
-        <v>0</v>
-      </c>
-      <c r="G32" s="149">
-        <v>0</v>
-      </c>
-      <c r="H32" s="149">
-        <v>0</v>
-      </c>
-      <c r="I32" s="97">
-        <v>0</v>
-      </c>
-      <c r="J32" s="147">
-        <v>0</v>
-      </c>
-      <c r="K32" s="173">
+      <c r="E32" s="183" t="s">
+        <v>57</v>
+      </c>
+      <c r="F32" s="189" t="s">
+        <v>57</v>
+      </c>
+      <c r="G32" s="100" t="s">
+        <v>57</v>
+      </c>
+      <c r="H32" s="149" t="s">
+        <v>57</v>
+      </c>
+      <c r="I32" s="149" t="s">
+        <v>57</v>
+      </c>
+      <c r="J32" s="97">
+        <v>0</v>
+      </c>
+      <c r="K32" s="147">
         <v>0</v>
       </c>
       <c r="L32" s="108">
@@ -4871,7 +5079,7 @@
         <v>143.5</v>
       </c>
       <c r="O32" s="165">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
       <c r="P32" s="8">
@@ -4889,8 +5097,8 @@
       <c r="U32" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="V32" s="62" t="s">
-        <v>57</v>
+      <c r="V32" s="62">
+        <v>20</v>
       </c>
       <c r="W32" s="62" t="s">
         <v>57</v>
@@ -4911,34 +5119,33 @@
         <v>0</v>
       </c>
       <c r="C33" s="88">
-        <f>T33*$T$40</f>
+        <f t="shared" si="5"/>
         <v>34.5</v>
       </c>
       <c r="D33" s="92">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
-      <c r="E33" s="85">
-        <v>0</v>
-      </c>
-      <c r="F33" s="156">
-        <v>0</v>
-      </c>
-      <c r="G33" s="149">
-        <v>0</v>
-      </c>
-      <c r="H33" s="149">
-        <v>0</v>
-      </c>
-      <c r="I33" s="97">
-        <v>0</v>
-      </c>
-      <c r="J33" s="147">
-        <v>0</v>
-      </c>
-      <c r="K33" s="173">
-        <f>23*(20/32)</f>
-        <v>14.375</v>
+      <c r="E33" s="183" t="s">
+        <v>57</v>
+      </c>
+      <c r="F33" s="189">
+        <v>12.777777777777779</v>
+      </c>
+      <c r="G33" s="100" t="s">
+        <v>57</v>
+      </c>
+      <c r="H33" s="149" t="s">
+        <v>57</v>
+      </c>
+      <c r="I33" s="149" t="s">
+        <v>57</v>
+      </c>
+      <c r="J33" s="97">
+        <v>0</v>
+      </c>
+      <c r="K33" s="147">
+        <v>0</v>
       </c>
       <c r="L33" s="108">
         <v>0</v>
@@ -4948,10 +5155,10 @@
       </c>
       <c r="N33" s="121">
         <f>SUM(B33:M33)+Y33</f>
-        <v>80.875</v>
+        <v>79.277777777777771</v>
       </c>
       <c r="O33" s="21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
       <c r="P33" s="94">
@@ -4969,8 +5176,8 @@
       <c r="U33" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="V33" s="62" t="s">
-        <v>57</v>
+      <c r="V33" s="62">
+        <v>20</v>
       </c>
       <c r="W33" s="62" t="s">
         <v>57</v>
@@ -4994,28 +5201,28 @@
         <v>0</v>
       </c>
       <c r="D34" s="92">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>60</v>
       </c>
-      <c r="E34" s="85">
-        <v>0</v>
-      </c>
-      <c r="F34" s="156">
-        <v>0</v>
-      </c>
-      <c r="G34" s="149">
-        <v>0</v>
-      </c>
-      <c r="H34" s="149">
-        <v>0</v>
-      </c>
-      <c r="I34" s="97">
-        <v>0</v>
-      </c>
-      <c r="J34" s="147">
-        <v>0</v>
-      </c>
-      <c r="K34" s="173">
+      <c r="E34" s="183" t="s">
+        <v>57</v>
+      </c>
+      <c r="F34" s="189" t="s">
+        <v>57</v>
+      </c>
+      <c r="G34" s="100" t="s">
+        <v>57</v>
+      </c>
+      <c r="H34" s="149" t="s">
+        <v>57</v>
+      </c>
+      <c r="I34" s="149" t="s">
+        <v>57</v>
+      </c>
+      <c r="J34" s="97">
+        <v>0</v>
+      </c>
+      <c r="K34" s="147">
         <v>0</v>
       </c>
       <c r="L34" s="108">
@@ -5029,7 +5236,7 @@
         <v>160</v>
       </c>
       <c r="O34" s="165">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
       <c r="P34" s="8">
@@ -5047,8 +5254,8 @@
       <c r="U34" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="V34" s="62" t="s">
-        <v>57</v>
+      <c r="V34" s="62">
+        <v>20</v>
       </c>
       <c r="W34" s="62" t="s">
         <v>57</v>
@@ -5069,36 +5276,35 @@
         <v>0</v>
       </c>
       <c r="C35" s="88">
-        <f>T35*$T$40</f>
+        <f t="shared" si="5"/>
         <v>10.5</v>
       </c>
       <c r="D35" s="92">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
-      <c r="E35" s="85">
-        <f t="shared" si="3"/>
+      <c r="E35" s="183">
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
-      <c r="F35" s="156">
-        <v>0</v>
-      </c>
-      <c r="G35" s="149">
-        <v>0</v>
-      </c>
-      <c r="H35" s="149">
-        <f t="shared" si="6"/>
-        <v>4</v>
-      </c>
-      <c r="I35" s="97">
-        <v>0</v>
-      </c>
-      <c r="J35" s="147">
-        <v>0</v>
-      </c>
-      <c r="K35" s="173">
-        <f>29*(20/32)</f>
-        <v>18.125</v>
+      <c r="F35" s="189">
+        <v>16.111111111111111</v>
+      </c>
+      <c r="G35" s="100" t="s">
+        <v>57</v>
+      </c>
+      <c r="H35" s="149" t="s">
+        <v>57</v>
+      </c>
+      <c r="I35" s="149">
+        <f>$U$40*U35</f>
+        <v>8</v>
+      </c>
+      <c r="J35" s="97">
+        <v>0</v>
+      </c>
+      <c r="K35" s="147">
+        <v>0</v>
       </c>
       <c r="L35" s="108">
         <v>0</v>
@@ -5108,10 +5314,10 @@
       </c>
       <c r="N35" s="61">
         <f>SUM(B35:M35)+Y35+Z35</f>
-        <v>146.125</v>
+        <v>148.11111111111111</v>
       </c>
       <c r="O35" s="165">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
       <c r="P35" s="8">
@@ -5129,8 +5335,8 @@
       <c r="U35" s="2">
         <v>4</v>
       </c>
-      <c r="V35" s="62" t="s">
-        <v>57</v>
+      <c r="V35" s="62">
+        <v>15</v>
       </c>
       <c r="W35" s="62" t="s">
         <v>57</v>
@@ -5152,32 +5358,32 @@
         <v>0</v>
       </c>
       <c r="C36" s="89">
-        <f>T36*$T$40</f>
+        <f>$T$40*T36</f>
         <v>13.5</v>
       </c>
       <c r="D36" s="93">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
-      <c r="E36" s="86">
-        <v>0</v>
-      </c>
-      <c r="F36" s="157">
-        <v>0</v>
-      </c>
-      <c r="G36" s="158">
-        <v>0</v>
-      </c>
-      <c r="H36" s="158">
-        <v>0</v>
-      </c>
-      <c r="I36" s="98">
-        <v>0</v>
-      </c>
-      <c r="J36" s="148">
-        <v>0</v>
-      </c>
-      <c r="K36" s="174">
+      <c r="E36" s="184" t="s">
+        <v>57</v>
+      </c>
+      <c r="F36" s="190" t="s">
+        <v>57</v>
+      </c>
+      <c r="G36" s="101" t="s">
+        <v>57</v>
+      </c>
+      <c r="H36" s="158" t="s">
+        <v>57</v>
+      </c>
+      <c r="I36" s="158" t="s">
+        <v>57</v>
+      </c>
+      <c r="J36" s="98">
+        <v>0</v>
+      </c>
+      <c r="K36" s="148">
         <v>0</v>
       </c>
       <c r="L36" s="109">
@@ -5191,7 +5397,7 @@
         <v>122.5</v>
       </c>
       <c r="O36" s="170">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
       <c r="P36" s="9">
@@ -5225,17 +5431,17 @@
     </row>
     <row r="37" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
-      <c r="F37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
-      <c r="N37" s="185" t="s">
+      <c r="L37" s="2"/>
+      <c r="N37" s="196" t="s">
         <v>111</v>
       </c>
-      <c r="O37" s="186"/>
-      <c r="P37" s="187"/>
+      <c r="O37" s="197"/>
+      <c r="P37" s="198"/>
       <c r="R37" s="2"/>
       <c r="S37" s="119"/>
       <c r="T37" s="2"/>
@@ -5247,12 +5453,12 @@
       <c r="B38" t="s">
         <v>66</v>
       </c>
-      <c r="F38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
       <c r="P38" s="2"/>
@@ -5267,12 +5473,12 @@
       <c r="B39" t="s">
         <v>114</v>
       </c>
-      <c r="F39" s="2"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
       <c r="P39" s="2"/>
@@ -5299,12 +5505,12 @@
       <c r="B40" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="F40" s="2"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
       <c r="P40" s="2"/>
@@ -5321,16 +5527,16 @@
         <v>2</v>
       </c>
       <c r="V40" s="2">
-        <v>0.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="F41" s="2"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
       <c r="N41" s="2"/>
       <c r="O41" s="2"/>
       <c r="P41" s="2"/>
@@ -5342,12 +5548,12 @@
       <c r="U41" s="2"/>
     </row>
     <row r="42" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="F42" s="2"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
       <c r="N42" s="2"/>
       <c r="O42" s="2"/>
       <c r="P42" s="2"/>
@@ -5357,14 +5563,14 @@
       <c r="U42" s="2"/>
     </row>
     <row r="43" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="F43" s="2"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
-      <c r="L43" s="179" t="s">
-        <v>132</v>
+      <c r="L43" s="2"/>
+      <c r="M43" s="175" t="s">
+        <v>131</v>
       </c>
       <c r="N43" s="2"/>
       <c r="O43" s="2"/>
@@ -5377,16 +5583,16 @@
       <c r="U43" s="2"/>
     </row>
     <row r="44" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="F44" s="2"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
-      <c r="K44" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="L44" t="s">
-        <v>133</v>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="M44" t="s">
+        <v>132</v>
       </c>
       <c r="N44" s="2"/>
       <c r="O44" s="2"/>
@@ -5396,16 +5602,16 @@
       <c r="T44" s="2"/>
     </row>
     <row r="45" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="F45" s="2"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
-      <c r="K45" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="L45" t="s">
-        <v>134</v>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="M45" t="s">
+        <v>133</v>
       </c>
       <c r="N45" s="2"/>
       <c r="O45" s="2"/>
@@ -5415,108 +5621,115 @@
       <c r="T45" s="2"/>
     </row>
     <row r="46" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="F46" s="2"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
-      <c r="K46" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="L46" t="s">
-        <v>135</v>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="M46" t="s">
+        <v>134</v>
       </c>
       <c r="N46" s="2"/>
       <c r="O46" s="2"/>
       <c r="P46" s="2"/>
       <c r="Q46" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="R46" s="2"/>
       <c r="S46" s="119"/>
       <c r="T46" s="2"/>
     </row>
     <row r="47" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="K47" s="2" t="s">
+      <c r="L47" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="M47" t="s">
         <v>138</v>
       </c>
-      <c r="L47" t="s">
+    </row>
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="L48" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="M48" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="K48" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="L48" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="11"/>
       <c r="B59" s="4" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E59" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="12" t="s">
         <v>53</v>
       </c>
       <c r="B60" s="134">
         <v>357</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E60">
+        <f>20/36</f>
+        <v>0.55555555555555558</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="130" t="s">
         <v>20</v>
       </c>
@@ -5524,7 +5737,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="130" t="s">
         <v>52</v>
       </c>
@@ -5532,7 +5745,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="130" t="s">
         <v>21</v>
       </c>
@@ -5543,7 +5756,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="130" t="s">
         <v>22</v>
       </c>
@@ -5805,7 +6018,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD46"/>
   <sheetViews>
@@ -8728,11 +8941,11 @@
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
-      <c r="N37" s="185" t="s">
+      <c r="N37" s="199" t="s">
         <v>111</v>
       </c>
-      <c r="O37" s="186"/>
-      <c r="P37" s="187"/>
+      <c r="O37" s="200"/>
+      <c r="P37" s="201"/>
       <c r="R37" s="2"/>
       <c r="S37" s="119"/>
       <c r="T37" s="2"/>
@@ -8918,7 +9131,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB46"/>
   <sheetViews>
@@ -11582,10 +11795,10 @@
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
-      <c r="M37" s="185" t="s">
+      <c r="M37" s="199" t="s">
         <v>111</v>
       </c>
-      <c r="N37" s="187"/>
+      <c r="N37" s="201"/>
       <c r="P37" s="2"/>
       <c r="Q37" s="119"/>
       <c r="R37" s="2"/>
@@ -11753,7 +11966,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA47"/>
   <sheetViews>
@@ -14015,10 +14228,10 @@
       <c r="X36" s="2"/>
     </row>
     <row r="37" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L37" s="188" t="s">
+      <c r="L37" s="202" t="s">
         <v>77</v>
       </c>
-      <c r="M37" s="189"/>
+      <c r="M37" s="203"/>
       <c r="O37" s="2"/>
       <c r="P37" s="2"/>
       <c r="Q37" s="2"/>
@@ -14110,7 +14323,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB47"/>
   <sheetViews>
@@ -16323,10 +16536,10 @@
     </row>
     <row r="37" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K37" s="62"/>
-      <c r="L37" s="190" t="s">
+      <c r="L37" s="204" t="s">
         <v>77</v>
       </c>
-      <c r="M37" s="189"/>
+      <c r="M37" s="203"/>
       <c r="O37" s="2"/>
       <c r="P37" s="2"/>
       <c r="Q37" s="2"/>
@@ -16418,7 +16631,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C19"/>
   <sheetViews>
@@ -16444,7 +16657,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="191" t="s">
+      <c r="A2" s="205" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="46" t="s">
@@ -16455,7 +16668,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="193"/>
+      <c r="A3" s="207"/>
       <c r="B3" s="47" t="s">
         <v>4</v>
       </c>
@@ -16464,7 +16677,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="183" t="s">
+      <c r="A4" s="194" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="48" t="s">
@@ -16475,7 +16688,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="184"/>
+      <c r="A5" s="195"/>
       <c r="B5" s="50" t="s">
         <v>9</v>
       </c>
@@ -16484,7 +16697,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="191" t="s">
+      <c r="A6" s="205" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="46" t="s">
@@ -16495,7 +16708,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="192"/>
+      <c r="A7" s="206"/>
       <c r="B7" s="51" t="s">
         <v>13</v>
       </c>
@@ -16504,7 +16717,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="184"/>
+      <c r="A8" s="195"/>
       <c r="B8" s="50" t="s">
         <v>14</v>
       </c>
@@ -16525,7 +16738,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="191" t="s">
+      <c r="A11" s="205" t="s">
         <v>2</v>
       </c>
       <c r="B11" s="46" t="s">
@@ -16536,7 +16749,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="193"/>
+      <c r="A12" s="207"/>
       <c r="B12" s="47" t="s">
         <v>4</v>
       </c>
@@ -16545,7 +16758,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="183" t="s">
+      <c r="A13" s="194" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="48" t="s">
@@ -16556,7 +16769,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="181"/>
+      <c r="A14" s="192"/>
       <c r="B14" s="49" t="s">
         <v>9</v>
       </c>
@@ -16565,7 +16778,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="181"/>
+      <c r="A15" s="192"/>
       <c r="B15" s="49" t="s">
         <v>74</v>
       </c>
@@ -16574,7 +16787,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="184"/>
+      <c r="A16" s="195"/>
       <c r="B16" s="50" t="s">
         <v>80</v>
       </c>
@@ -16583,7 +16796,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="191" t="s">
+      <c r="A17" s="205" t="s">
         <v>11</v>
       </c>
       <c r="B17" s="46" t="s">
@@ -16594,7 +16807,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="192"/>
+      <c r="A18" s="206"/>
       <c r="B18" s="51" t="s">
         <v>13</v>
       </c>
@@ -16603,7 +16816,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="184"/>
+      <c r="A19" s="195"/>
       <c r="B19" s="50" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
(C)    meal plan updates, less calories
</commit_message>
<xml_diff>
--- a/Suppl/nutrition plan.xlsx
+++ b/Suppl/nutrition plan.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1102" uniqueCount="155">
   <si>
     <t>Meal</t>
   </si>
@@ -466,21 +466,41 @@
     <t>Time</t>
   </si>
   <si>
-    <t>Post Workout Meal</t>
+    <t>Lunch (TP Shake)</t>
   </si>
   <si>
-    <t>Lunch (TP Shake)</t>
+    <t>(1 Blender Bottle, 28 oz)</t>
+  </si>
+  <si>
+    <t>(1Botl)</t>
+  </si>
+  <si>
+    <t>79</t>
+  </si>
+  <si>
+    <t>(Justin's Recipe, see /shake)</t>
+  </si>
+  <si>
+    <t>(normal is N=1.5)</t>
+  </si>
+  <si>
+    <t>(normal is N=2)</t>
+  </si>
+  <si>
+    <t>Pre-Workout Meal</t>
+  </si>
+  <si>
+    <t>Post-Workout Meal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="0.0"/>
+  <numFmts count="1">
     <numFmt numFmtId="165" formatCode="h\ AM/PM"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -517,6 +537,14 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="0" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1393,7 +1421,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="225">
+  <cellXfs count="230">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1905,67 +1933,10 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="15" borderId="58" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="15" borderId="59" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="15" borderId="60" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1989,6 +1960,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2011,6 +2006,48 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="15" borderId="59" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="15" borderId="60" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2380,7 +2417,7 @@
       <c r="C2" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="185" t="s">
+      <c r="E2" s="198" t="s">
         <v>91</v>
       </c>
       <c r="F2" s="79" t="s">
@@ -2398,7 +2435,7 @@
       <c r="C3" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="E3" s="186"/>
+      <c r="E3" s="199"/>
       <c r="F3" s="83" t="s">
         <v>93</v>
       </c>
@@ -2414,7 +2451,7 @@
       <c r="C4" s="53" t="s">
         <v>118</v>
       </c>
-      <c r="E4" s="187"/>
+      <c r="E4" s="200"/>
       <c r="F4" s="81" t="s">
         <v>9</v>
       </c>
@@ -2423,7 +2460,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="188" t="s">
+      <c r="A5" s="201" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="48" t="s">
@@ -2432,7 +2469,7 @@
       <c r="C5" s="54" t="s">
         <v>90</v>
       </c>
-      <c r="E5" s="185" t="s">
+      <c r="E5" s="198" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="82" t="s">
@@ -2443,14 +2480,14 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="186"/>
+      <c r="A6" s="199"/>
       <c r="B6" s="78" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="186"/>
+      <c r="E6" s="199"/>
       <c r="F6" s="80" t="s">
         <v>97</v>
       </c>
@@ -2459,14 +2496,14 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="189"/>
+      <c r="A7" s="202"/>
       <c r="B7" s="50" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="56" t="s">
         <v>101</v>
       </c>
-      <c r="E7" s="187"/>
+      <c r="E7" s="200"/>
       <c r="F7" s="81" t="s">
         <v>84</v>
       </c>
@@ -2486,10 +2523,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2528,22 +2565,30 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="183">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="B5" s="229" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="183">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="184">
+      <c r="B6" s="8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="184">
         <v>0.79166666666666663</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B7" s="9" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2555,10 +2600,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD94"/>
+  <dimension ref="A1:AC94"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="B18" sqref="B18:P36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2567,11 +2612,11 @@
     <col min="2" max="16" width="8.28515625" customWidth="1"/>
     <col min="19" max="19" width="9.140625" style="117"/>
     <col min="22" max="22" width="11.85546875" customWidth="1"/>
-    <col min="23" max="23" width="11.42578125" customWidth="1"/>
-    <col min="26" max="26" width="10.85546875" customWidth="1"/>
+    <col min="23" max="24" width="11.42578125" customWidth="1"/>
+    <col min="27" max="27" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11"/>
       <c r="B1" s="4" t="s">
         <v>54</v>
@@ -2588,7 +2633,7 @@
       <c r="F1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="208" t="s">
+      <c r="G1" s="189" t="s">
         <v>143</v>
       </c>
       <c r="H1" s="4" t="s">
@@ -2618,38 +2663,42 @@
       <c r="P1" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="228" t="s">
         <v>61</v>
       </c>
-      <c r="S1" s="117" t="s">
+      <c r="S1" s="228" t="s">
         <v>102</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="228" t="s">
         <v>56</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="228" t="s">
         <v>62</v>
       </c>
-      <c r="V1" t="s">
+      <c r="V1" s="228" t="s">
         <v>144</v>
       </c>
-      <c r="W1" t="s">
+      <c r="W1" s="228" t="s">
         <v>106</v>
       </c>
-      <c r="Y1" s="59" t="s">
+      <c r="X1" s="227" t="s">
+        <v>148</v>
+      </c>
+      <c r="Y1" s="223"/>
+      <c r="Z1" s="59" t="s">
         <v>85</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="175" t="s">
         <v>53</v>
       </c>
@@ -2661,19 +2710,19 @@
         <f t="shared" ref="C2" si="0">T2*$T$40</f>
         <v>366</v>
       </c>
-      <c r="D2" s="209">
+      <c r="D2" s="190">
         <f t="shared" ref="D2" si="1">S2*$S$40</f>
-        <v>77.8125</v>
-      </c>
-      <c r="E2" s="210">
+        <v>38.90625</v>
+      </c>
+      <c r="E2" s="191">
         <f>U2*$U$40</f>
-        <v>480</v>
-      </c>
-      <c r="F2" s="202"/>
+        <v>240</v>
+      </c>
+      <c r="F2" s="185"/>
       <c r="G2" s="179"/>
-      <c r="H2" s="206">
+      <c r="H2" s="187">
         <f>V2*V40</f>
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="I2" s="151">
         <f>W2</f>
@@ -2712,14 +2761,13 @@
       <c r="W2" s="62">
         <v>17.2</v>
       </c>
-      <c r="Y2" s="2"/>
+      <c r="X2" s="62"/>
+      <c r="Y2" s="223"/>
       <c r="Z2" s="2"/>
       <c r="AA2" s="2"/>
-      <c r="AD2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AB2" s="2"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="178" t="s">
         <v>20</v>
       </c>
@@ -2729,25 +2777,26 @@
       </c>
       <c r="C3" s="173">
         <f>$S$40*T3</f>
-        <v>183</v>
+        <v>91.5</v>
       </c>
       <c r="D3" s="90">
         <f>S3*S40</f>
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="E3" s="91">
         <f>$U$40*U3</f>
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="F3" s="84">
         <v>105</v>
       </c>
-      <c r="G3" s="203">
-        <v>278.33333333333337</v>
+      <c r="G3" s="186">
+        <f>X40*X3</f>
+        <v>311</v>
       </c>
       <c r="H3" s="153">
         <f>$V$40*V3</f>
-        <v>300</v>
+        <v>150</v>
       </c>
       <c r="I3" s="154">
         <f>W3</f>
@@ -2755,7 +2804,7 @@
       </c>
       <c r="J3" s="155">
         <f t="shared" ref="J3:J23" si="2">$U$40*U3</f>
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="K3" s="147">
         <v>270</v>
@@ -2767,8 +2816,8 @@
         <v>80</v>
       </c>
       <c r="N3" s="167">
-        <f>SUM(B3:M3)+SUM(Y3:AB3)</f>
-        <v>2026.3333333333335</v>
+        <f t="shared" ref="N3:N12" si="3">SUM(B3:M3)+SUM(Z3:AC3)</f>
+        <v>1607.5</v>
       </c>
       <c r="O3" s="168">
         <v>2000</v>
@@ -2778,7 +2827,7 @@
       </c>
       <c r="Q3" s="128">
         <f>N3/O3</f>
-        <v>1.0131666666666668</v>
+        <v>0.80374999999999996</v>
       </c>
       <c r="R3" s="2">
         <v>110</v>
@@ -2798,23 +2847,24 @@
       <c r="W3" s="62">
         <v>5</v>
       </c>
-      <c r="Y3" s="2" t="s">
-        <v>57</v>
-      </c>
+      <c r="X3" s="62">
+        <v>311</v>
+      </c>
+      <c r="Y3" s="224"/>
       <c r="Z3" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="AA3" s="2">
+      <c r="AA3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB3" s="2">
         <v>35</v>
       </c>
-      <c r="AB3" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AC3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="130" t="s">
         <v>52</v>
       </c>
@@ -2828,28 +2878,28 @@
       </c>
       <c r="D4" s="92">
         <f>$S$40*S4</f>
-        <v>45</v>
+        <v>22.5</v>
       </c>
       <c r="E4" s="26">
         <f>U4*$U$40</f>
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="F4" s="85">
         <v>3</v>
       </c>
-      <c r="G4" s="204" t="s">
+      <c r="G4" s="225" t="s">
         <v>57</v>
       </c>
       <c r="H4" s="156">
         <f>$V$40*V4</f>
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="I4" s="149" t="s">
         <v>57</v>
       </c>
       <c r="J4" s="97">
         <f t="shared" si="2"/>
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="K4" s="147">
         <v>60</v>
@@ -2861,8 +2911,8 @@
         <v>0</v>
       </c>
       <c r="N4" s="40">
-        <f>SUM(B4:M4)+SUM(Y4:AB4)</f>
-        <v>437.5</v>
+        <f t="shared" si="3"/>
+        <v>315</v>
       </c>
       <c r="O4" s="164" t="s">
         <v>57</v>
@@ -2889,58 +2939,60 @@
       <c r="W4" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="Y4" s="2" t="s">
-        <v>57</v>
-      </c>
+      <c r="X4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y4" s="224"/>
       <c r="Z4" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="AA4" s="2">
+      <c r="AA4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB4" s="2">
         <v>25</v>
       </c>
-      <c r="AB4" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AC4" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="130" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="139">
-        <f t="shared" ref="B5:B30" si="3">$R$40*R5</f>
+        <f t="shared" ref="B5:B30" si="4">$R$40*R5</f>
         <v>0</v>
       </c>
       <c r="C5" s="88">
-        <f t="shared" ref="C5:C35" si="4">$T$40*T5</f>
+        <f t="shared" ref="C5:C35" si="5">$T$40*T5</f>
         <v>0.89999999999999991</v>
       </c>
       <c r="D5" s="92">
-        <f t="shared" ref="D5:D36" si="5">$S$40*S5</f>
-        <v>4.5</v>
+        <f t="shared" ref="D5:D36" si="6">$S$40*S5</f>
+        <v>2.25</v>
       </c>
       <c r="E5" s="26">
-        <f t="shared" ref="E5:E35" si="6">U5*$U$40</f>
-        <v>5</v>
+        <f t="shared" ref="E5:E35" si="7">U5*$U$40</f>
+        <v>2.5</v>
       </c>
       <c r="F5" s="85">
         <v>0</v>
       </c>
-      <c r="G5" s="204">
-        <v>1.0944444444444446</v>
+      <c r="G5" s="225">
+        <f t="shared" ref="G5:G35" si="8">$X$40*X5</f>
+        <v>6</v>
       </c>
       <c r="H5" s="156">
         <f>$V$40*V5</f>
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="I5" s="149" t="s">
         <v>57</v>
       </c>
       <c r="J5" s="97">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="K5" s="147">
         <v>7</v>
@@ -2952,8 +3004,8 @@
         <v>0</v>
       </c>
       <c r="N5" s="122">
-        <f>SUM(B5:M5)+SUM(Y5:AB5)</f>
-        <v>42.994444444444447</v>
+        <f t="shared" si="3"/>
+        <v>34.65</v>
       </c>
       <c r="O5" s="166">
         <f>P5</f>
@@ -2964,7 +3016,7 @@
       </c>
       <c r="Q5" s="128">
         <f>N5/O5</f>
-        <v>0.66145299145299152</v>
+        <v>0.533076923076923</v>
       </c>
       <c r="R5" s="2">
         <v>0</v>
@@ -2984,48 +3036,51 @@
       <c r="W5" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="Y5" s="2" t="s">
-        <v>57</v>
-      </c>
+      <c r="X5" s="2">
+        <v>6</v>
+      </c>
+      <c r="Y5" s="224"/>
       <c r="Z5" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="AA5" s="2">
+      <c r="AA5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB5" s="2">
         <v>3</v>
       </c>
-      <c r="AB5" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AC5" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="130" t="s">
         <v>22</v>
       </c>
       <c r="B6" s="139">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="C6" s="88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.5</v>
       </c>
       <c r="D6" s="92">
-        <f t="shared" si="5"/>
-        <v>1.5</v>
+        <f t="shared" si="6"/>
+        <v>0.75</v>
       </c>
       <c r="E6" s="26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F6" s="85">
         <v>0</v>
       </c>
-      <c r="G6" s="204" t="s">
+      <c r="G6" s="225" t="s">
         <v>57</v>
       </c>
       <c r="H6" s="156">
         <f>$V$40*V6</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I6" s="149" t="s">
         <v>57</v>
@@ -3044,11 +3099,11 @@
         <v>0</v>
       </c>
       <c r="N6" s="40">
-        <f>SUM(B6:M6)+SUM(Y6:AB6)</f>
-        <v>18</v>
+        <f t="shared" si="3"/>
+        <v>14.25</v>
       </c>
       <c r="O6" s="165">
-        <f t="shared" ref="O6:O36" si="7">P6</f>
+        <f t="shared" ref="O6:O36" si="9">P6</f>
         <v>20</v>
       </c>
       <c r="P6" s="8">
@@ -3073,46 +3128,47 @@
       <c r="W6" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="Y6" s="2" t="s">
-        <v>57</v>
-      </c>
+      <c r="X6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y6" s="224"/>
       <c r="Z6" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="AA6" s="2">
+      <c r="AA6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB6" s="2">
         <v>1</v>
       </c>
-      <c r="AB6" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AC6" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="130" t="s">
         <v>23</v>
       </c>
       <c r="B7" s="139">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C7" s="88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D7" s="92">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E7" s="26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F7" s="85">
         <v>0</v>
       </c>
-      <c r="G7" s="204" t="s">
+      <c r="G7" s="225" t="s">
         <v>57</v>
       </c>
       <c r="H7" s="156">
@@ -3136,11 +3192,11 @@
         <v>0</v>
       </c>
       <c r="N7" s="40">
-        <f>SUM(B7:M7)+SUM(Y7:AB7)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O7" s="165" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-</v>
       </c>
       <c r="P7" s="8" t="s">
@@ -3165,45 +3221,46 @@
       <c r="W7" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="Y7" s="2" t="s">
-        <v>57</v>
-      </c>
+      <c r="X7" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y7" s="224"/>
       <c r="Z7" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="AA7" s="2">
+      <c r="AA7" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB7" s="2">
         <v>1</v>
       </c>
-      <c r="AB7" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AC7" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="130" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="139">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C8" s="88">
         <v>0</v>
       </c>
       <c r="D8" s="92">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E8" s="26">
-        <f t="shared" si="6"/>
-        <v>1</v>
+        <f t="shared" si="7"/>
+        <v>0.5</v>
       </c>
       <c r="F8" s="85">
         <v>0</v>
       </c>
-      <c r="G8" s="204" t="s">
+      <c r="G8" s="225" t="s">
         <v>57</v>
       </c>
       <c r="H8" s="156" t="s">
@@ -3214,7 +3271,7 @@
       </c>
       <c r="J8" s="97">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="K8" s="147">
         <v>0</v>
@@ -3226,11 +3283,11 @@
         <v>0</v>
       </c>
       <c r="N8" s="40">
-        <f>SUM(B8:M8)+SUM(Y8:AB8)</f>
-        <v>4.5</v>
+        <f t="shared" si="3"/>
+        <v>3.5</v>
       </c>
       <c r="O8" s="165" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-</v>
       </c>
       <c r="P8" s="8" t="s">
@@ -3255,42 +3312,46 @@
       <c r="W8" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="Y8" s="2" t="s">
-        <v>57</v>
-      </c>
+      <c r="X8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y8" s="224"/>
       <c r="Z8" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="AA8" s="2">
+      <c r="AA8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB8" s="2">
         <v>0.5</v>
       </c>
-      <c r="AB8" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AC8" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="130" t="s">
         <v>25</v>
       </c>
       <c r="B9" s="139">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C9" s="88">
         <v>0</v>
       </c>
       <c r="D9" s="92">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="E9" s="26">
-        <f t="shared" si="6"/>
-        <v>3</v>
+        <f t="shared" si="7"/>
+        <v>1.5</v>
       </c>
       <c r="F9" s="85">
         <v>0</v>
       </c>
-      <c r="G9" s="204" t="s">
+      <c r="G9" s="225" t="s">
         <v>57</v>
       </c>
       <c r="H9" s="156" t="s">
@@ -3301,7 +3362,7 @@
       </c>
       <c r="J9" s="97">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="K9" s="147">
         <v>0</v>
@@ -3313,11 +3374,11 @@
         <v>0</v>
       </c>
       <c r="N9" s="40">
-        <f>SUM(B9:M9)+SUM(Y9:AB9)</f>
-        <v>7</v>
+        <f t="shared" si="3"/>
+        <v>4</v>
       </c>
       <c r="O9" s="165" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-</v>
       </c>
       <c r="P9" s="8" t="s">
@@ -3342,49 +3403,50 @@
       <c r="W9" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="Y9" s="2" t="s">
-        <v>57</v>
-      </c>
+      <c r="X9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y9" s="224"/>
       <c r="Z9" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="AA9" s="2"/>
-      <c r="AB9" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AA9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB9" s="2"/>
+      <c r="AC9" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="130" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="139">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C10" s="88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="D10" s="92">
-        <f t="shared" si="5"/>
-        <v>90</v>
+        <f t="shared" si="6"/>
+        <v>45</v>
       </c>
       <c r="E10" s="26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F10" s="85">
         <v>0</v>
       </c>
-      <c r="G10" s="204" t="s">
+      <c r="G10" s="225" t="s">
         <v>57</v>
       </c>
       <c r="H10" s="156">
         <f>$V$40*V10</f>
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="I10" s="149" t="s">
         <v>57</v>
@@ -3403,11 +3465,11 @@
         <v>10</v>
       </c>
       <c r="N10" s="40">
-        <f>SUM(B10:M10)+SUM(Y10:AB10)</f>
-        <v>210</v>
+        <f t="shared" si="3"/>
+        <v>150</v>
       </c>
       <c r="O10" s="165">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>300</v>
       </c>
       <c r="P10" s="8">
@@ -3432,51 +3494,53 @@
       <c r="W10" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="Y10" s="2" t="s">
-        <v>57</v>
-      </c>
+      <c r="X10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y10" s="224"/>
       <c r="Z10" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="AA10" s="2">
+      <c r="AA10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB10" s="2">
         <v>25</v>
       </c>
-      <c r="AB10" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AC10" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="130" t="s">
         <v>26</v>
       </c>
       <c r="B11" s="139">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>380</v>
       </c>
       <c r="C11" s="88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>150</v>
       </c>
       <c r="D11" s="92">
-        <f t="shared" si="5"/>
-        <v>180</v>
+        <f t="shared" si="6"/>
+        <v>90</v>
       </c>
       <c r="E11" s="26">
-        <f t="shared" si="6"/>
-        <v>320</v>
+        <f t="shared" si="7"/>
+        <v>160</v>
       </c>
       <c r="F11" s="85">
         <v>1</v>
       </c>
-      <c r="G11" s="204" t="s">
-        <v>57</v>
+      <c r="G11" s="225">
+        <f t="shared" si="8"/>
+        <v>276</v>
       </c>
       <c r="H11" s="156">
         <f>$V$40*V11</f>
-        <v>320</v>
+        <v>160</v>
       </c>
       <c r="I11" s="149">
         <f>W11</f>
@@ -3484,7 +3548,7 @@
       </c>
       <c r="J11" s="97">
         <f t="shared" si="2"/>
-        <v>320</v>
+        <v>160</v>
       </c>
       <c r="K11" s="147">
         <v>480</v>
@@ -3496,11 +3560,11 @@
         <v>55</v>
       </c>
       <c r="N11" s="61">
-        <f>SUM(B11:M11)+SUM(Y11:AB11)</f>
-        <v>2546</v>
+        <f t="shared" si="3"/>
+        <v>2252</v>
       </c>
       <c r="O11" s="165">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2400</v>
       </c>
       <c r="P11" s="8">
@@ -3525,44 +3589,46 @@
       <c r="W11" s="62">
         <v>90</v>
       </c>
-      <c r="Y11" s="2" t="s">
-        <v>57</v>
-      </c>
+      <c r="X11" s="62">
+        <v>276</v>
+      </c>
+      <c r="Y11" s="224"/>
       <c r="Z11" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="AA11" s="2"/>
-      <c r="AB11" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AA11" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB11" s="2"/>
+      <c r="AC11" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="130" t="s">
         <v>27</v>
       </c>
       <c r="B12" s="139">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>140</v>
       </c>
       <c r="C12" s="88">
         <v>0</v>
       </c>
       <c r="D12" s="92">
-        <f t="shared" si="5"/>
-        <v>375</v>
+        <f t="shared" si="6"/>
+        <v>187.5</v>
       </c>
       <c r="E12" s="26">
-        <f t="shared" si="6"/>
-        <v>70</v>
+        <f t="shared" si="7"/>
+        <v>35</v>
       </c>
       <c r="F12" s="85">
         <v>0</v>
       </c>
-      <c r="G12" s="204" t="s">
-        <v>57</v>
+      <c r="G12" s="225">
+        <f t="shared" si="8"/>
+        <v>798</v>
       </c>
       <c r="H12" s="156">
         <v>0</v>
@@ -3572,7 +3638,7 @@
       </c>
       <c r="J12" s="97">
         <f t="shared" si="2"/>
-        <v>70</v>
+        <v>35</v>
       </c>
       <c r="K12" s="147">
         <v>0</v>
@@ -3584,11 +3650,11 @@
         <v>160</v>
       </c>
       <c r="N12" s="121">
-        <f>SUM(B12:M12)+SUM(Y12:AB12)</f>
-        <v>922.14285714285711</v>
+        <f t="shared" si="3"/>
+        <v>1462.6428571428571</v>
       </c>
       <c r="O12" s="21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3500</v>
       </c>
       <c r="P12" s="94">
@@ -3613,47 +3679,52 @@
       <c r="W12" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="Y12" s="2" t="s">
-        <v>57</v>
-      </c>
+      <c r="X12" s="2">
+        <v>798</v>
+      </c>
+      <c r="Y12" s="224"/>
       <c r="Z12" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="AA12" s="2"/>
-      <c r="AB12" s="120">
+      <c r="AA12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB12" s="2"/>
+      <c r="AC12" s="120">
         <f>(250/7)*3</f>
         <v>107.14285714285714</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="130" t="s">
         <v>29</v>
       </c>
       <c r="B13" s="139">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>54</v>
       </c>
       <c r="C13" s="88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
       <c r="D13" s="92">
-        <f t="shared" si="5"/>
-        <v>25.5</v>
+        <f t="shared" si="6"/>
+        <v>12.75</v>
       </c>
       <c r="E13" s="26">
-        <f t="shared" si="6"/>
-        <v>2</v>
+        <f t="shared" si="7"/>
+        <v>1</v>
       </c>
       <c r="F13" s="85">
         <v>27</v>
       </c>
-      <c r="G13" s="204">
-        <v>84.422222222222231</v>
+      <c r="G13" s="225">
+        <f t="shared" si="8"/>
+        <v>63</v>
       </c>
       <c r="H13" s="156">
-        <f t="shared" ref="H13:H21" si="8">$V$40*V13</f>
-        <v>18</v>
+        <f t="shared" ref="H13:H21" si="10">$V$40*V13</f>
+        <v>9</v>
       </c>
       <c r="I13" s="149">
         <f>W13</f>
@@ -3661,7 +3732,7 @@
       </c>
       <c r="J13" s="97">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K13" s="147">
         <v>41</v>
@@ -3673,11 +3744,11 @@
         <v>8</v>
       </c>
       <c r="N13" s="122">
-        <f>SUM(B13:M13)+SUM(Y13:AA13)</f>
-        <v>301.92222222222222</v>
+        <f>SUM(B13:M13)+SUM(Z13:AB13)</f>
+        <v>256.75</v>
       </c>
       <c r="O13" s="166">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>300</v>
       </c>
       <c r="P13" s="124">
@@ -3685,7 +3756,7 @@
       </c>
       <c r="Q13" s="128">
         <f>N13/O13</f>
-        <v>1.0064074074074074</v>
+        <v>0.85583333333333333</v>
       </c>
       <c r="R13" s="2">
         <v>27</v>
@@ -3705,55 +3776,60 @@
       <c r="W13" s="62">
         <v>1</v>
       </c>
-      <c r="Y13" s="2" t="s">
-        <v>57</v>
-      </c>
+      <c r="X13" s="62">
+        <v>63</v>
+      </c>
+      <c r="Y13" s="224"/>
       <c r="Z13" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="AA13" s="2">
+      <c r="AA13" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB13" s="2">
         <v>1</v>
       </c>
-      <c r="AB13" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AC13" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="130" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="139">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="C14" s="88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D14" s="92">
-        <f t="shared" si="5"/>
-        <v>12</v>
+        <f t="shared" si="6"/>
+        <v>6</v>
       </c>
       <c r="E14" s="26">
-        <f t="shared" si="6"/>
-        <v>2</v>
+        <f t="shared" si="7"/>
+        <v>1</v>
       </c>
       <c r="F14" s="85">
         <v>3</v>
       </c>
-      <c r="G14" s="204">
-        <v>16.444444444444446</v>
+      <c r="G14" s="225">
+        <f t="shared" si="8"/>
+        <v>14</v>
       </c>
       <c r="H14" s="156">
-        <f t="shared" si="8"/>
-        <v>4</v>
+        <f t="shared" si="10"/>
+        <v>2</v>
       </c>
       <c r="I14" s="149" t="s">
         <v>57</v>
       </c>
       <c r="J14" s="97">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K14" s="147">
         <v>1</v>
@@ -3765,11 +3841,11 @@
         <v>0</v>
       </c>
       <c r="N14" s="61">
-        <f>SUM(B14:M14)+SUM(Y14:Z14)</f>
-        <v>47.444444444444443</v>
+        <f>SUM(B14:M14)+SUM(Z14:AA14)</f>
+        <v>35</v>
       </c>
       <c r="O14" s="165">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>25</v>
       </c>
       <c r="P14" s="15">
@@ -3794,48 +3870,53 @@
       <c r="W14" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="Y14" s="2" t="s">
-        <v>57</v>
-      </c>
+      <c r="X14" s="2">
+        <v>14</v>
+      </c>
+      <c r="Y14" s="224"/>
       <c r="Z14" s="2" t="s">
         <v>57</v>
       </c>
       <c r="AA14" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB14" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="AB14" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AC14" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="130" t="s">
         <v>31</v>
       </c>
       <c r="B15" s="139">
-        <f t="shared" si="3"/>
-        <v>18</v>
-      </c>
-      <c r="C15" s="88">
         <f t="shared" si="4"/>
         <v>18</v>
       </c>
+      <c r="C15" s="88">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
       <c r="D15" s="92">
-        <f t="shared" si="5"/>
-        <v>4.5</v>
+        <f t="shared" si="6"/>
+        <v>2.25</v>
       </c>
       <c r="E15" s="26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F15" s="85">
         <v>14</v>
       </c>
-      <c r="G15" s="204">
-        <v>49.116666666666667</v>
+      <c r="G15" s="225">
+        <f t="shared" si="8"/>
+        <v>35</v>
       </c>
       <c r="H15" s="156">
-        <f t="shared" si="8"/>
-        <v>4</v>
+        <f t="shared" si="10"/>
+        <v>2</v>
       </c>
       <c r="I15" s="149" t="s">
         <v>57</v>
@@ -3854,11 +3935,11 @@
         <v>6</v>
       </c>
       <c r="N15" s="125">
-        <f>SUM(B15:M15)+SUM(Y15:Z15)</f>
-        <v>118.61666666666667</v>
+        <f>SUM(B15:M15)+SUM(Z15:AA15)</f>
+        <v>100.25</v>
       </c>
       <c r="O15" s="165" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-</v>
       </c>
       <c r="P15" s="126" t="s">
@@ -3883,9 +3964,10 @@
       <c r="W15" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="Y15" s="2" t="s">
-        <v>57</v>
-      </c>
+      <c r="X15" s="62">
+        <v>35</v>
+      </c>
+      <c r="Y15" s="224"/>
       <c r="Z15" s="2" t="s">
         <v>57</v>
       </c>
@@ -3895,43 +3977,47 @@
       <c r="AB15" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AC15" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="130" t="s">
         <v>32</v>
       </c>
       <c r="B16" s="139">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="C16" s="88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="D16" s="92">
-        <f t="shared" si="5"/>
-        <v>37.5</v>
+        <f t="shared" si="6"/>
+        <v>18.75</v>
       </c>
       <c r="E16" s="26">
-        <f t="shared" si="6"/>
-        <v>2</v>
+        <f t="shared" si="7"/>
+        <v>1</v>
       </c>
       <c r="F16" s="85">
         <v>1</v>
       </c>
-      <c r="G16" s="204">
-        <v>3.9944444444444449</v>
+      <c r="G16" s="225">
+        <f t="shared" si="8"/>
+        <v>9</v>
       </c>
       <c r="H16" s="156">
-        <f t="shared" si="8"/>
-        <v>32</v>
+        <f t="shared" si="10"/>
+        <v>16</v>
       </c>
       <c r="I16" s="149" t="s">
         <v>57</v>
       </c>
       <c r="J16" s="97">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K16" s="147">
         <v>12</v>
@@ -3943,8 +4029,8 @@
         <v>12</v>
       </c>
       <c r="N16" s="122">
-        <f>SUM(B16:M16)+SUM(Y16:Z16)</f>
-        <v>122.49444444444444</v>
+        <f>SUM(B16:M16)+SUM(Z16:AA16)</f>
+        <v>90.75</v>
       </c>
       <c r="O16" s="166">
         <v>150</v>
@@ -3954,7 +4040,7 @@
       </c>
       <c r="Q16" s="128">
         <f>N16/O16</f>
-        <v>0.81662962962962959</v>
+        <v>0.60499999999999998</v>
       </c>
       <c r="R16" s="2">
         <v>2</v>
@@ -3974,9 +4060,10 @@
       <c r="W16" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="Y16" s="2" t="s">
-        <v>57</v>
-      </c>
+      <c r="X16" s="2">
+        <v>9</v>
+      </c>
+      <c r="Y16" s="224"/>
       <c r="Z16" s="2" t="s">
         <v>57</v>
       </c>
@@ -3986,32 +4073,37 @@
       <c r="AB16" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC16" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" s="130"/>
-      <c r="B17" s="220"/>
-      <c r="C17" s="221"/>
-      <c r="D17" s="217"/>
-      <c r="E17" s="218"/>
-      <c r="F17" s="219"/>
-      <c r="G17" s="204"/>
-      <c r="H17" s="222"/>
-      <c r="I17" s="223"/>
-      <c r="J17" s="224"/>
-      <c r="K17" s="211"/>
-      <c r="L17" s="212"/>
-      <c r="M17" s="213"/>
-      <c r="N17" s="214"/>
-      <c r="O17" s="215"/>
-      <c r="P17" s="216"/>
+      <c r="B17" s="209"/>
+      <c r="C17" s="210"/>
+      <c r="D17" s="206"/>
+      <c r="E17" s="207"/>
+      <c r="F17" s="208"/>
+      <c r="G17" s="225">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="H17" s="211"/>
+      <c r="I17" s="212"/>
+      <c r="J17" s="213"/>
+      <c r="K17" s="192"/>
+      <c r="L17" s="193"/>
+      <c r="M17" s="194"/>
+      <c r="N17" s="195"/>
+      <c r="O17" s="196"/>
+      <c r="P17" s="197"/>
       <c r="Q17" s="128"/>
       <c r="R17" s="2"/>
       <c r="S17" s="119"/>
       <c r="T17" s="2"/>
       <c r="W17" s="62"/>
-      <c r="Y17" s="2" t="s">
-        <v>57</v>
-      </c>
+      <c r="X17" s="62"/>
+      <c r="Y17" s="224"/>
       <c r="Z17" s="2" t="s">
         <v>57</v>
       </c>
@@ -4021,43 +4113,47 @@
       <c r="AB17" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC17" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" s="130" t="s">
         <v>33</v>
       </c>
       <c r="B18" s="139">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="C18" s="88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>13.5</v>
       </c>
       <c r="D18" s="92">
-        <f t="shared" si="5"/>
-        <v>30</v>
+        <f t="shared" si="6"/>
+        <v>15</v>
       </c>
       <c r="E18" s="26">
-        <f t="shared" si="6"/>
-        <v>20</v>
+        <f t="shared" si="7"/>
+        <v>10</v>
       </c>
       <c r="F18" s="85">
         <v>2</v>
       </c>
-      <c r="G18" s="204">
-        <v>55.555555555555557</v>
+      <c r="G18" s="225">
+        <f t="shared" si="8"/>
+        <v>91</v>
       </c>
       <c r="H18" s="156">
-        <f t="shared" si="8"/>
-        <v>30</v>
+        <f t="shared" si="10"/>
+        <v>15</v>
       </c>
       <c r="I18" s="149" t="s">
         <v>57</v>
       </c>
       <c r="J18" s="97">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="K18" s="147">
         <v>4</v>
@@ -4069,11 +4165,11 @@
         <v>0</v>
       </c>
       <c r="N18" s="61">
-        <f>SUM(B18:M18)+Y18</f>
-        <v>267.05555555555554</v>
+        <f t="shared" ref="N18:N28" si="11">SUM(B18:M18)+Z18</f>
+        <v>252.5</v>
       </c>
       <c r="O18" s="165">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>100</v>
       </c>
       <c r="P18" s="8">
@@ -4098,48 +4194,53 @@
       <c r="W18" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="Y18" s="2">
+      <c r="X18" s="2">
+        <v>91</v>
+      </c>
+      <c r="Y18" s="224"/>
+      <c r="Z18" s="2">
         <v>70</v>
       </c>
-      <c r="Z18" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="AA18" s="2" t="s">
         <v>57</v>
       </c>
       <c r="AB18" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC18" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" s="130" t="s">
         <v>34</v>
       </c>
       <c r="B19" s="139">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
       <c r="C19" s="88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.5</v>
       </c>
       <c r="D19" s="92">
-        <f t="shared" si="5"/>
-        <v>90</v>
+        <f t="shared" si="6"/>
+        <v>45</v>
       </c>
       <c r="E19" s="26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F19" s="85">
         <v>17</v>
       </c>
-      <c r="G19" s="204">
-        <v>38.888888888888893</v>
+      <c r="G19" s="225">
+        <f t="shared" si="8"/>
+        <v>93</v>
       </c>
       <c r="H19" s="156">
-        <f t="shared" si="8"/>
-        <v>30</v>
+        <f t="shared" si="10"/>
+        <v>15</v>
       </c>
       <c r="I19" s="149" t="s">
         <v>57</v>
@@ -4158,11 +4259,11 @@
         <v>0</v>
       </c>
       <c r="N19" s="61">
-        <f>SUM(B19:M19)+Y19</f>
-        <v>349.38888888888891</v>
+        <f t="shared" si="11"/>
+        <v>343.5</v>
       </c>
       <c r="O19" s="165">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>100</v>
       </c>
       <c r="P19" s="8">
@@ -4186,11 +4287,12 @@
       <c r="W19" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="Y19" s="2">
-        <v>100</v>
-      </c>
-      <c r="Z19" s="2" t="s">
-        <v>57</v>
+      <c r="X19" s="62">
+        <v>93</v>
+      </c>
+      <c r="Y19" s="224"/>
+      <c r="Z19" s="2">
+        <v>100</v>
       </c>
       <c r="AA19" s="2" t="s">
         <v>57</v>
@@ -4198,43 +4300,47 @@
       <c r="AB19" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC19" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" s="130" t="s">
         <v>35</v>
       </c>
       <c r="B20" s="139">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C20" s="88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>43.5</v>
       </c>
       <c r="D20" s="92">
-        <f t="shared" si="5"/>
-        <v>75</v>
+        <f t="shared" si="6"/>
+        <v>37.5</v>
       </c>
       <c r="E20" s="26">
-        <f t="shared" si="6"/>
-        <v>90</v>
+        <f t="shared" si="7"/>
+        <v>45</v>
       </c>
       <c r="F20" s="85">
         <v>1</v>
       </c>
-      <c r="G20" s="204">
-        <v>9.4444444444444446</v>
+      <c r="G20" s="225">
+        <f t="shared" si="8"/>
+        <v>79</v>
       </c>
       <c r="H20" s="156">
-        <f t="shared" si="8"/>
-        <v>50</v>
+        <f t="shared" si="10"/>
+        <v>25</v>
       </c>
       <c r="I20" s="149" t="s">
         <v>57</v>
       </c>
       <c r="J20" s="97">
         <f t="shared" si="2"/>
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="K20" s="147">
         <v>20</v>
@@ -4246,11 +4352,11 @@
         <v>15</v>
       </c>
       <c r="N20" s="61">
-        <f>SUM(B20:M20)+Y20</f>
-        <v>417.94444444444446</v>
+        <f t="shared" si="11"/>
+        <v>335</v>
       </c>
       <c r="O20" s="165">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>100</v>
       </c>
       <c r="P20" s="8">
@@ -4274,55 +4380,60 @@
       <c r="W20" s="107" t="s">
         <v>57</v>
       </c>
-      <c r="Y20" s="2">
+      <c r="X20" s="107" t="s">
+        <v>149</v>
+      </c>
+      <c r="Y20" s="224"/>
+      <c r="Z20" s="2">
         <v>20</v>
       </c>
-      <c r="Z20" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="AA20" s="2" t="s">
         <v>57</v>
       </c>
       <c r="AB20" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC20" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" s="130" t="s">
         <v>36</v>
       </c>
       <c r="B21" s="139">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>90</v>
       </c>
       <c r="C21" s="88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D21" s="92">
-        <f t="shared" si="5"/>
-        <v>30</v>
+        <f t="shared" si="6"/>
+        <v>15</v>
       </c>
       <c r="E21" s="26">
-        <f t="shared" si="6"/>
-        <v>4</v>
+        <f t="shared" si="7"/>
+        <v>2</v>
       </c>
       <c r="F21" s="85">
         <v>2</v>
       </c>
-      <c r="G21" s="204">
-        <v>7.7777777777777786</v>
+      <c r="G21" s="225">
+        <f t="shared" si="8"/>
+        <v>35</v>
       </c>
       <c r="H21" s="156">
-        <f t="shared" si="8"/>
-        <v>30</v>
+        <f t="shared" si="10"/>
+        <v>15</v>
       </c>
       <c r="I21" s="149" t="s">
         <v>57</v>
       </c>
       <c r="J21" s="97">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K21" s="147">
         <v>10</v>
@@ -4334,11 +4445,11 @@
         <v>0</v>
       </c>
       <c r="N21" s="61">
-        <f>SUM(B21:M21)+Y21</f>
-        <v>283.77777777777777</v>
+        <f t="shared" si="11"/>
+        <v>277</v>
       </c>
       <c r="O21" s="165">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>100</v>
       </c>
       <c r="P21" s="8">
@@ -4362,11 +4473,12 @@
       <c r="W21" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="Y21" s="2">
-        <v>100</v>
-      </c>
-      <c r="Z21" s="2" t="s">
-        <v>57</v>
+      <c r="X21" s="2">
+        <v>35</v>
+      </c>
+      <c r="Y21" s="224"/>
+      <c r="Z21" s="2">
+        <v>100</v>
       </c>
       <c r="AA21" s="2" t="s">
         <v>57</v>
@@ -4374,31 +4486,35 @@
       <c r="AB21" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC21" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" s="130" t="s">
         <v>37</v>
       </c>
       <c r="B22" s="139">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="C22" s="88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>39</v>
       </c>
       <c r="D22" s="92">
         <v>0</v>
       </c>
       <c r="E22" s="26">
-        <f t="shared" si="6"/>
-        <v>50</v>
+        <f t="shared" si="7"/>
+        <v>25</v>
       </c>
       <c r="F22" s="85">
         <v>0</v>
       </c>
-      <c r="G22" s="204" t="s">
-        <v>57</v>
+      <c r="G22" s="225">
+        <f t="shared" si="8"/>
+        <v>110</v>
       </c>
       <c r="H22" s="156" t="s">
         <v>57</v>
@@ -4408,7 +4524,7 @@
       </c>
       <c r="J22" s="97">
         <f t="shared" si="2"/>
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="K22" s="147">
         <v>0</v>
@@ -4420,11 +4536,11 @@
         <v>0</v>
       </c>
       <c r="N22" s="61">
-        <f>SUM(B22:M22)+Y22</f>
-        <v>409</v>
+        <f t="shared" si="11"/>
+        <v>469</v>
       </c>
       <c r="O22" s="165">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>100</v>
       </c>
       <c r="P22" s="8">
@@ -4448,20 +4564,24 @@
       <c r="W22" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="Y22" s="2">
+      <c r="X22" s="2">
+        <v>110</v>
+      </c>
+      <c r="Y22" s="224"/>
+      <c r="Z22" s="2">
         <v>250</v>
       </c>
-      <c r="Z22" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="AA22" s="2" t="s">
         <v>57</v>
       </c>
       <c r="AB22" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC22" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" s="130" t="s">
         <v>38</v>
       </c>
@@ -4469,22 +4589,23 @@
         <v>0</v>
       </c>
       <c r="C23" s="88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="D23" s="92">
-        <f t="shared" si="5"/>
-        <v>30</v>
+        <f t="shared" si="6"/>
+        <v>15</v>
       </c>
       <c r="E23" s="26">
-        <f t="shared" si="6"/>
-        <v>40</v>
+        <f t="shared" si="7"/>
+        <v>20</v>
       </c>
       <c r="F23" s="85">
         <v>0</v>
       </c>
-      <c r="G23" s="204">
-        <v>6.1111111111111116</v>
+      <c r="G23" s="225">
+        <f t="shared" si="8"/>
+        <v>129</v>
       </c>
       <c r="H23" s="156" t="s">
         <v>57</v>
@@ -4494,7 +4615,7 @@
       </c>
       <c r="J23" s="97">
         <f t="shared" si="2"/>
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="K23" s="147">
         <v>0</v>
@@ -4506,11 +4627,11 @@
         <v>0</v>
       </c>
       <c r="N23" s="61">
-        <f>SUM(B23:M23)+Y23</f>
-        <v>216.11111111111111</v>
+        <f t="shared" si="11"/>
+        <v>284</v>
       </c>
       <c r="O23" s="165">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>100</v>
       </c>
       <c r="P23" s="8">
@@ -4534,11 +4655,12 @@
       <c r="W23" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="Y23" s="2">
-        <v>100</v>
-      </c>
-      <c r="Z23" s="2" t="s">
-        <v>57</v>
+      <c r="X23" s="2">
+        <v>129</v>
+      </c>
+      <c r="Y23" s="224"/>
+      <c r="Z23" s="2">
+        <v>100</v>
       </c>
       <c r="AA23" s="2" t="s">
         <v>57</v>
@@ -4546,8 +4668,11 @@
       <c r="AB23" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC23" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24" s="130" t="s">
         <v>39</v>
       </c>
@@ -4555,7 +4680,7 @@
         <v>0</v>
       </c>
       <c r="C24" s="88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.5</v>
       </c>
       <c r="D24" s="92">
@@ -4567,8 +4692,9 @@
       <c r="F24" s="85">
         <v>0</v>
       </c>
-      <c r="G24" s="204">
-        <v>55.555555555555557</v>
+      <c r="G24" s="225">
+        <f t="shared" si="8"/>
+        <v>19</v>
       </c>
       <c r="H24" s="156" t="s">
         <v>57</v>
@@ -4589,11 +4715,11 @@
         <v>0</v>
       </c>
       <c r="N24" s="61">
-        <f>SUM(B24:M24)+Y24</f>
-        <v>88.055555555555557</v>
+        <f t="shared" si="11"/>
+        <v>51.5</v>
       </c>
       <c r="O24" s="172">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>100</v>
       </c>
       <c r="P24" s="15">
@@ -4617,34 +4743,38 @@
       <c r="W24" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="Y24" s="2">
+      <c r="X24" s="62">
+        <v>19</v>
+      </c>
+      <c r="Y24" s="224"/>
+      <c r="Z24" s="2">
         <v>31</v>
       </c>
-      <c r="Z24" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="AA24" s="2" t="s">
         <v>57</v>
       </c>
       <c r="AB24" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC24" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" s="130" t="s">
         <v>40</v>
       </c>
       <c r="B25" s="139">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
       <c r="C25" s="88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="D25" s="92">
-        <f t="shared" si="5"/>
-        <v>30</v>
+        <f t="shared" si="6"/>
+        <v>15</v>
       </c>
       <c r="E25" s="26">
         <v>0</v>
@@ -4652,8 +4782,9 @@
       <c r="F25" s="85">
         <v>1</v>
       </c>
-      <c r="G25" s="204">
-        <v>16.111111111111111</v>
+      <c r="G25" s="225">
+        <f t="shared" si="8"/>
+        <v>74</v>
       </c>
       <c r="H25" s="156" t="s">
         <v>57</v>
@@ -4674,11 +4805,11 @@
         <v>0</v>
       </c>
       <c r="N25" s="61">
-        <f>SUM(B25:M25)+Y25</f>
-        <v>226.11111111111111</v>
+        <f t="shared" si="11"/>
+        <v>269</v>
       </c>
       <c r="O25" s="165">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>100</v>
       </c>
       <c r="P25" s="8">
@@ -4702,11 +4833,12 @@
       <c r="W25" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="Y25" s="2">
-        <v>100</v>
-      </c>
-      <c r="Z25" s="2" t="s">
-        <v>57</v>
+      <c r="X25" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y25" s="224"/>
+      <c r="Z25" s="2">
+        <v>100</v>
       </c>
       <c r="AA25" s="2" t="s">
         <v>57</v>
@@ -4714,32 +4846,36 @@
       <c r="AB25" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC25" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26" s="130" t="s">
         <v>41</v>
       </c>
       <c r="B26" s="139">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
       <c r="C26" s="88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>40.5</v>
       </c>
       <c r="D26" s="92">
-        <f t="shared" si="5"/>
-        <v>30</v>
+        <f t="shared" si="6"/>
+        <v>15</v>
       </c>
       <c r="E26" s="26">
-        <f t="shared" si="6"/>
-        <v>8</v>
+        <f t="shared" si="7"/>
+        <v>4</v>
       </c>
       <c r="F26" s="85">
         <v>0</v>
       </c>
-      <c r="G26" s="204">
-        <v>15</v>
+      <c r="G26" s="225">
+        <f t="shared" si="8"/>
+        <v>75</v>
       </c>
       <c r="H26" s="156" t="s">
         <v>57</v>
@@ -4749,7 +4885,7 @@
       </c>
       <c r="J26" s="97">
         <f>$U$40*U26</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K26" s="147">
         <v>0</v>
@@ -4761,11 +4897,11 @@
         <v>0</v>
       </c>
       <c r="N26" s="61">
-        <f>SUM(B26:M26)+Y26</f>
-        <v>271.5</v>
+        <f t="shared" si="11"/>
+        <v>308.5</v>
       </c>
       <c r="O26" s="165">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>100</v>
       </c>
       <c r="P26" s="8">
@@ -4789,11 +4925,12 @@
       <c r="W26" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="Y26" s="2">
-        <v>100</v>
-      </c>
-      <c r="Z26" s="2" t="s">
-        <v>57</v>
+      <c r="X26" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y26" s="224"/>
+      <c r="Z26" s="2">
+        <v>100</v>
       </c>
       <c r="AA26" s="2" t="s">
         <v>57</v>
@@ -4801,22 +4938,25 @@
       <c r="AB26" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC26" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A27" s="130" t="s">
         <v>42</v>
       </c>
       <c r="B27" s="139">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
       <c r="C27" s="88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.5</v>
       </c>
       <c r="D27" s="92">
-        <f t="shared" si="5"/>
-        <v>30</v>
+        <f t="shared" si="6"/>
+        <v>15</v>
       </c>
       <c r="E27" s="26" t="s">
         <v>57</v>
@@ -4824,10 +4964,11 @@
       <c r="F27" s="85">
         <v>0</v>
       </c>
-      <c r="G27" s="204">
-        <v>12.777777777777779</v>
-      </c>
-      <c r="H27" s="207" t="s">
+      <c r="G27" s="225">
+        <f t="shared" si="8"/>
+        <v>27</v>
+      </c>
+      <c r="H27" s="188" t="s">
         <v>57</v>
       </c>
       <c r="I27" s="149" t="s">
@@ -4846,11 +4987,11 @@
         <v>0</v>
       </c>
       <c r="N27" s="61">
-        <f>SUM(B27:M27)+Y27</f>
-        <v>214.27777777777777</v>
+        <f t="shared" si="11"/>
+        <v>213.5</v>
       </c>
       <c r="O27" s="165">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>100</v>
       </c>
       <c r="P27" s="8">
@@ -4874,11 +5015,12 @@
       <c r="W27" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="Y27" s="2">
-        <v>100</v>
-      </c>
-      <c r="Z27" s="2" t="s">
-        <v>57</v>
+      <c r="X27" s="2">
+        <v>27</v>
+      </c>
+      <c r="Y27" s="224"/>
+      <c r="Z27" s="2">
+        <v>100</v>
       </c>
       <c r="AA27" s="2" t="s">
         <v>57</v>
@@ -4886,22 +5028,25 @@
       <c r="AB27" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC27" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28" s="130" t="s">
         <v>43</v>
       </c>
       <c r="B28" s="139">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
       <c r="C28" s="88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7.5</v>
       </c>
       <c r="D28" s="92">
-        <f t="shared" si="5"/>
-        <v>30</v>
+        <f t="shared" si="6"/>
+        <v>15</v>
       </c>
       <c r="E28" s="26" t="s">
         <v>57</v>
@@ -4909,8 +5054,9 @@
       <c r="F28" s="85">
         <v>0</v>
       </c>
-      <c r="G28" s="204">
-        <v>25</v>
+      <c r="G28" s="225">
+        <f t="shared" si="8"/>
+        <v>106</v>
       </c>
       <c r="H28" s="156" t="s">
         <v>57</v>
@@ -4931,11 +5077,11 @@
         <v>0</v>
       </c>
       <c r="N28" s="61">
-        <f>SUM(B28:M28)+Y28</f>
-        <v>232.5</v>
+        <f t="shared" si="11"/>
+        <v>298.5</v>
       </c>
       <c r="O28" s="165">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>100</v>
       </c>
       <c r="P28" s="8">
@@ -4959,11 +5105,12 @@
       <c r="W28" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="Y28" s="2">
-        <v>100</v>
-      </c>
-      <c r="Z28" s="2" t="s">
-        <v>57</v>
+      <c r="X28" s="2">
+        <v>106</v>
+      </c>
+      <c r="Y28" s="224"/>
+      <c r="Z28" s="2">
+        <v>100</v>
       </c>
       <c r="AA28" s="2" t="s">
         <v>57</v>
@@ -4971,8 +5118,11 @@
       <c r="AB28" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC28" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A29" s="130" t="s">
         <v>44</v>
       </c>
@@ -4980,12 +5130,12 @@
         <v>0</v>
       </c>
       <c r="C29" s="88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.5</v>
       </c>
       <c r="D29" s="92">
-        <f t="shared" si="5"/>
-        <v>30</v>
+        <f t="shared" si="6"/>
+        <v>15</v>
       </c>
       <c r="E29" s="26" t="s">
         <v>57</v>
@@ -4993,8 +5143,9 @@
       <c r="F29" s="85">
         <v>0</v>
       </c>
-      <c r="G29" s="204">
-        <v>12.222222222222223</v>
+      <c r="G29" s="225">
+        <f t="shared" si="8"/>
+        <v>33</v>
       </c>
       <c r="H29" s="156" t="s">
         <v>57</v>
@@ -5016,10 +5167,10 @@
       </c>
       <c r="N29" s="121">
         <f>SUM(B29:M29)</f>
-        <v>46.722222222222221</v>
+        <v>52.5</v>
       </c>
       <c r="O29" s="21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>100</v>
       </c>
       <c r="P29" s="94">
@@ -5043,9 +5194,10 @@
       <c r="W29" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="Y29" s="2" t="s">
-        <v>57</v>
-      </c>
+      <c r="X29" s="62">
+        <v>33</v>
+      </c>
+      <c r="Y29" s="224"/>
       <c r="Z29" s="2" t="s">
         <v>57</v>
       </c>
@@ -5055,22 +5207,25 @@
       <c r="AB29" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC29" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30" s="130" t="s">
         <v>47</v>
       </c>
       <c r="B30" s="139">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
       <c r="C30" s="88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>28.5</v>
       </c>
       <c r="D30" s="92">
-        <f t="shared" si="5"/>
-        <v>30</v>
+        <f t="shared" si="6"/>
+        <v>15</v>
       </c>
       <c r="E30" s="26" t="s">
         <v>57</v>
@@ -5078,8 +5233,9 @@
       <c r="F30" s="85">
         <v>0</v>
       </c>
-      <c r="G30" s="204" t="s">
-        <v>57</v>
+      <c r="G30" s="225">
+        <f t="shared" si="8"/>
+        <v>125</v>
       </c>
       <c r="H30" s="156" t="s">
         <v>57</v>
@@ -5100,11 +5256,11 @@
         <v>0</v>
       </c>
       <c r="N30" s="61">
-        <f>SUM(B30:M30)+Y30</f>
-        <v>228.5</v>
+        <f>SUM(B30:M30)+Z30</f>
+        <v>338.5</v>
       </c>
       <c r="O30" s="165">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>100</v>
       </c>
       <c r="P30" s="8">
@@ -5128,11 +5284,12 @@
       <c r="W30" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="Y30" s="2">
-        <v>100</v>
-      </c>
-      <c r="Z30" s="2" t="s">
-        <v>57</v>
+      <c r="X30" s="2">
+        <v>125</v>
+      </c>
+      <c r="Y30" s="224"/>
+      <c r="Z30" s="2">
+        <v>100</v>
       </c>
       <c r="AA30" s="2" t="s">
         <v>57</v>
@@ -5140,8 +5297,11 @@
       <c r="AB30" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC30" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A31" s="130" t="s">
         <v>45</v>
       </c>
@@ -5152,42 +5312,42 @@
         <v>0</v>
       </c>
       <c r="D31" s="92">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+      <c r="E31" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="F31" s="85">
+        <v>0</v>
+      </c>
+      <c r="G31" s="225" t="s">
+        <v>57</v>
+      </c>
+      <c r="H31" s="156" t="s">
+        <v>57</v>
+      </c>
+      <c r="I31" s="149" t="s">
+        <v>57</v>
+      </c>
+      <c r="J31" s="97" t="s">
+        <v>57</v>
+      </c>
+      <c r="K31" s="147">
+        <v>0</v>
+      </c>
+      <c r="L31" s="108">
+        <v>0</v>
+      </c>
+      <c r="M31" s="160">
+        <v>0</v>
+      </c>
+      <c r="N31" s="121">
+        <f>20+Z31</f>
         <v>30</v>
       </c>
-      <c r="E31" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="F31" s="85">
-        <v>0</v>
-      </c>
-      <c r="G31" s="204" t="s">
-        <v>57</v>
-      </c>
-      <c r="H31" s="156" t="s">
-        <v>57</v>
-      </c>
-      <c r="I31" s="149" t="s">
-        <v>57</v>
-      </c>
-      <c r="J31" s="97" t="s">
-        <v>57</v>
-      </c>
-      <c r="K31" s="147">
-        <v>0</v>
-      </c>
-      <c r="L31" s="108">
-        <v>0</v>
-      </c>
-      <c r="M31" s="160">
-        <v>0</v>
-      </c>
-      <c r="N31" s="121">
-        <f>20+Y31</f>
-        <v>30</v>
-      </c>
       <c r="O31" s="21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>100</v>
       </c>
       <c r="P31" s="94">
@@ -5211,20 +5371,24 @@
       <c r="W31" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="Y31" s="2">
+      <c r="X31" s="62" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y31" s="224"/>
+      <c r="Z31" s="2">
         <v>10</v>
       </c>
-      <c r="Z31" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="AA31" s="2" t="s">
         <v>57</v>
       </c>
       <c r="AB31" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC31" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A32" s="130" t="s">
         <v>46</v>
       </c>
@@ -5232,12 +5396,12 @@
         <v>0</v>
       </c>
       <c r="C32" s="88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>13.5</v>
       </c>
       <c r="D32" s="92">
-        <f t="shared" si="5"/>
-        <v>30</v>
+        <f t="shared" si="6"/>
+        <v>15</v>
       </c>
       <c r="E32" s="26" t="s">
         <v>57</v>
@@ -5245,8 +5409,9 @@
       <c r="F32" s="85">
         <v>0</v>
       </c>
-      <c r="G32" s="204" t="s">
-        <v>57</v>
+      <c r="G32" s="225">
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="H32" s="156" t="s">
         <v>57</v>
@@ -5267,11 +5432,11 @@
         <v>0</v>
       </c>
       <c r="N32" s="61">
-        <f>SUM(B32:M32)+Y32</f>
-        <v>143.5</v>
+        <f>SUM(B32:M32)+Z32</f>
+        <v>128.5</v>
       </c>
       <c r="O32" s="165">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>100</v>
       </c>
       <c r="P32" s="8">
@@ -5295,11 +5460,12 @@
       <c r="W32" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="Y32" s="2">
-        <v>100</v>
-      </c>
-      <c r="Z32" s="2" t="s">
-        <v>57</v>
+      <c r="X32" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y32" s="224"/>
+      <c r="Z32" s="2">
+        <v>100</v>
       </c>
       <c r="AA32" s="2" t="s">
         <v>57</v>
@@ -5307,8 +5473,11 @@
       <c r="AB32" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC32" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A33" s="130" t="s">
         <v>48</v>
       </c>
@@ -5316,12 +5485,12 @@
         <v>0</v>
       </c>
       <c r="C33" s="88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>34.5</v>
       </c>
       <c r="D33" s="92">
-        <f t="shared" si="5"/>
-        <v>30</v>
+        <f t="shared" si="6"/>
+        <v>15</v>
       </c>
       <c r="E33" s="26" t="s">
         <v>57</v>
@@ -5329,8 +5498,9 @@
       <c r="F33" s="85">
         <v>0</v>
       </c>
-      <c r="G33" s="204">
-        <v>12.777777777777779</v>
+      <c r="G33" s="225">
+        <f t="shared" si="8"/>
+        <v>12</v>
       </c>
       <c r="H33" s="156" t="s">
         <v>57</v>
@@ -5351,11 +5521,11 @@
         <v>0</v>
       </c>
       <c r="N33" s="121">
-        <f>SUM(B33:M33)+Y33</f>
-        <v>79.277777777777771</v>
+        <f>SUM(B33:M33)+Z33</f>
+        <v>63.5</v>
       </c>
       <c r="O33" s="21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>100</v>
       </c>
       <c r="P33" s="94">
@@ -5379,20 +5549,24 @@
       <c r="W33" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="Y33" s="2">
+      <c r="X33" s="62">
+        <v>12</v>
+      </c>
+      <c r="Y33" s="224"/>
+      <c r="Z33" s="2">
         <v>2</v>
       </c>
-      <c r="Z33" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="AA33" s="2" t="s">
         <v>57</v>
       </c>
       <c r="AB33" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC33" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A34" s="130" t="s">
         <v>49</v>
       </c>
@@ -5403,8 +5577,8 @@
         <v>0</v>
       </c>
       <c r="D34" s="92">
-        <f t="shared" si="5"/>
-        <v>60</v>
+        <f t="shared" si="6"/>
+        <v>30</v>
       </c>
       <c r="E34" s="26" t="s">
         <v>57</v>
@@ -5412,7 +5586,7 @@
       <c r="F34" s="85">
         <v>0</v>
       </c>
-      <c r="G34" s="204" t="s">
+      <c r="G34" s="225" t="s">
         <v>57</v>
       </c>
       <c r="H34" s="156" t="s">
@@ -5434,11 +5608,11 @@
         <v>0</v>
       </c>
       <c r="N34" s="61">
-        <f>SUM(B34:M34)+Y34</f>
-        <v>160</v>
+        <f>SUM(B34:M34)+Z34</f>
+        <v>130</v>
       </c>
       <c r="O34" s="165">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>100</v>
       </c>
       <c r="P34" s="8">
@@ -5462,11 +5636,12 @@
       <c r="W34" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="Y34" s="2">
-        <v>100</v>
-      </c>
-      <c r="Z34" s="2" t="s">
-        <v>57</v>
+      <c r="X34" s="62" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y34" s="224"/>
+      <c r="Z34" s="2">
+        <v>100</v>
       </c>
       <c r="AA34" s="2" t="s">
         <v>57</v>
@@ -5474,8 +5649,11 @@
       <c r="AB34" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC34" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A35" s="130" t="s">
         <v>50</v>
       </c>
@@ -5483,22 +5661,23 @@
         <v>0</v>
       </c>
       <c r="C35" s="88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>10.5</v>
       </c>
       <c r="D35" s="92">
-        <f t="shared" si="5"/>
-        <v>30</v>
+        <f t="shared" si="6"/>
+        <v>15</v>
       </c>
       <c r="E35" s="26">
-        <f t="shared" si="6"/>
-        <v>8</v>
+        <f t="shared" si="7"/>
+        <v>4</v>
       </c>
       <c r="F35" s="85">
         <v>0</v>
       </c>
-      <c r="G35" s="204">
-        <v>16.111111111111111</v>
+      <c r="G35" s="225">
+        <f t="shared" si="8"/>
+        <v>18</v>
       </c>
       <c r="H35" s="156" t="s">
         <v>57</v>
@@ -5508,7 +5687,7 @@
       </c>
       <c r="J35" s="97">
         <f>$U$40*U35</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K35" s="147">
         <v>0</v>
@@ -5520,11 +5699,11 @@
         <v>0</v>
       </c>
       <c r="N35" s="61">
-        <f>SUM(B35:M35)+Y35+Z35</f>
-        <v>148.11111111111111</v>
+        <f>SUM(B35:M35)+Z35+AA35</f>
+        <v>127</v>
       </c>
       <c r="O35" s="165">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>100</v>
       </c>
       <c r="P35" s="8">
@@ -5548,21 +5727,25 @@
       <c r="W35" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="Y35" s="2">
+      <c r="X35" s="62">
+        <v>18</v>
+      </c>
+      <c r="Y35" s="224"/>
+      <c r="Z35" s="2">
         <v>13</v>
       </c>
-      <c r="Z35" s="2">
+      <c r="AA35" s="2">
         <f>250/400*100</f>
         <v>62.5</v>
       </c>
-      <c r="AA35" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="AB35" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="36" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AC35" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="131" t="s">
         <v>51</v>
       </c>
@@ -5574,8 +5757,8 @@
         <v>13.5</v>
       </c>
       <c r="D36" s="93">
-        <f t="shared" si="5"/>
-        <v>30</v>
+        <f t="shared" si="6"/>
+        <v>15</v>
       </c>
       <c r="E36" s="27" t="s">
         <v>57</v>
@@ -5583,8 +5766,9 @@
       <c r="F36" s="86">
         <v>0</v>
       </c>
-      <c r="G36" s="205" t="s">
-        <v>57</v>
+      <c r="G36" s="226">
+        <f>X40*X36</f>
+        <v>2</v>
       </c>
       <c r="H36" s="157" t="s">
         <v>57</v>
@@ -5605,11 +5789,11 @@
         <v>0</v>
       </c>
       <c r="N36" s="60">
-        <f>SUM(B36:M36)+Y36</f>
-        <v>122.5</v>
+        <f>SUM(B36:M36)+Z36</f>
+        <v>109.5</v>
       </c>
       <c r="O36" s="170">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>100</v>
       </c>
       <c r="P36" s="9">
@@ -5633,36 +5817,41 @@
       <c r="W36" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="Y36" s="2">
+      <c r="X36" s="62">
+        <v>2</v>
+      </c>
+      <c r="Y36" s="224"/>
+      <c r="Z36" s="2">
         <v>79</v>
       </c>
-      <c r="Z36" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="AA36" s="2" t="s">
         <v>57</v>
       </c>
       <c r="AB36" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="37" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AC36" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
-      <c r="N37" s="190" t="s">
+      <c r="N37" s="203" t="s">
         <v>111</v>
       </c>
-      <c r="O37" s="191"/>
-      <c r="P37" s="192"/>
+      <c r="O37" s="204"/>
+      <c r="P37" s="205"/>
       <c r="R37" s="2"/>
       <c r="S37" s="119"/>
       <c r="T37" s="2"/>
-    </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="Y37" s="223"/>
+    </row>
+    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>110</v>
       </c>
@@ -5681,7 +5870,7 @@
       <c r="S38" s="119"/>
       <c r="T38" s="2"/>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>112</v>
       </c>
@@ -5711,8 +5900,11 @@
       <c r="V39" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="X39" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A40" s="106" t="s">
         <v>112</v>
       </c>
@@ -5731,19 +5923,23 @@
         <v>2</v>
       </c>
       <c r="S40" s="119">
-        <v>1.5</v>
+        <f>1.5/2</f>
+        <v>0.75</v>
       </c>
       <c r="T40" s="2">
         <v>1.5</v>
       </c>
       <c r="U40" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V40" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="X40" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
@@ -5759,7 +5955,7 @@
       </c>
       <c r="U41" s="2"/>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:29" x14ac:dyDescent="0.25">
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
@@ -5773,7 +5969,7 @@
       <c r="T42" s="2"/>
       <c r="U42" s="2"/>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
@@ -5791,8 +5987,11 @@
         <v>63</v>
       </c>
       <c r="U43" s="2"/>
-    </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="X43" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="44" spans="1:29" x14ac:dyDescent="0.25">
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
@@ -5807,10 +6006,18 @@
       <c r="O44" s="2"/>
       <c r="P44" s="2"/>
       <c r="R44" s="2"/>
-      <c r="S44" s="119"/>
+      <c r="S44" s="119" t="s">
+        <v>151</v>
+      </c>
       <c r="T44" s="2"/>
-    </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="V44" s="119" t="s">
+        <v>152</v>
+      </c>
+      <c r="X44" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="45" spans="1:29" x14ac:dyDescent="0.25">
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
@@ -5827,8 +6034,11 @@
       <c r="R45" s="2"/>
       <c r="S45" s="119"/>
       <c r="T45" s="2"/>
-    </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="U45" s="119" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="46" spans="1:29" x14ac:dyDescent="0.25">
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
@@ -5849,7 +6059,7 @@
       <c r="S46" s="119"/>
       <c r="T46" s="2"/>
     </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:29" x14ac:dyDescent="0.25">
       <c r="L47" s="2" t="s">
         <v>137</v>
       </c>
@@ -5857,7 +6067,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:29" x14ac:dyDescent="0.25">
       <c r="L48" s="2" t="s">
         <v>140</v>
       </c>
@@ -6221,7 +6431,7 @@
     <mergeCell ref="H17:J17"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="Y1" r:id="rId1"/>
+    <hyperlink ref="Z1" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId2"/>
@@ -9154,11 +9364,11 @@
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
-      <c r="N37" s="193" t="s">
+      <c r="N37" s="214" t="s">
         <v>111</v>
       </c>
-      <c r="O37" s="194"/>
-      <c r="P37" s="195"/>
+      <c r="O37" s="215"/>
+      <c r="P37" s="216"/>
       <c r="R37" s="2"/>
       <c r="S37" s="119"/>
       <c r="T37" s="2"/>
@@ -12008,10 +12218,10 @@
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
-      <c r="M37" s="193" t="s">
+      <c r="M37" s="214" t="s">
         <v>111</v>
       </c>
-      <c r="N37" s="195"/>
+      <c r="N37" s="216"/>
       <c r="P37" s="2"/>
       <c r="Q37" s="119"/>
       <c r="R37" s="2"/>
@@ -14441,10 +14651,10 @@
       <c r="X36" s="2"/>
     </row>
     <row r="37" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L37" s="196" t="s">
+      <c r="L37" s="217" t="s">
         <v>77</v>
       </c>
-      <c r="M37" s="197"/>
+      <c r="M37" s="218"/>
       <c r="O37" s="2"/>
       <c r="P37" s="2"/>
       <c r="Q37" s="2"/>
@@ -16749,10 +16959,10 @@
     </row>
     <row r="37" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K37" s="62"/>
-      <c r="L37" s="198" t="s">
+      <c r="L37" s="219" t="s">
         <v>77</v>
       </c>
-      <c r="M37" s="197"/>
+      <c r="M37" s="218"/>
       <c r="O37" s="2"/>
       <c r="P37" s="2"/>
       <c r="Q37" s="2"/>
@@ -16870,7 +17080,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="199" t="s">
+      <c r="A2" s="220" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="46" t="s">
@@ -16881,7 +17091,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="201"/>
+      <c r="A3" s="222"/>
       <c r="B3" s="47" t="s">
         <v>4</v>
       </c>
@@ -16890,7 +17100,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="188" t="s">
+      <c r="A4" s="201" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="48" t="s">
@@ -16901,7 +17111,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="189"/>
+      <c r="A5" s="202"/>
       <c r="B5" s="50" t="s">
         <v>9</v>
       </c>
@@ -16910,7 +17120,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="199" t="s">
+      <c r="A6" s="220" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="46" t="s">
@@ -16921,7 +17131,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="200"/>
+      <c r="A7" s="221"/>
       <c r="B7" s="51" t="s">
         <v>13</v>
       </c>
@@ -16930,7 +17140,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="189"/>
+      <c r="A8" s="202"/>
       <c r="B8" s="50" t="s">
         <v>14</v>
       </c>
@@ -16951,7 +17161,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="199" t="s">
+      <c r="A11" s="220" t="s">
         <v>2</v>
       </c>
       <c r="B11" s="46" t="s">
@@ -16962,7 +17172,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="201"/>
+      <c r="A12" s="222"/>
       <c r="B12" s="47" t="s">
         <v>4</v>
       </c>
@@ -16971,7 +17181,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="188" t="s">
+      <c r="A13" s="201" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="48" t="s">
@@ -16982,7 +17192,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="186"/>
+      <c r="A14" s="199"/>
       <c r="B14" s="49" t="s">
         <v>9</v>
       </c>
@@ -16991,7 +17201,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="186"/>
+      <c r="A15" s="199"/>
       <c r="B15" s="49" t="s">
         <v>74</v>
       </c>
@@ -17000,7 +17210,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="189"/>
+      <c r="A16" s="202"/>
       <c r="B16" s="50" t="s">
         <v>80</v>
       </c>
@@ -17009,7 +17219,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="199" t="s">
+      <c r="A17" s="220" t="s">
         <v>11</v>
       </c>
       <c r="B17" s="46" t="s">
@@ -17020,7 +17230,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="200"/>
+      <c r="A18" s="221"/>
       <c r="B18" s="51" t="s">
         <v>13</v>
       </c>
@@ -17029,7 +17239,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="189"/>
+      <c r="A19" s="202"/>
       <c r="B19" s="50" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
(U)    added diet notes to Thrive in-prog plan
</commit_message>
<xml_diff>
--- a/Suppl/nutrition plan.xlsx
+++ b/Suppl/nutrition plan.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="5" r:id="rId1"/>
     <sheet name="Schedule" sheetId="8" r:id="rId2"/>
-    <sheet name="Nutrition r5 - Growth" sheetId="9" r:id="rId3"/>
-    <sheet name="Nutrition r4 - With Juicer" sheetId="7" r:id="rId4"/>
-    <sheet name="Nutrition r3 - Upcoming" sheetId="6" r:id="rId5"/>
-    <sheet name="Nutrition r2 - Present" sheetId="4" r:id="rId6"/>
-    <sheet name="Nutrition r1- Prev" sheetId="3" r:id="rId7"/>
-    <sheet name="Items  - Prev" sheetId="1" r:id="rId8"/>
+    <sheet name="newGrowthStuff" sheetId="10" r:id="rId3"/>
+    <sheet name="Nutrition r5 - Growth" sheetId="9" r:id="rId4"/>
+    <sheet name="Nutrition r4 - With Juicer" sheetId="7" r:id="rId5"/>
+    <sheet name="Nutrition r3 - Upcoming" sheetId="6" r:id="rId6"/>
+    <sheet name="Nutrition r2 - Present" sheetId="4" r:id="rId7"/>
+    <sheet name="Nutrition r1- Prev" sheetId="3" r:id="rId8"/>
+    <sheet name="Items  - Prev" sheetId="1" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1377" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1504" uniqueCount="207">
   <si>
     <t>Meal</t>
   </si>
@@ -539,6 +540,114 @@
   </si>
   <si>
     <t>1 LP</t>
+  </si>
+  <si>
+    <t>Goal Right Now</t>
+  </si>
+  <si>
+    <t>Quick</t>
+  </si>
+  <si>
+    <t>Quick is your orig one more or less</t>
+  </si>
+  <si>
+    <t>Both feat same calorie content</t>
+  </si>
+  <si>
+    <t>Special K Red Berry Cereal</t>
+  </si>
+  <si>
+    <t>Non-fat Milk</t>
+  </si>
+  <si>
+    <t>Total Lean Shake</t>
+  </si>
+  <si>
+    <t>Full</t>
+  </si>
+  <si>
+    <t>Switch to a Full/Quick Mode, Core is real food and Quick is shakes</t>
+  </si>
+  <si>
+    <t>Turkey Sandwich</t>
+  </si>
+  <si>
+    <t>Cooked Chicken</t>
+  </si>
+  <si>
+    <t>Cooked Vegetables</t>
+  </si>
+  <si>
+    <t>Salad w/Dressing</t>
+  </si>
+  <si>
+    <t>Healthy TV Dinner</t>
+  </si>
+  <si>
+    <t>Bread</t>
+  </si>
+  <si>
+    <t>Both Listing</t>
+  </si>
+  <si>
+    <t>Nutrition (all items)</t>
+  </si>
+  <si>
+    <t>NM</t>
+  </si>
+  <si>
+    <t>JCR</t>
+  </si>
+  <si>
+    <t>TLS</t>
+  </si>
+  <si>
+    <t>BAR</t>
+  </si>
+  <si>
+    <t>AM1</t>
+  </si>
+  <si>
+    <t>PS</t>
+  </si>
+  <si>
+    <t>AMN</t>
+  </si>
+  <si>
+    <t>AM2</t>
+  </si>
+  <si>
+    <t>SLD</t>
+  </si>
+  <si>
+    <t>TVD</t>
+  </si>
+  <si>
+    <t>BRD</t>
+  </si>
+  <si>
+    <t>TKS</t>
+  </si>
+  <si>
+    <t>CHPS</t>
+  </si>
+  <si>
+    <t>CKDV</t>
+  </si>
+  <si>
+    <t>CKDC</t>
+  </si>
+  <si>
+    <t>!!!Note</t>
+  </si>
+  <si>
+    <t>1 Cup</t>
+  </si>
+  <si>
+    <t>8 oz.</t>
+  </si>
+  <si>
+    <t>28 oz.</t>
   </si>
 </sst>
 </file>
@@ -1990,94 +2099,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2103,22 +2128,61 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2128,8 +2192,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2498,7 +2607,7 @@
       <c r="C2" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="199" t="s">
+      <c r="E2" s="215" t="s">
         <v>89</v>
       </c>
       <c r="F2" s="72" t="s">
@@ -2516,7 +2625,7 @@
       <c r="C3" s="48" t="s">
         <v>65</v>
       </c>
-      <c r="E3" s="200"/>
+      <c r="E3" s="216"/>
       <c r="F3" s="76" t="s">
         <v>91</v>
       </c>
@@ -2532,7 +2641,7 @@
       <c r="C4" s="46" t="s">
         <v>116</v>
       </c>
-      <c r="E4" s="201"/>
+      <c r="E4" s="217"/>
       <c r="F4" s="74" t="s">
         <v>9</v>
       </c>
@@ -2541,7 +2650,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="202" t="s">
+      <c r="A5" s="218" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="41" t="s">
@@ -2550,7 +2659,7 @@
       <c r="C5" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="E5" s="199" t="s">
+      <c r="E5" s="215" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="75" t="s">
@@ -2561,14 +2670,14 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="200"/>
+      <c r="A6" s="216"/>
       <c r="B6" s="71" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="200"/>
+      <c r="E6" s="216"/>
       <c r="F6" s="73" t="s">
         <v>95</v>
       </c>
@@ -2577,14 +2686,14 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="203"/>
+      <c r="A7" s="219"/>
       <c r="B7" s="43" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="49" t="s">
         <v>99</v>
       </c>
-      <c r="E7" s="201"/>
+      <c r="E7" s="217"/>
       <c r="F7" s="74" t="s">
         <v>82</v>
       </c>
@@ -2606,7 +2715,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -2740,10 +2849,1764 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AF52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>171</v>
+      </c>
+      <c r="L1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>179</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
+      <c r="AF2" s="2"/>
+    </row>
+    <row r="3" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>173</v>
+      </c>
+      <c r="K3" s="168" t="s">
+        <v>52</v>
+      </c>
+      <c r="L3" s="2">
+        <v>31</v>
+      </c>
+      <c r="M3" s="2">
+        <v>244</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="2"/>
+      <c r="AF3" s="2"/>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>174</v>
+      </c>
+      <c r="K4" s="171" t="s">
+        <v>159</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="2"/>
+      <c r="AA4" s="2"/>
+      <c r="AB4" s="2"/>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="2"/>
+      <c r="AE4" s="2"/>
+      <c r="AF4" s="2"/>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="K5" s="123" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" s="2">
+        <v>110</v>
+      </c>
+      <c r="M5" s="2">
+        <v>122</v>
+      </c>
+      <c r="N5" s="2">
+        <v>311</v>
+      </c>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="2"/>
+      <c r="AA5" s="2"/>
+      <c r="AB5" s="2"/>
+      <c r="AC5" s="2"/>
+      <c r="AD5" s="2"/>
+      <c r="AE5" s="2"/>
+      <c r="AF5" s="2"/>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>172</v>
+      </c>
+      <c r="F6" t="s">
+        <v>186</v>
+      </c>
+      <c r="K6" s="123" t="s">
+        <v>51</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0</v>
+      </c>
+      <c r="M6" s="2">
+        <v>43</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="2"/>
+      <c r="Z6" s="2"/>
+      <c r="AA6" s="2"/>
+      <c r="AB6" s="2"/>
+      <c r="AC6" s="2"/>
+      <c r="AD6" s="2"/>
+      <c r="AE6" s="2"/>
+      <c r="AF6" s="2"/>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>175</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>175</v>
+      </c>
+      <c r="K7" s="123" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0</v>
+      </c>
+      <c r="M7" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="N7" s="2">
+        <v>6</v>
+      </c>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="2"/>
+      <c r="AA7" s="2"/>
+      <c r="AB7" s="2"/>
+      <c r="AC7" s="2"/>
+      <c r="AD7" s="2"/>
+      <c r="AE7" s="2"/>
+      <c r="AF7" s="2"/>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>176</v>
+      </c>
+      <c r="F8">
+        <f>F7+1</f>
+        <v>2</v>
+      </c>
+      <c r="G8" t="s">
+        <v>176</v>
+      </c>
+      <c r="K8" s="123" t="s">
+        <v>21</v>
+      </c>
+      <c r="L8" s="2">
+        <v>0</v>
+      </c>
+      <c r="M8" s="2">
+        <v>3</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2"/>
+      <c r="AA8" s="2"/>
+      <c r="AB8" s="2"/>
+      <c r="AC8" s="2"/>
+      <c r="AD8" s="2"/>
+      <c r="AE8" s="2"/>
+      <c r="AF8" s="2"/>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>141</v>
+      </c>
+      <c r="F9">
+        <f t="shared" ref="F9:F21" si="0">F8+1</f>
+        <v>3</v>
+      </c>
+      <c r="G9" t="s">
+        <v>141</v>
+      </c>
+      <c r="K9" s="123" t="s">
+        <v>22</v>
+      </c>
+      <c r="L9" s="2">
+        <v>0</v>
+      </c>
+      <c r="M9" s="2">
+        <v>0</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2"/>
+      <c r="Z9" s="2"/>
+      <c r="AA9" s="2"/>
+      <c r="AB9" s="2"/>
+      <c r="AC9" s="2"/>
+      <c r="AD9" s="2"/>
+      <c r="AE9" s="2"/>
+      <c r="AF9" s="2"/>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>177</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G10" t="s">
+        <v>177</v>
+      </c>
+      <c r="K10" s="123" t="s">
+        <v>23</v>
+      </c>
+      <c r="L10" s="2">
+        <v>0</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
+      <c r="Z10" s="2"/>
+      <c r="AA10" s="2"/>
+      <c r="AB10" s="2"/>
+      <c r="AC10" s="2"/>
+      <c r="AD10" s="2"/>
+      <c r="AE10" s="2"/>
+      <c r="AF10" s="2"/>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>73</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G11" t="s">
+        <v>73</v>
+      </c>
+      <c r="K11" s="123" t="s">
+        <v>24</v>
+      </c>
+      <c r="L11" s="2">
+        <v>0</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2"/>
+      <c r="Y11" s="2"/>
+      <c r="Z11" s="2"/>
+      <c r="AA11" s="2"/>
+      <c r="AB11" s="2"/>
+      <c r="AC11" s="2"/>
+      <c r="AD11" s="2"/>
+      <c r="AE11" s="2"/>
+      <c r="AF11" s="2"/>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="G12" t="s">
+        <v>9</v>
+      </c>
+      <c r="K12" s="123" t="s">
+        <v>27</v>
+      </c>
+      <c r="L12" s="2">
+        <v>0</v>
+      </c>
+      <c r="M12" s="2">
+        <v>20</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2"/>
+      <c r="Y12" s="2"/>
+      <c r="Z12" s="2"/>
+      <c r="AA12" s="2"/>
+      <c r="AB12" s="2"/>
+      <c r="AC12" s="2"/>
+      <c r="AD12" s="2"/>
+      <c r="AE12" s="2"/>
+      <c r="AF12" s="2"/>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>90</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="G13" t="s">
+        <v>90</v>
+      </c>
+      <c r="K13" s="123" t="s">
+        <v>25</v>
+      </c>
+      <c r="L13" s="2">
+        <v>190</v>
+      </c>
+      <c r="M13" s="2">
+        <v>100</v>
+      </c>
+      <c r="N13" s="2">
+        <v>276</v>
+      </c>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2"/>
+      <c r="Z13" s="2"/>
+      <c r="AA13" s="2"/>
+      <c r="AB13" s="2"/>
+      <c r="AC13" s="2"/>
+      <c r="AD13" s="2"/>
+      <c r="AE13" s="2"/>
+      <c r="AF13" s="2"/>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="G14" t="s">
+        <v>91</v>
+      </c>
+      <c r="K14" s="123" t="s">
+        <v>26</v>
+      </c>
+      <c r="L14" s="2">
+        <v>70</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="N14" s="2">
+        <v>798</v>
+      </c>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2"/>
+      <c r="Y14" s="2"/>
+      <c r="Z14" s="2"/>
+      <c r="AA14" s="2"/>
+      <c r="AB14" s="2"/>
+      <c r="AC14" s="2"/>
+      <c r="AD14" s="2"/>
+      <c r="AE14" s="2"/>
+      <c r="AF14" s="2"/>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="G15" t="s">
+        <v>9</v>
+      </c>
+      <c r="K15" s="123" t="s">
+        <v>28</v>
+      </c>
+      <c r="L15" s="2">
+        <v>27</v>
+      </c>
+      <c r="M15" s="2">
+        <v>12</v>
+      </c>
+      <c r="N15" s="2">
+        <v>63</v>
+      </c>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2"/>
+      <c r="Y15" s="2"/>
+      <c r="Z15" s="2"/>
+      <c r="AA15" s="2"/>
+      <c r="AB15" s="2"/>
+      <c r="AC15" s="2"/>
+      <c r="AD15" s="2"/>
+      <c r="AE15" s="2"/>
+      <c r="AF15" s="2"/>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>183</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G16" t="s">
+        <v>183</v>
+      </c>
+      <c r="K16" s="123" t="s">
+        <v>29</v>
+      </c>
+      <c r="L16" s="2">
+        <v>3</v>
+      </c>
+      <c r="M16" s="2">
+        <v>0</v>
+      </c>
+      <c r="N16" s="2">
+        <v>14</v>
+      </c>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="2"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2"/>
+      <c r="Y16" s="2"/>
+      <c r="Z16" s="2"/>
+      <c r="AA16" s="2"/>
+      <c r="AB16" s="2"/>
+      <c r="AC16" s="2"/>
+      <c r="AD16" s="2"/>
+      <c r="AE16" s="2"/>
+      <c r="AF16" s="2"/>
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>184</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="G17" t="s">
+        <v>184</v>
+      </c>
+      <c r="K17" s="123" t="s">
+        <v>30</v>
+      </c>
+      <c r="L17" s="2">
+        <v>9</v>
+      </c>
+      <c r="M17" s="2">
+        <v>12</v>
+      </c>
+      <c r="N17" s="2">
+        <v>35</v>
+      </c>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2"/>
+      <c r="V17" s="2"/>
+      <c r="W17" s="2"/>
+      <c r="X17" s="2"/>
+      <c r="Y17" s="2"/>
+      <c r="Z17" s="2"/>
+      <c r="AA17" s="2"/>
+      <c r="AB17" s="2"/>
+      <c r="AC17" s="2"/>
+      <c r="AD17" s="2"/>
+      <c r="AE17" s="2"/>
+      <c r="AF17" s="2"/>
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>185</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="G18" t="s">
+        <v>185</v>
+      </c>
+      <c r="K18" s="123" t="s">
+        <v>31</v>
+      </c>
+      <c r="L18" s="2">
+        <v>2</v>
+      </c>
+      <c r="M18" s="2">
+        <v>8</v>
+      </c>
+      <c r="N18" s="2">
+        <v>9</v>
+      </c>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+      <c r="W18" s="2"/>
+      <c r="X18" s="2"/>
+      <c r="Y18" s="2"/>
+      <c r="Z18" s="2"/>
+      <c r="AA18" s="2"/>
+      <c r="AB18" s="2"/>
+      <c r="AC18" s="2"/>
+      <c r="AD18" s="2"/>
+      <c r="AE18" s="2"/>
+      <c r="AF18" s="2"/>
+    </row>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="G19" t="s">
+        <v>180</v>
+      </c>
+      <c r="K19" s="123"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2">
+        <v>0</v>
+      </c>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
+      <c r="U19" s="2"/>
+      <c r="V19" s="2"/>
+      <c r="W19" s="2"/>
+      <c r="X19" s="2"/>
+      <c r="Y19" s="2"/>
+      <c r="Z19" s="2"/>
+      <c r="AA19" s="2"/>
+      <c r="AB19" s="2"/>
+      <c r="AC19" s="2"/>
+      <c r="AD19" s="2"/>
+      <c r="AE19" s="2"/>
+      <c r="AF19" s="2"/>
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>178</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="G20" t="s">
+        <v>13</v>
+      </c>
+      <c r="K20" s="123" t="s">
+        <v>32</v>
+      </c>
+      <c r="L20" s="2">
+        <v>10</v>
+      </c>
+      <c r="M20" s="2">
+        <v>9</v>
+      </c>
+      <c r="N20" s="2">
+        <v>91</v>
+      </c>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
+      <c r="S20" s="2"/>
+      <c r="T20" s="2"/>
+      <c r="U20" s="2"/>
+      <c r="V20" s="2"/>
+      <c r="W20" s="2"/>
+      <c r="X20" s="2"/>
+      <c r="Y20" s="2"/>
+      <c r="Z20" s="2"/>
+      <c r="AA20" s="2"/>
+      <c r="AB20" s="2"/>
+      <c r="AC20" s="2"/>
+      <c r="AD20" s="2"/>
+      <c r="AE20" s="2"/>
+      <c r="AF20" s="2"/>
+    </row>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>175</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="G21" t="s">
+        <v>182</v>
+      </c>
+      <c r="K21" s="123" t="s">
+        <v>33</v>
+      </c>
+      <c r="L21" s="2">
+        <v>35</v>
+      </c>
+      <c r="M21" s="2">
+        <v>1</v>
+      </c>
+      <c r="N21" s="2">
+        <v>93</v>
+      </c>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
+      <c r="S21" s="2"/>
+      <c r="T21" s="2"/>
+      <c r="U21" s="2"/>
+      <c r="V21" s="2"/>
+      <c r="W21" s="2"/>
+      <c r="X21" s="2"/>
+      <c r="Y21" s="2"/>
+      <c r="Z21" s="2"/>
+      <c r="AA21" s="2"/>
+      <c r="AB21" s="2"/>
+      <c r="AC21" s="2"/>
+      <c r="AD21" s="2"/>
+      <c r="AE21" s="2"/>
+      <c r="AF21" s="2"/>
+    </row>
+    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>176</v>
+      </c>
+      <c r="G22" t="s">
+        <v>181</v>
+      </c>
+      <c r="K22" s="123" t="s">
+        <v>34</v>
+      </c>
+      <c r="L22" s="2">
+        <v>0</v>
+      </c>
+      <c r="M22" s="2">
+        <v>29</v>
+      </c>
+      <c r="N22" s="2">
+        <v>79</v>
+      </c>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
+      <c r="S22" s="2"/>
+      <c r="T22" s="2"/>
+      <c r="U22" s="2"/>
+      <c r="V22" s="2"/>
+      <c r="W22" s="2"/>
+      <c r="X22" s="2"/>
+      <c r="Y22" s="2"/>
+      <c r="Z22" s="2"/>
+      <c r="AA22" s="2"/>
+      <c r="AB22" s="2"/>
+      <c r="AC22" s="2"/>
+      <c r="AD22" s="2"/>
+      <c r="AE22" s="2"/>
+      <c r="AF22" s="2"/>
+    </row>
+    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="K23" s="123" t="s">
+        <v>35</v>
+      </c>
+      <c r="L23" s="2">
+        <v>45</v>
+      </c>
+      <c r="M23" s="2">
+        <v>0</v>
+      </c>
+      <c r="N23" s="2">
+        <v>35</v>
+      </c>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2"/>
+      <c r="V23" s="2"/>
+      <c r="W23" s="2"/>
+      <c r="X23" s="2"/>
+      <c r="Y23" s="2"/>
+      <c r="Z23" s="2"/>
+      <c r="AA23" s="2"/>
+      <c r="AB23" s="2"/>
+      <c r="AC23" s="2"/>
+      <c r="AD23" s="2"/>
+      <c r="AE23" s="2"/>
+      <c r="AF23" s="2"/>
+    </row>
+    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>180</v>
+      </c>
+      <c r="K24" s="123" t="s">
+        <v>36</v>
+      </c>
+      <c r="L24" s="2">
+        <v>10</v>
+      </c>
+      <c r="M24" s="2">
+        <v>26</v>
+      </c>
+      <c r="N24" s="2">
+        <v>110</v>
+      </c>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2"/>
+      <c r="S24" s="2"/>
+      <c r="T24" s="2"/>
+      <c r="U24" s="2"/>
+      <c r="V24" s="2"/>
+      <c r="W24" s="2"/>
+      <c r="X24" s="2"/>
+      <c r="Y24" s="2"/>
+      <c r="Z24" s="2"/>
+      <c r="AA24" s="2"/>
+      <c r="AB24" s="2"/>
+      <c r="AC24" s="2"/>
+      <c r="AD24" s="2"/>
+      <c r="AE24" s="2"/>
+      <c r="AF24" s="2"/>
+    </row>
+    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>13</v>
+      </c>
+      <c r="K25" s="123" t="s">
+        <v>37</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M25" s="2">
+        <v>0</v>
+      </c>
+      <c r="N25" s="2">
+        <v>129</v>
+      </c>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="2"/>
+      <c r="S25" s="2"/>
+      <c r="T25" s="2"/>
+      <c r="U25" s="2"/>
+      <c r="V25" s="2"/>
+      <c r="W25" s="2"/>
+      <c r="X25" s="2"/>
+      <c r="Y25" s="2"/>
+      <c r="Z25" s="2"/>
+      <c r="AA25" s="2"/>
+      <c r="AB25" s="2"/>
+      <c r="AC25" s="2"/>
+      <c r="AD25" s="2"/>
+      <c r="AE25" s="2"/>
+      <c r="AF25" s="2"/>
+    </row>
+    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>141</v>
+      </c>
+      <c r="K26" s="123" t="s">
+        <v>38</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M26" s="2">
+        <v>1</v>
+      </c>
+      <c r="N26" s="2">
+        <v>19</v>
+      </c>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="2"/>
+      <c r="S26" s="2"/>
+      <c r="T26" s="2"/>
+      <c r="U26" s="2"/>
+      <c r="V26" s="2"/>
+      <c r="W26" s="2"/>
+      <c r="X26" s="2"/>
+      <c r="Y26" s="2"/>
+      <c r="Z26" s="2"/>
+      <c r="AA26" s="2"/>
+      <c r="AB26" s="2"/>
+      <c r="AC26" s="2"/>
+      <c r="AD26" s="2"/>
+      <c r="AE26" s="2"/>
+      <c r="AF26" s="2"/>
+    </row>
+    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>73</v>
+      </c>
+      <c r="K27" s="123" t="s">
+        <v>39</v>
+      </c>
+      <c r="L27" s="2">
+        <v>35</v>
+      </c>
+      <c r="M27" s="2">
+        <v>6</v>
+      </c>
+      <c r="N27" s="2">
+        <v>74</v>
+      </c>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2"/>
+      <c r="S27" s="2"/>
+      <c r="T27" s="2"/>
+      <c r="U27" s="2"/>
+      <c r="V27" s="2"/>
+      <c r="W27" s="2"/>
+      <c r="X27" s="2"/>
+      <c r="Y27" s="2"/>
+      <c r="Z27" s="2"/>
+      <c r="AA27" s="2"/>
+      <c r="AB27" s="2"/>
+      <c r="AC27" s="2"/>
+      <c r="AD27" s="2"/>
+      <c r="AE27" s="2"/>
+      <c r="AF27" s="2"/>
+    </row>
+    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>90</v>
+      </c>
+      <c r="K28" s="123" t="s">
+        <v>40</v>
+      </c>
+      <c r="L28" s="2">
+        <v>35</v>
+      </c>
+      <c r="M28" s="2">
+        <v>27</v>
+      </c>
+      <c r="N28" s="2">
+        <v>75</v>
+      </c>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="2"/>
+      <c r="S28" s="2"/>
+      <c r="T28" s="2"/>
+      <c r="U28" s="2"/>
+      <c r="V28" s="2"/>
+      <c r="W28" s="2"/>
+      <c r="X28" s="2"/>
+      <c r="Y28" s="2"/>
+      <c r="Z28" s="2"/>
+      <c r="AA28" s="2"/>
+      <c r="AB28" s="2"/>
+      <c r="AC28" s="2"/>
+      <c r="AD28" s="2"/>
+      <c r="AE28" s="2"/>
+      <c r="AF28" s="2"/>
+    </row>
+    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>91</v>
+      </c>
+      <c r="K29" s="123" t="s">
+        <v>41</v>
+      </c>
+      <c r="L29" s="2">
+        <v>35</v>
+      </c>
+      <c r="M29" s="2">
+        <v>1</v>
+      </c>
+      <c r="N29" s="2">
+        <v>27</v>
+      </c>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="2"/>
+      <c r="S29" s="2"/>
+      <c r="T29" s="2"/>
+      <c r="U29" s="2"/>
+      <c r="V29" s="2"/>
+      <c r="W29" s="2"/>
+      <c r="X29" s="2"/>
+      <c r="Y29" s="2"/>
+      <c r="Z29" s="2"/>
+      <c r="AA29" s="2"/>
+      <c r="AB29" s="2"/>
+      <c r="AC29" s="2"/>
+      <c r="AD29" s="2"/>
+      <c r="AE29" s="2"/>
+      <c r="AF29" s="2"/>
+    </row>
+    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>9</v>
+      </c>
+      <c r="K30" s="123" t="s">
+        <v>42</v>
+      </c>
+      <c r="L30" s="2">
+        <v>35</v>
+      </c>
+      <c r="M30" s="2">
+        <v>5</v>
+      </c>
+      <c r="N30" s="2">
+        <v>106</v>
+      </c>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+      <c r="R30" s="2"/>
+      <c r="S30" s="2"/>
+      <c r="T30" s="2"/>
+      <c r="U30" s="2"/>
+      <c r="V30" s="2"/>
+      <c r="W30" s="2"/>
+      <c r="X30" s="2"/>
+      <c r="Y30" s="2"/>
+      <c r="Z30" s="2"/>
+      <c r="AA30" s="2"/>
+      <c r="AB30" s="2"/>
+      <c r="AC30" s="2"/>
+      <c r="AD30" s="2"/>
+      <c r="AE30" s="2"/>
+      <c r="AF30" s="2"/>
+    </row>
+    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>183</v>
+      </c>
+      <c r="K31" s="123" t="s">
+        <v>43</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M31" s="2">
+        <v>3</v>
+      </c>
+      <c r="N31" s="2">
+        <v>33</v>
+      </c>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
+      <c r="R31" s="2"/>
+      <c r="S31" s="2"/>
+      <c r="T31" s="2"/>
+      <c r="U31" s="2"/>
+      <c r="V31" s="2"/>
+      <c r="W31" s="2"/>
+      <c r="X31" s="2"/>
+      <c r="Y31" s="2"/>
+      <c r="Z31" s="2"/>
+      <c r="AA31" s="2"/>
+      <c r="AB31" s="2"/>
+      <c r="AC31" s="2"/>
+      <c r="AD31" s="2"/>
+      <c r="AE31" s="2"/>
+      <c r="AF31" s="2"/>
+    </row>
+    <row r="32" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>182</v>
+      </c>
+      <c r="K32" s="123" t="s">
+        <v>46</v>
+      </c>
+      <c r="L32" s="2">
+        <v>35</v>
+      </c>
+      <c r="M32" s="2">
+        <v>19</v>
+      </c>
+      <c r="N32" s="2">
+        <v>125</v>
+      </c>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="2"/>
+      <c r="R32" s="2"/>
+      <c r="S32" s="2"/>
+      <c r="T32" s="2"/>
+      <c r="U32" s="2"/>
+      <c r="V32" s="2"/>
+      <c r="W32" s="2"/>
+      <c r="X32" s="2"/>
+      <c r="Y32" s="2"/>
+      <c r="Z32" s="2"/>
+      <c r="AA32" s="2"/>
+      <c r="AB32" s="2"/>
+      <c r="AC32" s="2"/>
+      <c r="AD32" s="2"/>
+      <c r="AE32" s="2"/>
+      <c r="AF32" s="2"/>
+    </row>
+    <row r="33" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>181</v>
+      </c>
+      <c r="K33" s="123" t="s">
+        <v>44</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M33" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="N33" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="2"/>
+      <c r="R33" s="2"/>
+      <c r="S33" s="2"/>
+      <c r="T33" s="2"/>
+      <c r="U33" s="2"/>
+      <c r="V33" s="2"/>
+      <c r="W33" s="2"/>
+      <c r="X33" s="2"/>
+      <c r="Y33" s="2"/>
+      <c r="Z33" s="2"/>
+      <c r="AA33" s="2"/>
+      <c r="AB33" s="2"/>
+      <c r="AC33" s="2"/>
+      <c r="AD33" s="2"/>
+      <c r="AE33" s="2"/>
+      <c r="AF33" s="2"/>
+    </row>
+    <row r="34" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="K34" s="123" t="s">
+        <v>45</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M34" s="2">
+        <v>9</v>
+      </c>
+      <c r="N34" s="2">
+        <v>0</v>
+      </c>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2"/>
+      <c r="R34" s="2"/>
+      <c r="S34" s="2"/>
+      <c r="T34" s="2"/>
+      <c r="U34" s="2"/>
+      <c r="V34" s="2"/>
+      <c r="W34" s="2"/>
+      <c r="X34" s="2"/>
+      <c r="Y34" s="2"/>
+      <c r="Z34" s="2"/>
+      <c r="AA34" s="2"/>
+      <c r="AB34" s="2"/>
+      <c r="AC34" s="2"/>
+      <c r="AD34" s="2"/>
+      <c r="AE34" s="2"/>
+      <c r="AF34" s="2"/>
+    </row>
+    <row r="35" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="K35" s="123" t="s">
+        <v>47</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M35" s="2">
+        <v>23</v>
+      </c>
+      <c r="N35" s="2">
+        <v>12</v>
+      </c>
+      <c r="O35" s="2"/>
+      <c r="P35" s="2"/>
+      <c r="Q35" s="2"/>
+      <c r="R35" s="2"/>
+      <c r="S35" s="2"/>
+      <c r="T35" s="2"/>
+      <c r="U35" s="2"/>
+      <c r="V35" s="2"/>
+      <c r="W35" s="2"/>
+      <c r="X35" s="2"/>
+      <c r="Y35" s="2"/>
+      <c r="Z35" s="2"/>
+      <c r="AA35" s="2"/>
+      <c r="AB35" s="2"/>
+      <c r="AC35" s="2"/>
+      <c r="AD35" s="2"/>
+      <c r="AE35" s="2"/>
+      <c r="AF35" s="2"/>
+    </row>
+    <row r="36" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="K36" s="123" t="s">
+        <v>48</v>
+      </c>
+      <c r="L36" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M36" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="N36" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="O36" s="2"/>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="2"/>
+      <c r="R36" s="2"/>
+      <c r="S36" s="2"/>
+      <c r="T36" s="2"/>
+      <c r="U36" s="2"/>
+      <c r="V36" s="2"/>
+      <c r="W36" s="2"/>
+      <c r="X36" s="2"/>
+      <c r="Y36" s="2"/>
+      <c r="Z36" s="2"/>
+      <c r="AA36" s="2"/>
+      <c r="AB36" s="2"/>
+      <c r="AC36" s="2"/>
+      <c r="AD36" s="2"/>
+      <c r="AE36" s="2"/>
+      <c r="AF36" s="2"/>
+    </row>
+    <row r="37" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="K37" s="123" t="s">
+        <v>49</v>
+      </c>
+      <c r="L37" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M37" s="2">
+        <v>7</v>
+      </c>
+      <c r="N37" s="2">
+        <v>18</v>
+      </c>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2"/>
+      <c r="Q37" s="2"/>
+      <c r="R37" s="2"/>
+      <c r="S37" s="2"/>
+      <c r="T37" s="2"/>
+      <c r="U37" s="2"/>
+      <c r="V37" s="2"/>
+      <c r="W37" s="2"/>
+      <c r="X37" s="2"/>
+      <c r="Y37" s="2"/>
+      <c r="Z37" s="2"/>
+      <c r="AA37" s="2"/>
+      <c r="AB37" s="2"/>
+      <c r="AC37" s="2"/>
+      <c r="AD37" s="2"/>
+      <c r="AE37" s="2"/>
+      <c r="AF37" s="2"/>
+    </row>
+    <row r="38" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="198" t="s">
+        <v>203</v>
+      </c>
+      <c r="K38" s="124" t="s">
+        <v>50</v>
+      </c>
+      <c r="L38" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M38" s="2">
+        <v>9</v>
+      </c>
+      <c r="N38" s="2">
+        <v>2</v>
+      </c>
+      <c r="O38" s="2"/>
+      <c r="P38" s="2"/>
+      <c r="Q38" s="2"/>
+      <c r="R38" s="2"/>
+      <c r="S38" s="2"/>
+      <c r="T38" s="2"/>
+      <c r="U38" s="2"/>
+      <c r="V38" s="2"/>
+      <c r="W38" s="2"/>
+      <c r="X38" s="2"/>
+      <c r="Y38" s="2"/>
+      <c r="Z38" s="2"/>
+      <c r="AA38" s="2"/>
+      <c r="AB38" s="2"/>
+      <c r="AC38" s="2"/>
+      <c r="AD38" s="2"/>
+      <c r="AE38" s="2"/>
+      <c r="AF38" s="2"/>
+    </row>
+    <row r="39" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+      <c r="O39" s="2"/>
+      <c r="P39" s="2"/>
+      <c r="Q39" s="2"/>
+      <c r="R39" s="2"/>
+      <c r="S39" s="2"/>
+      <c r="T39" s="2"/>
+      <c r="U39" s="2"/>
+      <c r="V39" s="2"/>
+      <c r="W39" s="2"/>
+      <c r="X39" s="2"/>
+      <c r="Y39" s="2"/>
+      <c r="Z39" s="2"/>
+      <c r="AA39" s="2"/>
+      <c r="AB39" s="2"/>
+      <c r="AC39" s="2"/>
+      <c r="AD39" s="2"/>
+      <c r="AE39" s="2"/>
+      <c r="AF39" s="2"/>
+    </row>
+    <row r="40" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="2"/>
+      <c r="P40" s="2"/>
+      <c r="Q40" s="2"/>
+      <c r="R40" s="2"/>
+      <c r="S40" s="2"/>
+      <c r="T40" s="2"/>
+      <c r="U40" s="2"/>
+      <c r="V40" s="2"/>
+      <c r="W40" s="2"/>
+      <c r="X40" s="2"/>
+      <c r="Y40" s="2"/>
+      <c r="Z40" s="2"/>
+      <c r="AA40" s="2"/>
+      <c r="AB40" s="2"/>
+      <c r="AC40" s="2"/>
+      <c r="AD40" s="2"/>
+      <c r="AE40" s="2"/>
+      <c r="AF40" s="2"/>
+    </row>
+    <row r="41" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="L41" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+      <c r="O41" s="2"/>
+      <c r="P41" s="2"/>
+      <c r="Q41" s="2"/>
+      <c r="R41" s="2"/>
+      <c r="S41" s="2"/>
+      <c r="T41" s="2"/>
+      <c r="U41" s="2"/>
+      <c r="V41" s="2"/>
+      <c r="W41" s="2"/>
+      <c r="X41" s="2"/>
+      <c r="Y41" s="2"/>
+      <c r="Z41" s="2"/>
+      <c r="AA41" s="2"/>
+      <c r="AB41" s="2"/>
+      <c r="AC41" s="2"/>
+      <c r="AD41" s="2"/>
+      <c r="AE41" s="2"/>
+      <c r="AF41" s="2"/>
+    </row>
+    <row r="42" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="L42" s="2">
+        <v>2</v>
+      </c>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+      <c r="O42" s="2"/>
+      <c r="P42" s="2"/>
+      <c r="Q42" s="2"/>
+      <c r="R42" s="2"/>
+      <c r="S42" s="2"/>
+      <c r="T42" s="2"/>
+      <c r="U42" s="2"/>
+      <c r="V42" s="2"/>
+      <c r="W42" s="2"/>
+      <c r="X42" s="2"/>
+      <c r="Y42" s="2"/>
+      <c r="Z42" s="2"/>
+      <c r="AA42" s="2"/>
+      <c r="AB42" s="2"/>
+      <c r="AC42" s="2"/>
+      <c r="AD42" s="2"/>
+      <c r="AE42" s="2"/>
+      <c r="AF42" s="2"/>
+    </row>
+    <row r="43" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="O43" s="2"/>
+      <c r="P43" s="2"/>
+      <c r="Q43" s="2"/>
+      <c r="R43" s="2"/>
+      <c r="S43" s="2"/>
+      <c r="T43" s="2"/>
+      <c r="U43" s="2"/>
+      <c r="V43" s="2"/>
+      <c r="W43" s="2"/>
+      <c r="X43" s="2"/>
+      <c r="Y43" s="2"/>
+      <c r="Z43" s="2"/>
+      <c r="AA43" s="2"/>
+      <c r="AB43" s="2"/>
+      <c r="AC43" s="2"/>
+      <c r="AD43" s="2"/>
+      <c r="AE43" s="2"/>
+      <c r="AF43" s="2"/>
+    </row>
+    <row r="44" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+      <c r="O44" s="2"/>
+      <c r="P44" s="2"/>
+      <c r="Q44" s="2"/>
+      <c r="R44" s="2"/>
+      <c r="S44" s="2"/>
+      <c r="T44" s="2"/>
+      <c r="U44" s="2"/>
+      <c r="V44" s="2"/>
+      <c r="W44" s="2"/>
+      <c r="X44" s="2"/>
+      <c r="Y44" s="2"/>
+      <c r="Z44" s="2"/>
+      <c r="AA44" s="2"/>
+      <c r="AB44" s="2"/>
+      <c r="AC44" s="2"/>
+      <c r="AD44" s="2"/>
+      <c r="AE44" s="2"/>
+      <c r="AF44" s="2"/>
+    </row>
+    <row r="45" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+      <c r="O45" s="2"/>
+      <c r="P45" s="2"/>
+      <c r="Q45" s="2"/>
+      <c r="R45" s="2"/>
+      <c r="S45" s="2"/>
+      <c r="T45" s="2"/>
+      <c r="U45" s="2"/>
+      <c r="V45" s="2"/>
+      <c r="W45" s="2"/>
+      <c r="X45" s="2"/>
+      <c r="Y45" s="2"/>
+      <c r="Z45" s="2"/>
+      <c r="AA45" s="2"/>
+      <c r="AB45" s="2"/>
+      <c r="AC45" s="2"/>
+      <c r="AD45" s="2"/>
+      <c r="AE45" s="2"/>
+      <c r="AF45" s="2"/>
+    </row>
+    <row r="46" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
+      <c r="O46" s="2"/>
+      <c r="P46" s="2"/>
+      <c r="Q46" s="2"/>
+      <c r="R46" s="2"/>
+      <c r="S46" s="2"/>
+      <c r="T46" s="2"/>
+      <c r="U46" s="2"/>
+      <c r="V46" s="2"/>
+      <c r="W46" s="2"/>
+      <c r="X46" s="2"/>
+      <c r="Y46" s="2"/>
+      <c r="Z46" s="2"/>
+      <c r="AA46" s="2"/>
+      <c r="AB46" s="2"/>
+      <c r="AC46" s="2"/>
+      <c r="AD46" s="2"/>
+      <c r="AE46" s="2"/>
+      <c r="AF46" s="2"/>
+    </row>
+    <row r="47" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+      <c r="N47" s="2"/>
+      <c r="O47" s="2"/>
+      <c r="P47" s="2"/>
+      <c r="Q47" s="2"/>
+      <c r="R47" s="2"/>
+      <c r="S47" s="2"/>
+      <c r="T47" s="2"/>
+      <c r="U47" s="2"/>
+      <c r="V47" s="2"/>
+      <c r="W47" s="2"/>
+      <c r="X47" s="2"/>
+      <c r="Y47" s="2"/>
+      <c r="Z47" s="2"/>
+      <c r="AA47" s="2"/>
+      <c r="AB47" s="2"/>
+      <c r="AC47" s="2"/>
+      <c r="AD47" s="2"/>
+      <c r="AE47" s="2"/>
+      <c r="AF47" s="2"/>
+    </row>
+    <row r="48" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="L48" s="2"/>
+      <c r="M48" s="2"/>
+      <c r="N48" s="2"/>
+      <c r="O48" s="2"/>
+      <c r="P48" s="2"/>
+      <c r="Q48" s="2"/>
+      <c r="R48" s="2"/>
+      <c r="S48" s="2"/>
+      <c r="T48" s="2"/>
+      <c r="U48" s="2"/>
+      <c r="V48" s="2"/>
+      <c r="W48" s="2"/>
+      <c r="X48" s="2"/>
+      <c r="Y48" s="2"/>
+      <c r="Z48" s="2"/>
+      <c r="AA48" s="2"/>
+      <c r="AB48" s="2"/>
+      <c r="AC48" s="2"/>
+      <c r="AD48" s="2"/>
+      <c r="AE48" s="2"/>
+      <c r="AF48" s="2"/>
+    </row>
+    <row r="49" spans="12:32" x14ac:dyDescent="0.25">
+      <c r="L49" s="2"/>
+      <c r="M49" s="2"/>
+      <c r="N49" s="2"/>
+      <c r="O49" s="2"/>
+      <c r="P49" s="2"/>
+      <c r="Q49" s="2"/>
+      <c r="R49" s="2"/>
+      <c r="S49" s="2"/>
+      <c r="T49" s="2"/>
+      <c r="U49" s="2"/>
+      <c r="V49" s="2"/>
+      <c r="W49" s="2"/>
+      <c r="X49" s="2"/>
+      <c r="Y49" s="2"/>
+      <c r="Z49" s="2"/>
+      <c r="AA49" s="2"/>
+      <c r="AB49" s="2"/>
+      <c r="AC49" s="2"/>
+      <c r="AD49" s="2"/>
+      <c r="AE49" s="2"/>
+      <c r="AF49" s="2"/>
+    </row>
+    <row r="50" spans="12:32" x14ac:dyDescent="0.25">
+      <c r="L50" s="2"/>
+      <c r="M50" s="2"/>
+      <c r="N50" s="2"/>
+      <c r="O50" s="2"/>
+      <c r="P50" s="2"/>
+      <c r="Q50" s="2"/>
+      <c r="R50" s="2"/>
+      <c r="S50" s="2"/>
+      <c r="T50" s="2"/>
+      <c r="U50" s="2"/>
+      <c r="V50" s="2"/>
+      <c r="W50" s="2"/>
+      <c r="X50" s="2"/>
+      <c r="Y50" s="2"/>
+      <c r="Z50" s="2"/>
+      <c r="AA50" s="2"/>
+      <c r="AB50" s="2"/>
+      <c r="AC50" s="2"/>
+      <c r="AD50" s="2"/>
+      <c r="AE50" s="2"/>
+      <c r="AF50" s="2"/>
+    </row>
+    <row r="51" spans="12:32" x14ac:dyDescent="0.25">
+      <c r="L51" s="2"/>
+      <c r="M51" s="2"/>
+      <c r="N51" s="2"/>
+      <c r="O51" s="2"/>
+      <c r="P51" s="2"/>
+      <c r="Q51" s="2"/>
+      <c r="R51" s="2"/>
+      <c r="S51" s="2"/>
+      <c r="T51" s="2"/>
+      <c r="U51" s="2"/>
+      <c r="V51" s="2"/>
+      <c r="W51" s="2"/>
+      <c r="X51" s="2"/>
+      <c r="Y51" s="2"/>
+      <c r="Z51" s="2"/>
+      <c r="AA51" s="2"/>
+      <c r="AB51" s="2"/>
+      <c r="AC51" s="2"/>
+      <c r="AD51" s="2"/>
+      <c r="AE51" s="2"/>
+      <c r="AF51" s="2"/>
+    </row>
+    <row r="52" spans="12:32" x14ac:dyDescent="0.25">
+      <c r="L52" s="2"/>
+      <c r="M52" s="2"/>
+      <c r="N52" s="2"/>
+      <c r="O52" s="2"/>
+      <c r="P52" s="2"/>
+      <c r="Q52" s="2"/>
+      <c r="R52" s="2"/>
+      <c r="S52" s="2"/>
+      <c r="T52" s="2"/>
+      <c r="U52" s="2"/>
+      <c r="V52" s="2"/>
+      <c r="W52" s="2"/>
+      <c r="X52" s="2"/>
+      <c r="Y52" s="2"/>
+      <c r="Z52" s="2"/>
+      <c r="AA52" s="2"/>
+      <c r="AB52" s="2"/>
+      <c r="AC52" s="2"/>
+      <c r="AD52" s="2"/>
+      <c r="AE52" s="2"/>
+      <c r="AF52" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:P37"/>
+      <selection activeCell="G2" sqref="G2:G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2835,7 +4698,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="16.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="168" t="s">
         <v>52</v>
       </c>
@@ -2925,30 +4788,30 @@
       <c r="F3" s="77" t="s">
         <v>169</v>
       </c>
-      <c r="G3" s="249" t="s">
+      <c r="G3" s="214" t="s">
         <v>165</v>
       </c>
-      <c r="H3" s="242" t="s">
+      <c r="H3" s="212" t="s">
         <v>88</v>
       </c>
-      <c r="I3" s="231" t="s">
+      <c r="I3" s="203" t="s">
         <v>93</v>
       </c>
       <c r="J3" s="89" t="s">
         <v>163</v>
       </c>
-      <c r="K3" s="238" t="s">
+      <c r="K3" s="210" t="s">
         <v>170</v>
       </c>
-      <c r="L3" s="232" t="s">
+      <c r="L3" s="204" t="s">
         <v>164</v>
       </c>
-      <c r="M3" s="234" t="s">
+      <c r="M3" s="206" t="s">
         <v>92</v>
       </c>
-      <c r="N3" s="246"/>
-      <c r="O3" s="247"/>
-      <c r="P3" s="248"/>
+      <c r="N3" s="231"/>
+      <c r="O3" s="232"/>
+      <c r="P3" s="233"/>
       <c r="R3" s="2"/>
       <c r="S3" s="111"/>
       <c r="T3" s="2"/>
@@ -2984,7 +4847,7 @@
       <c r="F4" s="78">
         <v>200</v>
       </c>
-      <c r="G4" s="236">
+      <c r="G4" s="208">
         <f>X41*X4</f>
         <v>311</v>
       </c>
@@ -3010,10 +4873,10 @@
         <v>80</v>
       </c>
       <c r="N4" s="116">
-        <f>SUM(B4:M4)+SUM(Z4:AC4)</f>
+        <f t="shared" ref="N4:N13" si="3">SUM(B4:M4)+SUM(Z4:AC4)</f>
         <v>2364</v>
       </c>
-      <c r="O4" s="226">
+      <c r="O4" s="200">
         <v>2200</v>
       </c>
       <c r="P4" s="120">
@@ -3081,7 +4944,7 @@
       <c r="F5" s="78">
         <v>140</v>
       </c>
-      <c r="G5" s="236" t="s">
+      <c r="G5" s="208" t="s">
         <v>56</v>
       </c>
       <c r="H5" s="149">
@@ -3105,7 +4968,7 @@
         <v>0</v>
       </c>
       <c r="N5" s="34">
-        <f>SUM(B5:M5)+SUM(Z5:AC5)</f>
+        <f t="shared" si="3"/>
         <v>674.5</v>
       </c>
       <c r="O5" s="157" t="s">
@@ -3155,7 +5018,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="132">
-        <f t="shared" ref="B6:B31" si="3">$R$41*R6</f>
+        <f t="shared" ref="B6:B31" si="4">$R$41*R6</f>
         <v>0</v>
       </c>
       <c r="C6" s="28">
@@ -3163,18 +5026,18 @@
         <v>0.89999999999999991</v>
       </c>
       <c r="D6" s="85">
-        <f t="shared" ref="D6:D37" si="4">$S$41*S6</f>
+        <f t="shared" ref="D6:D37" si="5">$S$41*S6</f>
         <v>4.5</v>
       </c>
       <c r="E6" s="24">
-        <f t="shared" ref="E6:E36" si="5">U6*$U$41</f>
+        <f t="shared" ref="E6:E36" si="6">U6*$U$41</f>
         <v>7.5</v>
       </c>
       <c r="F6" s="78">
         <v>15</v>
       </c>
-      <c r="G6" s="236">
-        <f t="shared" ref="G6:G36" si="6">$X$41*X6</f>
+      <c r="G6" s="208">
+        <f t="shared" ref="G6:G36" si="7">$X$41*X6</f>
         <v>6</v>
       </c>
       <c r="H6" s="149">
@@ -3198,7 +5061,7 @@
         <v>0</v>
       </c>
       <c r="N6" s="115">
-        <f>SUM(B6:M6)+SUM(Z6:AC6)</f>
+        <f t="shared" si="3"/>
         <v>73.900000000000006</v>
       </c>
       <c r="O6" s="159">
@@ -3259,17 +5122,17 @@
         <v>4.5</v>
       </c>
       <c r="D7" s="85">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.5</v>
       </c>
       <c r="E7" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F7" s="78">
         <v>3</v>
       </c>
-      <c r="G7" s="236" t="s">
+      <c r="G7" s="208" t="s">
         <v>56</v>
       </c>
       <c r="H7" s="149">
@@ -3293,11 +5156,11 @@
         <v>0</v>
       </c>
       <c r="N7" s="34">
-        <f>SUM(B7:M7)+SUM(Z7:AC7)</f>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="O7" s="158">
-        <f t="shared" ref="O7:O37" si="7">P7</f>
+        <f t="shared" ref="O7:O37" si="8">P7</f>
         <v>20</v>
       </c>
       <c r="P7" s="8">
@@ -3344,7 +5207,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="132">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C8" s="28">
@@ -3352,17 +5215,17 @@
         <v>0</v>
       </c>
       <c r="D8" s="85">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E8" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F8" s="78">
         <v>0</v>
       </c>
-      <c r="G8" s="236" t="s">
+      <c r="G8" s="208" t="s">
         <v>56</v>
       </c>
       <c r="H8" s="149">
@@ -3386,11 +5249,11 @@
         <v>0</v>
       </c>
       <c r="N8" s="34">
-        <f>SUM(B8:M8)+SUM(Z8:AC8)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O8" s="158" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-</v>
       </c>
       <c r="P8" s="8" t="s">
@@ -3437,24 +5300,24 @@
         <v>23</v>
       </c>
       <c r="B9" s="132">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C9" s="28">
         <v>0</v>
       </c>
       <c r="D9" s="85">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E9" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.5</v>
       </c>
       <c r="F9" s="78" t="s">
         <v>56</v>
       </c>
-      <c r="G9" s="236" t="s">
+      <c r="G9" s="208" t="s">
         <v>56</v>
       </c>
       <c r="H9" s="149" t="s">
@@ -3477,11 +5340,11 @@
         <v>0</v>
       </c>
       <c r="N9" s="34">
-        <f>SUM(B9:M9)+SUM(Z9:AC9)</f>
+        <f t="shared" si="3"/>
         <v>5.5</v>
       </c>
       <c r="O9" s="158" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-</v>
       </c>
       <c r="P9" s="8" t="s">
@@ -3528,24 +5391,24 @@
         <v>24</v>
       </c>
       <c r="B10" s="132">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C10" s="28">
         <v>0</v>
       </c>
       <c r="D10" s="85">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E10" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.5</v>
       </c>
       <c r="F10" s="78" t="s">
         <v>56</v>
       </c>
-      <c r="G10" s="236" t="s">
+      <c r="G10" s="208" t="s">
         <v>56</v>
       </c>
       <c r="H10" s="149" t="s">
@@ -3568,11 +5431,11 @@
         <v>0</v>
       </c>
       <c r="N10" s="34">
-        <f>SUM(B10:M10)+SUM(Z10:AC10)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="O10" s="158" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-</v>
       </c>
       <c r="P10" s="8" t="s">
@@ -3617,7 +5480,7 @@
         <v>27</v>
       </c>
       <c r="B11" s="132">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C11" s="28">
@@ -3625,17 +5488,17 @@
         <v>30</v>
       </c>
       <c r="D11" s="85">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>90</v>
       </c>
       <c r="E11" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F11" s="78">
         <v>0</v>
       </c>
-      <c r="G11" s="236" t="s">
+      <c r="G11" s="208" t="s">
         <v>56</v>
       </c>
       <c r="H11" s="149">
@@ -3659,11 +5522,11 @@
         <v>10</v>
       </c>
       <c r="N11" s="34">
-        <f>SUM(B11:M11)+SUM(Z11:AC11)</f>
+        <f t="shared" si="3"/>
         <v>225</v>
       </c>
       <c r="O11" s="158">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>300</v>
       </c>
       <c r="P11" s="8">
@@ -3710,7 +5573,7 @@
         <v>25</v>
       </c>
       <c r="B12" s="132">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>380</v>
       </c>
       <c r="C12" s="28">
@@ -3718,18 +5581,18 @@
         <v>150</v>
       </c>
       <c r="D12" s="85">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>180</v>
       </c>
       <c r="E12" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>480</v>
       </c>
       <c r="F12" s="78">
         <v>125</v>
       </c>
-      <c r="G12" s="236">
-        <f t="shared" si="6"/>
+      <c r="G12" s="208">
+        <f t="shared" si="7"/>
         <v>276</v>
       </c>
       <c r="H12" s="149">
@@ -3754,11 +5617,11 @@
         <v>55</v>
       </c>
       <c r="N12" s="54">
-        <f>SUM(B12:M12)+SUM(Z12:AC12)</f>
+        <f t="shared" si="3"/>
         <v>3426</v>
       </c>
       <c r="O12" s="158">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2400</v>
       </c>
       <c r="P12" s="8">
@@ -3803,25 +5666,25 @@
         <v>26</v>
       </c>
       <c r="B13" s="132">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>140</v>
       </c>
       <c r="C13" s="28">
         <v>0</v>
       </c>
       <c r="D13" s="85">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>375</v>
       </c>
       <c r="E13" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>105</v>
       </c>
       <c r="F13" s="78">
         <v>210</v>
       </c>
-      <c r="G13" s="236">
-        <f t="shared" si="6"/>
+      <c r="G13" s="208">
+        <f t="shared" si="7"/>
         <v>798</v>
       </c>
       <c r="H13" s="149">
@@ -3844,11 +5707,11 @@
         <v>160</v>
       </c>
       <c r="N13" s="114">
-        <f>SUM(B13:M13)+SUM(Z13:AC13)</f>
+        <f t="shared" si="3"/>
         <v>2000.1428571428571</v>
       </c>
       <c r="O13" s="20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3500</v>
       </c>
       <c r="P13" s="87">
@@ -3894,7 +5757,7 @@
         <v>28</v>
       </c>
       <c r="B14" s="132">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>54</v>
       </c>
       <c r="C14" s="28">
@@ -3902,22 +5765,22 @@
         <v>18</v>
       </c>
       <c r="D14" s="85">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>25.5</v>
       </c>
       <c r="E14" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="F14" s="78">
         <v>16</v>
       </c>
-      <c r="G14" s="236">
-        <f t="shared" si="6"/>
+      <c r="G14" s="208">
+        <f t="shared" si="7"/>
         <v>63</v>
       </c>
       <c r="H14" s="149">
-        <f t="shared" ref="H14:H22" si="8">$V$41*V14</f>
+        <f t="shared" ref="H14:H22" si="9">$V$41*V14</f>
         <v>27</v>
       </c>
       <c r="I14" s="142">
@@ -3942,7 +5805,7 @@
         <v>280.5</v>
       </c>
       <c r="O14" s="159">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>300</v>
       </c>
       <c r="P14" s="117">
@@ -3992,7 +5855,7 @@
         <v>29</v>
       </c>
       <c r="B15" s="132">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="C15" s="28">
@@ -4000,22 +5863,22 @@
         <v>0</v>
       </c>
       <c r="D15" s="85">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="E15" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="F15" s="78">
         <v>7</v>
       </c>
-      <c r="G15" s="236">
-        <f t="shared" si="6"/>
+      <c r="G15" s="208">
+        <f t="shared" si="7"/>
         <v>14</v>
       </c>
       <c r="H15" s="149">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="I15" s="142" t="s">
@@ -4039,7 +5902,7 @@
         <v>53</v>
       </c>
       <c r="O15" s="158">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>25</v>
       </c>
       <c r="P15" s="15">
@@ -4086,7 +5949,7 @@
         <v>30</v>
       </c>
       <c r="B16" s="132">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="C16" s="28">
@@ -4094,22 +5957,22 @@
         <v>18</v>
       </c>
       <c r="D16" s="85">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.5</v>
       </c>
       <c r="E16" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F16" s="78">
         <v>5</v>
       </c>
-      <c r="G16" s="236">
-        <f t="shared" si="6"/>
+      <c r="G16" s="208">
+        <f t="shared" si="7"/>
         <v>35</v>
       </c>
       <c r="H16" s="149">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="I16" s="142" t="s">
@@ -4133,7 +5996,7 @@
         <v>97.5</v>
       </c>
       <c r="O16" s="158" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-</v>
       </c>
       <c r="P16" s="119" t="s">
@@ -4180,7 +6043,7 @@
         <v>31</v>
       </c>
       <c r="B17" s="132">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="C17" s="28">
@@ -4188,22 +6051,22 @@
         <v>12</v>
       </c>
       <c r="D17" s="85">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>37.5</v>
       </c>
       <c r="E17" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="F17" s="78">
         <v>6</v>
       </c>
-      <c r="G17" s="236">
-        <f t="shared" si="6"/>
+      <c r="G17" s="208">
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
       <c r="H17" s="149">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>48</v>
       </c>
       <c r="I17" s="142" t="s">
@@ -4273,24 +6136,24 @@
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" s="123"/>
-      <c r="B18" s="224"/>
-      <c r="C18" s="223"/>
-      <c r="D18" s="240"/>
-      <c r="E18" s="227"/>
-      <c r="F18" s="241"/>
-      <c r="G18" s="236">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="H18" s="243"/>
-      <c r="I18" s="228"/>
-      <c r="J18" s="244"/>
-      <c r="K18" s="239"/>
-      <c r="L18" s="229"/>
-      <c r="M18" s="235"/>
-      <c r="N18" s="245"/>
-      <c r="O18" s="230"/>
-      <c r="P18" s="233"/>
+      <c r="B18" s="229"/>
+      <c r="C18" s="230"/>
+      <c r="D18" s="220"/>
+      <c r="E18" s="221"/>
+      <c r="F18" s="222"/>
+      <c r="G18" s="208">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H18" s="223"/>
+      <c r="I18" s="224"/>
+      <c r="J18" s="225"/>
+      <c r="K18" s="211"/>
+      <c r="L18" s="201"/>
+      <c r="M18" s="207"/>
+      <c r="N18" s="213"/>
+      <c r="O18" s="202"/>
+      <c r="P18" s="205"/>
       <c r="Q18" s="121"/>
       <c r="R18" s="2"/>
       <c r="S18" s="112"/>
@@ -4316,30 +6179,30 @@
         <v>32</v>
       </c>
       <c r="B19" s="132">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="C19" s="28">
-        <f>1.5*T19</f>
+        <f t="shared" ref="C19:C31" si="10">1.5*T19</f>
         <v>13.5</v>
       </c>
       <c r="D19" s="85">
-        <f t="shared" si="4"/>
-        <v>30</v>
-      </c>
-      <c r="E19" s="24">
         <f t="shared" si="5"/>
         <v>30</v>
       </c>
+      <c r="E19" s="24">
+        <f t="shared" si="6"/>
+        <v>30</v>
+      </c>
       <c r="F19" s="78">
         <v>0</v>
       </c>
-      <c r="G19" s="236">
-        <f t="shared" si="6"/>
+      <c r="G19" s="208">
+        <f t="shared" si="7"/>
         <v>91</v>
       </c>
       <c r="H19" s="149">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>45</v>
       </c>
       <c r="I19" s="142" t="s">
@@ -4359,11 +6222,11 @@
         <v>0</v>
       </c>
       <c r="N19" s="54">
-        <f>SUM(B19:M19)+Z19</f>
+        <f t="shared" ref="N19:N29" si="11">SUM(B19:M19)+Z19</f>
         <v>335.5</v>
       </c>
       <c r="O19" s="158">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
       <c r="P19" s="8">
@@ -4410,30 +6273,30 @@
         <v>33</v>
       </c>
       <c r="B20" s="132">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
       <c r="C20" s="28">
-        <f>1.5*T20</f>
+        <f t="shared" si="10"/>
         <v>1.5</v>
       </c>
       <c r="D20" s="85">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>90</v>
       </c>
       <c r="E20" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F20" s="78">
         <v>0</v>
       </c>
-      <c r="G20" s="236">
-        <f t="shared" si="6"/>
+      <c r="G20" s="208">
+        <f t="shared" si="7"/>
         <v>93</v>
       </c>
       <c r="H20" s="149">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>45</v>
       </c>
       <c r="I20" s="142" t="s">
@@ -4453,11 +6316,11 @@
         <v>0</v>
       </c>
       <c r="N20" s="54">
-        <f>SUM(B20:M20)+Z20</f>
+        <f t="shared" si="11"/>
         <v>401.5</v>
       </c>
       <c r="O20" s="158">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
       <c r="P20" s="8">
@@ -4503,30 +6366,30 @@
         <v>34</v>
       </c>
       <c r="B21" s="132">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C21" s="28">
-        <f>1.5*T21</f>
+        <f t="shared" si="10"/>
         <v>43.5</v>
       </c>
       <c r="D21" s="85">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>75</v>
       </c>
       <c r="E21" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>135</v>
       </c>
       <c r="F21" s="78">
         <v>6</v>
       </c>
-      <c r="G21" s="236">
-        <f t="shared" si="6"/>
+      <c r="G21" s="208">
+        <f t="shared" si="7"/>
         <v>79</v>
       </c>
       <c r="H21" s="149">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>75</v>
       </c>
       <c r="I21" s="142" t="s">
@@ -4546,11 +6409,11 @@
         <v>15</v>
       </c>
       <c r="N21" s="54">
-        <f>SUM(B21:M21)+Z21</f>
+        <f t="shared" si="11"/>
         <v>607.5</v>
       </c>
       <c r="O21" s="158">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
       <c r="P21" s="8">
@@ -4596,30 +6459,30 @@
         <v>35</v>
       </c>
       <c r="B22" s="132">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>90</v>
       </c>
       <c r="C22" s="28">
-        <f>1.5*T22</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="D22" s="85">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="E22" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="F22" s="78">
         <v>8</v>
       </c>
-      <c r="G22" s="236">
-        <f t="shared" si="6"/>
+      <c r="G22" s="208">
+        <f t="shared" si="7"/>
         <v>35</v>
       </c>
       <c r="H22" s="149">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>45</v>
       </c>
       <c r="I22" s="142" t="s">
@@ -4639,11 +6502,11 @@
         <v>0</v>
       </c>
       <c r="N22" s="54">
-        <f>SUM(B22:M22)+Z22</f>
+        <f t="shared" si="11"/>
         <v>336</v>
       </c>
       <c r="O22" s="158">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
       <c r="P22" s="8">
@@ -4689,25 +6552,25 @@
         <v>36</v>
       </c>
       <c r="B23" s="132">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="C23" s="28">
-        <f>1.5*T23</f>
+        <f t="shared" si="10"/>
         <v>39</v>
       </c>
       <c r="D23" s="85">
         <v>0</v>
       </c>
       <c r="E23" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>75</v>
       </c>
       <c r="F23" s="78" t="s">
         <v>56</v>
       </c>
-      <c r="G23" s="236">
-        <f t="shared" si="6"/>
+      <c r="G23" s="208">
+        <f t="shared" si="7"/>
         <v>110</v>
       </c>
       <c r="H23" s="149" t="s">
@@ -4730,11 +6593,11 @@
         <v>0</v>
       </c>
       <c r="N23" s="54">
-        <f>SUM(B23:M23)+Z23</f>
+        <f t="shared" si="11"/>
         <v>569</v>
       </c>
       <c r="O23" s="158">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
       <c r="P23" s="8">
@@ -4783,22 +6646,22 @@
         <v>0</v>
       </c>
       <c r="C24" s="28">
-        <f>1.5*T24</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="D24" s="85">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="E24" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>60</v>
       </c>
       <c r="F24" s="78">
         <v>25</v>
       </c>
-      <c r="G24" s="236">
-        <f t="shared" si="6"/>
+      <c r="G24" s="208">
+        <f t="shared" si="7"/>
         <v>129</v>
       </c>
       <c r="H24" s="149" t="s">
@@ -4821,11 +6684,11 @@
         <v>0</v>
       </c>
       <c r="N24" s="54">
-        <f>SUM(B24:M24)+Z24</f>
+        <f t="shared" si="11"/>
         <v>404</v>
       </c>
       <c r="O24" s="158">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
       <c r="P24" s="8">
@@ -4874,7 +6737,7 @@
         <v>0</v>
       </c>
       <c r="C25" s="28">
-        <f>1.5*T25</f>
+        <f t="shared" si="10"/>
         <v>1.5</v>
       </c>
       <c r="D25" s="85">
@@ -4886,8 +6749,8 @@
       <c r="F25" s="78" t="s">
         <v>56</v>
       </c>
-      <c r="G25" s="236">
-        <f t="shared" si="6"/>
+      <c r="G25" s="208">
+        <f t="shared" si="7"/>
         <v>19</v>
       </c>
       <c r="H25" s="149" t="s">
@@ -4909,11 +6772,11 @@
         <v>0</v>
       </c>
       <c r="N25" s="54">
-        <f>SUM(B25:M25)+Z25</f>
+        <f t="shared" si="11"/>
         <v>51.5</v>
       </c>
       <c r="O25" s="165">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
       <c r="P25" s="15">
@@ -4959,15 +6822,15 @@
         <v>39</v>
       </c>
       <c r="B26" s="132">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
       <c r="C26" s="28">
-        <f>1.5*T26</f>
+        <f t="shared" si="10"/>
         <v>9</v>
       </c>
       <c r="D26" s="85">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="E26" s="24">
@@ -4976,8 +6839,8 @@
       <c r="F26" s="78" t="s">
         <v>56</v>
       </c>
-      <c r="G26" s="236">
-        <f t="shared" si="6"/>
+      <c r="G26" s="208">
+        <f t="shared" si="7"/>
         <v>74</v>
       </c>
       <c r="H26" s="149" t="s">
@@ -4999,11 +6862,11 @@
         <v>0</v>
       </c>
       <c r="N26" s="54">
-        <f>SUM(B26:M26)+Z26</f>
+        <f t="shared" si="11"/>
         <v>283</v>
       </c>
       <c r="O26" s="158">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
       <c r="P26" s="8">
@@ -5049,26 +6912,26 @@
         <v>40</v>
       </c>
       <c r="B27" s="132">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
       <c r="C27" s="28">
-        <f>1.5*T27</f>
+        <f t="shared" si="10"/>
         <v>40.5</v>
       </c>
       <c r="D27" s="85">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="E27" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="F27" s="78" t="s">
         <v>56</v>
       </c>
-      <c r="G27" s="236">
-        <f t="shared" si="6"/>
+      <c r="G27" s="208">
+        <f t="shared" si="7"/>
         <v>75</v>
       </c>
       <c r="H27" s="149" t="s">
@@ -5091,11 +6954,11 @@
         <v>0</v>
       </c>
       <c r="N27" s="54">
-        <f>SUM(B27:M27)+Z27</f>
+        <f t="shared" si="11"/>
         <v>339.5</v>
       </c>
       <c r="O27" s="158">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
       <c r="P27" s="8">
@@ -5141,15 +7004,15 @@
         <v>41</v>
       </c>
       <c r="B28" s="132">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
       <c r="C28" s="28">
-        <f>1.5*T28</f>
+        <f t="shared" si="10"/>
         <v>1.5</v>
       </c>
       <c r="D28" s="85">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="E28" s="24" t="s">
@@ -5158,8 +7021,8 @@
       <c r="F28" s="78" t="s">
         <v>56</v>
       </c>
-      <c r="G28" s="236">
-        <f t="shared" si="6"/>
+      <c r="G28" s="208">
+        <f t="shared" si="7"/>
         <v>27</v>
       </c>
       <c r="H28" s="181" t="s">
@@ -5181,11 +7044,11 @@
         <v>0</v>
       </c>
       <c r="N28" s="54">
-        <f>SUM(B28:M28)+Z28</f>
+        <f t="shared" si="11"/>
         <v>228.5</v>
       </c>
       <c r="O28" s="158">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
       <c r="P28" s="8">
@@ -5231,15 +7094,15 @@
         <v>42</v>
       </c>
       <c r="B29" s="132">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
       <c r="C29" s="28">
-        <f>1.5*T29</f>
+        <f t="shared" si="10"/>
         <v>7.5</v>
       </c>
       <c r="D29" s="85">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="E29" s="24" t="s">
@@ -5248,8 +7111,8 @@
       <c r="F29" s="78" t="s">
         <v>56</v>
       </c>
-      <c r="G29" s="236">
-        <f t="shared" si="6"/>
+      <c r="G29" s="208">
+        <f t="shared" si="7"/>
         <v>106</v>
       </c>
       <c r="H29" s="149" t="s">
@@ -5271,11 +7134,11 @@
         <v>0</v>
       </c>
       <c r="N29" s="54">
-        <f>SUM(B29:M29)+Z29</f>
+        <f t="shared" si="11"/>
         <v>313.5</v>
       </c>
       <c r="O29" s="158">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
       <c r="P29" s="8">
@@ -5324,11 +7187,11 @@
         <v>0</v>
       </c>
       <c r="C30" s="28">
-        <f>1.5*T30</f>
+        <f t="shared" si="10"/>
         <v>4.5</v>
       </c>
       <c r="D30" s="85">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="E30" s="24" t="s">
@@ -5337,8 +7200,8 @@
       <c r="F30" s="78" t="s">
         <v>56</v>
       </c>
-      <c r="G30" s="236">
-        <f t="shared" si="6"/>
+      <c r="G30" s="208">
+        <f t="shared" si="7"/>
         <v>33</v>
       </c>
       <c r="H30" s="149" t="s">
@@ -5364,7 +7227,7 @@
         <v>67.5</v>
       </c>
       <c r="O30" s="20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
       <c r="P30" s="87">
@@ -5410,15 +7273,15 @@
         <v>46</v>
       </c>
       <c r="B31" s="132">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
       <c r="C31" s="28">
-        <f>1.5*T31</f>
+        <f t="shared" si="10"/>
         <v>28.5</v>
       </c>
       <c r="D31" s="85">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="E31" s="24" t="s">
@@ -5427,8 +7290,8 @@
       <c r="F31" s="78" t="s">
         <v>56</v>
       </c>
-      <c r="G31" s="236">
-        <f t="shared" si="6"/>
+      <c r="G31" s="208">
+        <f t="shared" si="7"/>
         <v>125</v>
       </c>
       <c r="H31" s="149" t="s">
@@ -5454,7 +7317,7 @@
         <v>353.5</v>
       </c>
       <c r="O31" s="158">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
       <c r="P31" s="8">
@@ -5506,7 +7369,7 @@
         <v>0</v>
       </c>
       <c r="D32" s="85">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="E32" s="24" t="s">
@@ -5515,7 +7378,7 @@
       <c r="F32" s="78" t="s">
         <v>56</v>
       </c>
-      <c r="G32" s="236" t="s">
+      <c r="G32" s="208" t="s">
         <v>56</v>
       </c>
       <c r="H32" s="149" t="s">
@@ -5541,7 +7404,7 @@
         <v>30</v>
       </c>
       <c r="O32" s="20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
       <c r="P32" s="87">
@@ -5594,7 +7457,7 @@
         <v>13.5</v>
       </c>
       <c r="D33" s="85">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="E33" s="24" t="s">
@@ -5603,8 +7466,8 @@
       <c r="F33" s="78" t="s">
         <v>56</v>
       </c>
-      <c r="G33" s="236">
-        <f t="shared" si="6"/>
+      <c r="G33" s="208">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H33" s="149" t="s">
@@ -5630,7 +7493,7 @@
         <v>143.5</v>
       </c>
       <c r="O33" s="158">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
       <c r="P33" s="8">
@@ -5683,7 +7546,7 @@
         <v>34.5</v>
       </c>
       <c r="D34" s="85">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="E34" s="24" t="s">
@@ -5692,8 +7555,8 @@
       <c r="F34" s="78" t="s">
         <v>56</v>
       </c>
-      <c r="G34" s="236">
-        <f t="shared" si="6"/>
+      <c r="G34" s="208">
+        <f t="shared" si="7"/>
         <v>12</v>
       </c>
       <c r="H34" s="149" t="s">
@@ -5719,7 +7582,7 @@
         <v>78.5</v>
       </c>
       <c r="O34" s="20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
       <c r="P34" s="87">
@@ -5771,7 +7634,7 @@
         <v>0</v>
       </c>
       <c r="D35" s="85">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>60</v>
       </c>
       <c r="E35" s="24" t="s">
@@ -5780,7 +7643,7 @@
       <c r="F35" s="78" t="s">
         <v>56</v>
       </c>
-      <c r="G35" s="236" t="s">
+      <c r="G35" s="208" t="s">
         <v>56</v>
       </c>
       <c r="H35" s="149" t="s">
@@ -5806,7 +7669,7 @@
         <v>160</v>
       </c>
       <c r="O35" s="158">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
       <c r="P35" s="8">
@@ -5859,18 +7722,18 @@
         <v>10.5</v>
       </c>
       <c r="D36" s="85">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="E36" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="F36" s="78">
         <v>15</v>
       </c>
-      <c r="G36" s="236">
-        <f t="shared" si="6"/>
+      <c r="G36" s="208">
+        <f t="shared" si="7"/>
         <v>18</v>
       </c>
       <c r="H36" s="149" t="s">
@@ -5897,7 +7760,7 @@
         <v>173</v>
       </c>
       <c r="O36" s="158">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
       <c r="P36" s="8">
@@ -5951,7 +7814,7 @@
         <v>13.5</v>
       </c>
       <c r="D37" s="86">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="E37" s="25" t="s">
@@ -5960,7 +7823,7 @@
       <c r="F37" s="79" t="s">
         <v>56</v>
       </c>
-      <c r="G37" s="237">
+      <c r="G37" s="209">
         <f>X41*X37</f>
         <v>2</v>
       </c>
@@ -5987,7 +7850,7 @@
         <v>124.5</v>
       </c>
       <c r="O37" s="163">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
       <c r="P37" s="9">
@@ -6035,11 +7898,11 @@
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
-      <c r="N38" s="204" t="s">
+      <c r="N38" s="226" t="s">
         <v>109</v>
       </c>
-      <c r="O38" s="205"/>
-      <c r="P38" s="206"/>
+      <c r="O38" s="227"/>
+      <c r="P38" s="228"/>
       <c r="R38" s="2"/>
       <c r="S38" s="112"/>
       <c r="T38" s="2"/>
@@ -6166,7 +8029,7 @@
       <c r="U43" s="2"/>
     </row>
     <row r="44" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A44" s="225" t="s">
+      <c r="A44" s="199" t="s">
         <v>157</v>
       </c>
       <c r="H44" s="2"/>
@@ -6191,7 +8054,7 @@
       </c>
     </row>
     <row r="45" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A45" s="225" t="s">
+      <c r="A45" s="199" t="s">
         <v>166</v>
       </c>
       <c r="H45" s="2"/>
@@ -6321,12 +8184,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC94"/>
   <sheetViews>
     <sheetView topLeftCell="U19" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:AV48"/>
+      <selection activeCell="AB27" sqref="AB27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7802,18 +9665,18 @@
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" s="123"/>
-      <c r="B17" s="210"/>
-      <c r="C17" s="211"/>
-      <c r="D17" s="207"/>
-      <c r="E17" s="208"/>
-      <c r="F17" s="209"/>
+      <c r="B17" s="237"/>
+      <c r="C17" s="238"/>
+      <c r="D17" s="234"/>
+      <c r="E17" s="235"/>
+      <c r="F17" s="236"/>
       <c r="G17" s="193">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="H17" s="212"/>
-      <c r="I17" s="213"/>
-      <c r="J17" s="214"/>
+      <c r="H17" s="239"/>
+      <c r="I17" s="240"/>
+      <c r="J17" s="241"/>
       <c r="K17" s="185"/>
       <c r="L17" s="186"/>
       <c r="M17" s="187"/>
@@ -9564,11 +11427,11 @@
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
-      <c r="N37" s="204" t="s">
+      <c r="N37" s="226" t="s">
         <v>109</v>
       </c>
-      <c r="O37" s="205"/>
-      <c r="P37" s="206"/>
+      <c r="O37" s="227"/>
+      <c r="P37" s="228"/>
       <c r="R37" s="2"/>
       <c r="S37" s="112"/>
       <c r="T37" s="2"/>
@@ -10164,7 +12027,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD46"/>
   <sheetViews>
@@ -13087,11 +14950,11 @@
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
-      <c r="N37" s="215" t="s">
+      <c r="N37" s="242" t="s">
         <v>109</v>
       </c>
-      <c r="O37" s="216"/>
-      <c r="P37" s="217"/>
+      <c r="O37" s="243"/>
+      <c r="P37" s="244"/>
       <c r="R37" s="2"/>
       <c r="S37" s="112"/>
       <c r="T37" s="2"/>
@@ -13277,7 +15140,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB46"/>
   <sheetViews>
@@ -15941,10 +17804,10 @@
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
-      <c r="M37" s="215" t="s">
+      <c r="M37" s="242" t="s">
         <v>109</v>
       </c>
-      <c r="N37" s="217"/>
+      <c r="N37" s="244"/>
       <c r="P37" s="2"/>
       <c r="Q37" s="112"/>
       <c r="R37" s="2"/>
@@ -16112,7 +17975,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB47"/>
   <sheetViews>
@@ -18325,10 +20188,10 @@
     </row>
     <row r="37" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K37" s="55"/>
-      <c r="L37" s="218" t="s">
+      <c r="L37" s="245" t="s">
         <v>75</v>
       </c>
-      <c r="M37" s="219"/>
+      <c r="M37" s="246"/>
       <c r="O37" s="2"/>
       <c r="P37" s="2"/>
       <c r="Q37" s="2"/>
@@ -18420,7 +20283,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C19"/>
   <sheetViews>
@@ -18446,7 +20309,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="220" t="s">
+      <c r="A2" s="247" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="39" t="s">
@@ -18457,7 +20320,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="222"/>
+      <c r="A3" s="249"/>
       <c r="B3" s="40" t="s">
         <v>4</v>
       </c>
@@ -18466,7 +20329,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="202" t="s">
+      <c r="A4" s="218" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="41" t="s">
@@ -18477,7 +20340,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="203"/>
+      <c r="A5" s="219"/>
       <c r="B5" s="43" t="s">
         <v>9</v>
       </c>
@@ -18486,7 +20349,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="220" t="s">
+      <c r="A6" s="247" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="39" t="s">
@@ -18497,7 +20360,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="221"/>
+      <c r="A7" s="248"/>
       <c r="B7" s="44" t="s">
         <v>13</v>
       </c>
@@ -18506,7 +20369,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="203"/>
+      <c r="A8" s="219"/>
       <c r="B8" s="43" t="s">
         <v>14</v>
       </c>
@@ -18527,7 +20390,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="220" t="s">
+      <c r="A11" s="247" t="s">
         <v>2</v>
       </c>
       <c r="B11" s="39" t="s">
@@ -18538,7 +20401,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="222"/>
+      <c r="A12" s="249"/>
       <c r="B12" s="40" t="s">
         <v>4</v>
       </c>
@@ -18547,7 +20410,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="202" t="s">
+      <c r="A13" s="218" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="41" t="s">
@@ -18558,7 +20421,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="200"/>
+      <c r="A14" s="216"/>
       <c r="B14" s="42" t="s">
         <v>9</v>
       </c>
@@ -18567,7 +20430,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="200"/>
+      <c r="A15" s="216"/>
       <c r="B15" s="42" t="s">
         <v>72</v>
       </c>
@@ -18576,7 +20439,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="203"/>
+      <c r="A16" s="219"/>
       <c r="B16" s="43" t="s">
         <v>78</v>
       </c>
@@ -18585,7 +20448,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="220" t="s">
+      <c r="A17" s="247" t="s">
         <v>11</v>
       </c>
       <c r="B17" s="39" t="s">
@@ -18596,7 +20459,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="221"/>
+      <c r="A18" s="248"/>
       <c r="B18" s="44" t="s">
         <v>13</v>
       </c>
@@ -18605,7 +20468,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="203"/>
+      <c r="A19" s="219"/>
       <c r="B19" s="43" t="s">
         <v>14</v>
       </c>

</xml_diff>